<commit_message>
Update: Excelfile der Übersetzungen
</commit_message>
<xml_diff>
--- a/_specs/slirv_translations.xlsx
+++ b/_specs/slirv_translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30020" windowHeight="22900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30940" windowHeight="18560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="slirv_translations" localSheetId="0">Blatt1!$A$2:$H$115</definedName>
+    <definedName name="slirv_translations" localSheetId="0">Blatt1!$A$2:$H$116</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="528">
   <si>
     <t>typ</t>
   </si>
@@ -1024,9 +1024,6 @@
     <t>impressum</t>
   </si>
   <si>
-    <t>Konsum, Handel oder Herstellen von Drogen</t>
-  </si>
-  <si>
     <t>Consumption, trade or manufacture of drugs</t>
   </si>
   <si>
@@ -1219,9 +1216,6 @@
     <t>Tecnologia</t>
   </si>
   <si>
-    <t>Delict Gravant</t>
-  </si>
-  <si>
     <t>servetsch da spiunadi scumandà</t>
   </si>
   <si>
@@ -1255,9 +1249,6 @@
     <t>cell phone</t>
   </si>
   <si>
-    <t>Basisinformationen, z.B. wem gehört eine eine bestimmte Telefonnummer oder eine bestimmte IP-Adresse zu einer bestimmten Zeit.</t>
-  </si>
-  <si>
     <t>simple basic information, ex. who used a certrain cell number or who used an IP adress at a certain time</t>
   </si>
   <si>
@@ -1423,9 +1414,6 @@
     <t>Gravi crimini sono evidenziati, in quanto questi sono ripetutamente cresciuti nel sostenere per la sorveglianza.</t>
   </si>
   <si>
-    <t>Ein Antennensuchlauf, auch Funkzellenabfrage oder Rasterfahndung, erfasst alle Mobiltelefone in einem Gebiet</t>
-  </si>
-  <si>
     <t>A mobile subscriber scan,  radiocell-inquiry or dragnet. All mobile phones registered in a certain area</t>
   </si>
   <si>
@@ -1447,12 +1435,6 @@
     <t>salvataggio di emergenza viene utilizzato per la ricerca e il salvataggio di mancanti o fuggito.</t>
   </si>
   <si>
-    <t>Die Digitale Gesellschaft Schweiz veröffentlicht jährlich den Swiss Lawful Interception Report über die staatliche Überwachung in der Schweiz..&lt;br&gt;Diese Visualiserung ergänzt den Report interaktiv und zeigt detailiert auf, wie in den Kantonen überwacht wird. Finden Sie heraus, für welche Delikte Ihre Grundrechte eingeschränkt werden.&lt;br&gt;&lt;br&gt;&lt;small&gt;Die Daten in dieser Statistik beinhalten nur Überwachungmassnahmen nach Strafprozessordnung. Ausgenommen sind Einsätze von IMSI-Catcher, Staatstrojanern oder Überwachungsmassnahmen des Nachrichtendienstes.&lt;/small&gt;</t>
-  </si>
-  <si>
-    <t>Die Digitale Gesellschaft ist ein offener Zusammenschluss netzpolitisch interessierter Kreise. Dem Bündnis angeschlossen sind rund 50 Einzelpersonen und 15 Gruppierungen. Dazu gehören Grundrechtsorganisationen, Parteien, KünstlerInnen-Kollektive, BetreiberInnen von Netzwerkdiensten und weiteren Gruppen, die sich der kritischen, digitalen Zivilgesellschaft verpflichtet fühlen. &lt;br&gt;Weitere Informationen zu netzpolitischen Themen sind im Blog zu finden: &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;&lt;br&gt;&lt;br&gt;Programmierung: Ueli Kunz, &lt;a href='http://ideadapt.net'&gt;ideadapt.net&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Die Digitale Gesellschaft ist ein offener Zusammenschluss netzpolitisch interessierter Kreise. Dem Bündnis angeschlossen sind rund 50 Einzelpersonen und 15 Gruppierungen. Dazu gehören Grundrechtsorganisationen, Parteien, KünstlerInnen-Kollektive, BetreiberInnen von Netzwerkdiensten und weiteren Gruppen, die sich der kritischen, digitalen Zivilgesellschaft verpflichtet fühlen. &lt;br&gt;Weitere Informationen zu netzpolitischen Themen sind im Blog zu finden: &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;&lt;br&gt;&lt;br&gt;Coded By: Ueli Kunz, &lt;a href='http://ideadapt.net'&gt;ideadapt.net&lt;/a&gt;</t>
   </si>
   <si>
@@ -1604,6 +1586,46 @@
   </si>
   <si>
     <t>slir_intro</t>
+  </si>
+  <si>
+    <t>Die Digitale Gesellschaft Schweiz veröffentlicht jährlich den Swiss Lawful Interception Report über die staatliche Überwachung in der Schweiz. Diese Visualiserung ergänzt den Report interaktiv und zeigt detailiert auf, wie in den Kantonen überwacht wird. Finden Sie heraus, für welche Delikte Ihre Grundrechte eingeschränkt werden.&lt;br&gt;&lt;br&gt;&lt;small&gt;Die Daten in dieser Statistik beinhalten nur Überwachungmassnahmen nach Strafprozessordnung. Ausgenommen sind Einsätze von IMSI-Catcher, Staatstrojanern oder Überwachungsmassnahmen des Nachrichtendienstes.&lt;/small&gt;</t>
+  </si>
+  <si>
+    <t>Herstellen, Handel oder Konsum  von Drogen</t>
+  </si>
+  <si>
+    <t>Störung des öffentlichen Friedens, Demonstrationen, Kriminelle Organisationen, Gefährdung durch Waffen</t>
+  </si>
+  <si>
+    <t>Landesverrat, Verbreiten menschlicher Krankheiten, Amtsmissbrauch, verbotener Nachrichtendienst</t>
+  </si>
+  <si>
+    <t>Strukturierte Gruppe, welche mittels Gewaltverbrechen oder sich durch verbrecherische Mittel
+Einkünfte bereichert, wie Mafia oder Djihad</t>
+  </si>
+  <si>
+    <t>wem gehört eine eine bestimmte Telefonnummer oder eine bestimmte IP-Adresse zu einer bestimmten Zeit.</t>
+  </si>
+  <si>
+    <t>Auch Funkzellenabfrage oder Rasterfahndung genannt, erfasst alle Mobiltelefone in einem Gebiet.</t>
+  </si>
+  <si>
+    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden.&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>Swiss Lawful Interception Report 2015</t>
+  </si>
+  <si>
+    <t>Die Digitale Gesellschaft ist ein offener Zusammenschluss netzpolitisch interessierter Kreise. Dem Bündnis angeschlossen sind rund 50 Einzelpersonen und 15 Gruppierungen. Dazu gehören Grundrechtsorganisationen, Parteien, KünstlerInnen-Kollektive, BetreiberInnen von Netzwerkdiensten und weiteren Gruppen, die sich der kritischen, digitalen Zivilgesellschaft verpflichtet fühlen. &lt;br&gt;&lt;br&gt;Weitere Informationen zu netzpolitischen Themen sind im Blog zu finden: &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;&lt;br&gt;&lt;br&gt;Programmierung: Ueli Kunz, &lt;a href='http://ideadapt.net'&gt;ideadapt.net&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Delicts Gravant</t>
+  </si>
+  <si>
+    <t>sämtliche Handlungen, welche geeignet sind, die Ermittlung der Herkunft, die Auffindung oder die Einziehung von Vermögenswerten zu vereiteln.</t>
+  </si>
+  <si>
+    <t>Menschen anwerben, anbieten, vermitteln oder beherbergen durch Anwendung unerlaubternMittel wie Täuschung, Drohung oder Nötigung zum Zwecke der Ausbeutung.</t>
   </si>
 </sst>
 </file>
@@ -1663,7 +1685,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="193">
+  <cellStyleXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1854,6 +1876,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1882,7 +1906,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="193">
+  <cellStyles count="195">
     <cellStyle name="Besuchter Link" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
@@ -1987,6 +2011,7 @@
     <cellStyle name="Besuchter Link" xfId="189" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
@@ -2075,6 +2100,7 @@
     <cellStyle name="Link" xfId="186" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="188" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -2145,8 +2171,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:J115" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J115"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:J116" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J116"/>
   <tableColumns count="10">
     <tableColumn id="1" name="group" dataDxfId="9"/>
     <tableColumn id="2" name="typ" dataDxfId="8"/>
@@ -2485,10 +2511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2497,7 +2523,8 @@
     <col min="2" max="2" width="9" style="4" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="32.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="3"/>
+    <col min="9" max="9" width="10.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2526,10 +2553,10 @@
         <v>175</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2716,16 +2743,16 @@
         <v>157</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="1"/>
@@ -2741,19 +2768,19 @@
         <v>112</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="1"/>
@@ -2769,19 +2796,19 @@
         <v>111</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I9" s="6">
         <v>1</v>
@@ -2802,16 +2829,16 @@
         <v>116</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>392</v>
+        <v>525</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="1"/>
@@ -2830,16 +2857,16 @@
         <v>115</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>115</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="1"/>
@@ -2858,16 +2885,16 @@
         <v>114</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>396</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="1"/>
@@ -2883,19 +2910,19 @@
         <v>325</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="1"/>
@@ -2911,19 +2938,19 @@
         <v>326</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>387</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="1"/>
@@ -2936,22 +2963,22 @@
         <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="1"/>
@@ -2970,7 +2997,7 @@
         <v>117</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>297</v>
@@ -2979,7 +3006,7 @@
         <v>298</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="1"/>
@@ -3007,7 +3034,7 @@
         <v>299</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="1"/>
@@ -3020,22 +3047,22 @@
         <v>55</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="1"/>
@@ -3054,7 +3081,7 @@
         <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>267</v>
@@ -3063,7 +3090,7 @@
         <v>300</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="1"/>
@@ -3076,22 +3103,22 @@
         <v>55</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="I20" s="6">
         <v>1</v>
@@ -3106,22 +3133,22 @@
         <v>55</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>447</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>450</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="1"/>
@@ -3134,22 +3161,22 @@
         <v>55</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>413</v>
       </c>
       <c r="I22" s="6">
         <v>1</v>
@@ -3164,22 +3191,22 @@
         <v>55</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>481</v>
-      </c>
       <c r="H23" s="2" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I23" s="6">
         <v>1</v>
@@ -3194,22 +3221,22 @@
         <v>55</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>484</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="I24" s="6">
         <v>1</v>
@@ -3224,22 +3251,22 @@
         <v>55</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="I25" s="6">
         <v>1</v>
@@ -3269,7 +3296,7 @@
         <v>237</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="1"/>
@@ -3297,7 +3324,7 @@
         <v>324</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="1"/>
@@ -4103,7 +4130,7 @@
         <v>283</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I54" s="6"/>
       <c r="J54" s="1"/>
@@ -4131,7 +4158,7 @@
         <v>276</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I55" s="6"/>
       <c r="J55" s="1"/>
@@ -4159,7 +4186,7 @@
         <v>284</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="I56" s="6"/>
       <c r="J56" s="1"/>
@@ -4187,7 +4214,7 @@
         <v>285</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="1"/>
@@ -4215,7 +4242,7 @@
         <v>278</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I58" s="6"/>
       <c r="J58" s="1"/>
@@ -4243,7 +4270,7 @@
         <v>286</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I59" s="6"/>
       <c r="J59" s="1"/>
@@ -4271,7 +4298,7 @@
         <v>279</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="1"/>
@@ -4299,7 +4326,7 @@
         <v>280</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="I61" s="6"/>
       <c r="J61" s="1"/>
@@ -4327,7 +4354,7 @@
         <v>317</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I62" s="6"/>
       <c r="J62" s="1"/>
@@ -4343,19 +4370,19 @@
         <v>85</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I63" s="6"/>
       <c r="J63" s="1"/>
@@ -4371,19 +4398,19 @@
         <v>86</v>
       </c>
       <c r="D64" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="F64" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="G64" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="G64" s="1" t="s">
-        <v>330</v>
-      </c>
       <c r="H64" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I64" s="6"/>
       <c r="J64" s="1"/>
@@ -4399,19 +4426,19 @@
         <v>87</v>
       </c>
       <c r="D65" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="F65" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>342</v>
-      </c>
       <c r="G65" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="I65" s="6"/>
       <c r="J65" s="1"/>
@@ -4436,10 +4463,10 @@
         <v>242</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I66" s="6"/>
       <c r="J66" s="1"/>
@@ -4467,12 +4494,12 @@
         <v>277</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I67" s="6"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" ht="60">
       <c r="A68" s="4" t="s">
         <v>75</v>
       </c>
@@ -4483,7 +4510,7 @@
         <v>90</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>106</v>
+        <v>517</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>134</v>
@@ -4495,7 +4522,7 @@
         <v>278</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="I68" s="6"/>
       <c r="J68" s="1"/>
@@ -4523,12 +4550,12 @@
         <v>166</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I69" s="6"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" ht="60">
       <c r="A70" s="4" t="s">
         <v>75</v>
       </c>
@@ -4539,7 +4566,7 @@
         <v>92</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>105</v>
+        <v>518</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>138</v>
@@ -4551,7 +4578,7 @@
         <v>279</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I70" s="6"/>
       <c r="J70" s="1"/>
@@ -4567,19 +4594,19 @@
         <v>93</v>
       </c>
       <c r="D71" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="F71" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="G71" s="1" t="s">
+      <c r="H71" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="I71" s="6"/>
       <c r="J71" s="1"/>
@@ -4595,16 +4622,16 @@
         <v>63</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>456</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>459</v>
       </c>
       <c r="I72" s="6"/>
       <c r="J72" s="1"/>
@@ -4623,7 +4650,7 @@
         <v>102</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>258</v>
@@ -4632,7 +4659,7 @@
         <v>290</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I73" s="6"/>
       <c r="J73" s="1"/>
@@ -4651,7 +4678,7 @@
         <v>96</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>259</v>
@@ -4660,7 +4687,7 @@
         <v>291</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I74" s="6"/>
       <c r="J74" s="1"/>
@@ -4679,7 +4706,7 @@
         <v>99</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>260</v>
@@ -4688,7 +4715,7 @@
         <v>292</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I75" s="6"/>
       <c r="J75" s="1"/>
@@ -4707,7 +4734,7 @@
         <v>171</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>261</v>
@@ -4716,7 +4743,7 @@
         <v>293</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I76" s="6"/>
       <c r="J76" s="1"/>
@@ -4744,7 +4771,7 @@
         <v>140</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I77" s="6"/>
       <c r="J77" s="1"/>
@@ -4763,7 +4790,7 @@
         <v>107</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>263</v>
@@ -4772,12 +4799,12 @@
         <v>294</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I78" s="6"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" ht="75">
       <c r="A79" s="4" t="s">
         <v>94</v>
       </c>
@@ -4788,24 +4815,24 @@
         <v>103</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>419</v>
+        <v>526</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I79" s="6"/>
       <c r="J79" s="1"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" ht="75">
       <c r="A80" s="4" t="s">
         <v>94</v>
       </c>
@@ -4816,24 +4843,24 @@
         <v>97</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>423</v>
+        <v>519</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="I80" s="6"/>
       <c r="J80" s="1"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" ht="75">
       <c r="A81" s="4" t="s">
         <v>94</v>
       </c>
@@ -4844,19 +4871,19 @@
         <v>100</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>419</v>
+        <v>527</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I81" s="6"/>
       <c r="J81" s="1"/>
@@ -4884,7 +4911,7 @@
         <v>287</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I82" s="6"/>
       <c r="J82" s="1"/>
@@ -4912,7 +4939,7 @@
         <v>288</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I83" s="6"/>
       <c r="J83" s="1"/>
@@ -4940,7 +4967,7 @@
         <v>289</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I84" s="6"/>
       <c r="J84" s="1"/>
@@ -4984,19 +5011,19 @@
         <v>60</v>
       </c>
       <c r="D86" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="F86" s="1" t="s">
+      <c r="G86" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="G86" s="1" t="s">
+      <c r="H86" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>372</v>
       </c>
       <c r="I86" s="6"/>
       <c r="J86" s="1"/>
@@ -5124,7 +5151,7 @@
         <v>58</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>158</v>
@@ -5136,7 +5163,7 @@
         <v>301</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I91" s="6"/>
       <c r="J91" s="1"/>
@@ -5152,24 +5179,24 @@
         <v>60</v>
       </c>
       <c r="D92" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="H92" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="I92" s="6"/>
       <c r="J92" s="1"/>
     </row>
-    <row r="93" spans="1:10" ht="60">
+    <row r="93" spans="1:10" ht="45">
       <c r="A93" s="4" t="s">
         <v>0</v>
       </c>
@@ -5180,19 +5207,19 @@
         <v>64</v>
       </c>
       <c r="D93" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G93" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>407</v>
-      </c>
       <c r="H93" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="I93" s="6"/>
       <c r="J93" s="1"/>
@@ -5208,19 +5235,19 @@
         <v>59</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="I94" s="6"/>
       <c r="J94" s="1"/>
@@ -5230,28 +5257,30 @@
         <v>0</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>310</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="H95" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
         <v>https://de-de.facebook.com/help/405183566203254</v>
       </c>
-      <c r="I95" s="6"/>
+      <c r="I95" s="6">
+        <v>1</v>
+      </c>
       <c r="J95" s="1">
         <v>1</v>
       </c>
@@ -5267,7 +5296,7 @@
         <v>310</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="I96" s="6"/>
       <c r="J96" s="1"/>
@@ -5283,7 +5312,7 @@
         <v>311</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="I97" s="6"/>
       <c r="J97" s="1"/>
@@ -5367,7 +5396,7 @@
         <v>273</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I100" s="6"/>
       <c r="J100" s="1"/>
@@ -5439,16 +5468,16 @@
         <v>120</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>460</v>
+        <v>521</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="I103" s="6"/>
       <c r="J103" s="1"/>
@@ -5464,16 +5493,16 @@
         <v>121</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="I104" s="6"/>
       <c r="J104" s="1"/>
@@ -5492,7 +5521,7 @@
         <v>71</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>265</v>
@@ -5501,7 +5530,7 @@
         <v>295</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I105" s="6"/>
       <c r="J105" s="1"/>
@@ -5548,7 +5577,7 @@
         <v>73</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>264</v>
@@ -5557,7 +5586,7 @@
         <v>296</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I107" s="6"/>
       <c r="J107" s="1"/>
@@ -5585,92 +5614,109 @@
         <v>274</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I108" s="6"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109" spans="1:10" ht="45">
-      <c r="A109" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="C109" s="4" t="s">
+    <row r="109" spans="1:10" s="1" customFormat="1">
+      <c r="A109" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>325</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>451</v>
+        <v>523</v>
       </c>
       <c r="E109" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
-        <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
+        <v>Swiss Lawful Interception Report 2015</v>
       </c>
       <c r="F109" s="1" t="str">
         <f>Tabelle2[[#This Row],[en]]</f>
-        <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
+        <v>Swiss Lawful Interception Report 2015</v>
       </c>
       <c r="G109" s="1" t="str">
         <f>Tabelle2[[#This Row],[fr]]</f>
-        <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
+        <v>Swiss Lawful Interception Report 2015</v>
       </c>
       <c r="H109" s="1" t="str">
         <f>Tabelle2[[#This Row],[it]]</f>
+        <v>Swiss Lawful Interception Report 2015</v>
+      </c>
+      <c r="I109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="45">
+      <c r="A110" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E110" s="1" t="str">
+        <f>Tabelle2[[#This Row],[de]]</f>
         <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
-      <c r="I109" s="6">
-        <v>1</v>
-      </c>
-      <c r="J109" s="1"/>
-    </row>
-    <row r="110" spans="1:10" ht="330">
-      <c r="A110" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>503</v>
+      <c r="F110" s="1" t="str">
+        <f>Tabelle2[[#This Row],[en]]</f>
+        <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
+      </c>
+      <c r="G110" s="1" t="str">
+        <f>Tabelle2[[#This Row],[fr]]</f>
+        <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
+      </c>
+      <c r="H110" s="1" t="str">
+        <f>Tabelle2[[#This Row],[it]]</f>
+        <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
       <c r="I110" s="6">
         <v>1</v>
       </c>
       <c r="J110" s="1"/>
     </row>
-    <row r="111" spans="1:10" ht="270">
-      <c r="A111" s="4" t="s">
+    <row r="111" spans="1:10" ht="330">
+      <c r="A111" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C111" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="I111" s="6"/>
+      <c r="C111" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="I111" s="6">
+        <v>1</v>
+      </c>
       <c r="J111" s="1"/>
     </row>
-    <row r="112" spans="1:10" ht="120">
+    <row r="112" spans="1:10" ht="270">
       <c r="A112" s="4" t="s">
         <v>318</v>
       </c>
@@ -5678,29 +5724,15 @@
         <v>63</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>520</v>
+        <v>319</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="H112" s="1" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="I112" s="6"/>
-      <c r="J112" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" ht="105">
+      <c r="J112" s="1"/>
+    </row>
+    <row r="113" spans="1:10" ht="120">
       <c r="A113" s="4" t="s">
         <v>318</v>
       </c>
@@ -5708,31 +5740,29 @@
         <v>63</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>513</v>
+        <v>522</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="I113" s="6">
-        <v>1</v>
-      </c>
+        <v>506</v>
+      </c>
+      <c r="I113" s="6"/>
       <c r="J113" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="210">
+    <row r="114" spans="1:10" ht="105">
       <c r="A114" s="4" t="s">
         <v>318</v>
       </c>
@@ -5740,63 +5770,96 @@
         <v>63</v>
       </c>
       <c r="C114" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="D114" s="1" t="str">
+        <f>CONCATENATE("&lt;a href='",D110,"' title='",D109,"' target='_blank'&gt;",D109,"&lt;/a&gt;")</f>
+        <v>&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="I114" s="6">
+        <v>1</v>
+      </c>
+      <c r="J114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="210">
+      <c r="A115" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C115" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="D114" s="1" t="str">
-        <f>CONCATENATE(D112,D113)</f>
-        <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
-      </c>
-      <c r="E114" s="1" t="str">
-        <f>CONCATENATE(E112,E113)</f>
+      <c r="D115" s="1" t="str">
+        <f>CONCATENATE(D113,D114)</f>
+        <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden.&lt;br&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
+      </c>
+      <c r="E115" s="1" t="str">
+        <f>CONCATENATE(E113,E114)</f>
         <v>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</v>
       </c>
-      <c r="F114" s="1" t="str">
-        <f t="shared" ref="F114:H114" si="0">CONCATENATE(F112,F113)</f>
+      <c r="F115" s="1" t="str">
+        <f t="shared" ref="F115:H115" si="0">CONCATENATE(F113,F114)</f>
         <v>En plus de cette visualisation de la surveillance la société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</v>
       </c>
-      <c r="G114" s="1" t="str">
+      <c r="G115" s="1" t="str">
         <f t="shared" si="0"/>
         <v>In aggiunta a questa visualizzazione della sorveglianza. La società digitale pubblica una relazione annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Le Swiss Lawful Interception Report può essere scaricato qui. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</v>
       </c>
-      <c r="H114" s="1" t="str">
+      <c r="H115" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
-      <c r="I114" s="6">
+      <c r="I115" s="6">
         <v>1</v>
       </c>
-      <c r="J114" s="1"/>
-    </row>
-    <row r="115" spans="1:10" ht="300">
-      <c r="A115" s="4" t="s">
+      <c r="J115" s="1"/>
+    </row>
+    <row r="116" spans="1:10" ht="300">
+      <c r="A116" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C115" s="4" t="s">
+      <c r="C116" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="I115" s="6"/>
-      <c r="J115" s="1"/>
+      <c r="D116" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="I116" s="6"/>
+      <c r="J116" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="I1:I108 I110:I1048576">
     <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",I1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update TranslationsUpdate: Excelfile der Übersetzungen
</commit_message>
<xml_diff>
--- a/_specs/slirv_translations.xlsx
+++ b/_specs/slirv_translations.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30940" windowHeight="18560" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="800" windowWidth="30940" windowHeight="18560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="3" r:id="rId1"/>
+    <sheet name="Blatt2" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="slirv_translations" localSheetId="0">Blatt1!$A$2:$H$116</definedName>
+    <definedName name="slirv_translations" localSheetId="0">Blatt1!$A$2:$H$117</definedName>
+    <definedName name="slirv_translations_1" localSheetId="1">Blatt2!$A$2:$H$116</definedName>
+    <definedName name="slirv_translations_2" localSheetId="1">Blatt2!$A$2:$H$116</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="535">
   <si>
     <t>typ</t>
   </si>
@@ -1303,9 +1306,6 @@
     <t>url</t>
   </si>
   <si>
-    <t>Mafia, Djihad</t>
-  </si>
-  <si>
     <t>infurmaziun da basa p.ex. a tgi esser determinà numer da telefon u una adressa ip</t>
   </si>
   <si>
@@ -1402,9 +1402,6 @@
     <t>delicts pussanza</t>
   </si>
   <si>
-    <t>Schwere Delikte sind hervorgehoben, da diese immer wieder ins Feld geführt werden, um Überwachung zu rechtfertigen.</t>
-  </si>
-  <si>
     <t>Serious crimes are highlighted, because those are repeatedly brought up in arguing for surveillance.</t>
   </si>
   <si>
@@ -1498,9 +1495,6 @@
     <t>Appenzell Dadora</t>
   </si>
   <si>
-    <t>Anzahl betroffene Microsoft/Skype Accounts</t>
-  </si>
-  <si>
     <t>tmp_url</t>
   </si>
   <si>
@@ -1516,25 +1510,7 @@
     <t>https://fr-fr.facebook.com/help/405183566203254</t>
   </si>
   <si>
-    <t>Anzahl betroffene Facebook Accounts. Diese Liste der Facebook Daten zeigt den Umfang auf.</t>
-  </si>
-  <si>
     <t>notEXport</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.li.admin.ch/de' target='_blank'&gt;Dienst Überwachung Post- und Fernmeldeverkehr&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Microsoft / Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Basiskarte: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Bundesamt für Landestopografie&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.li.admin.ch/en' target='_blank'&gt;Post and Telecommunications Surveillance Service&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Microsoft / Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Base map: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Federal Office of Topography swisstopo &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.li.admin.ch/fr' target='_blank'&gt;Service Surveillance de la correspondance par poste et télécommunication&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Microsoft / Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;plan de base: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Office fédéral de topographie swisstopo&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.li.admin.ch/it' target='_blank'&gt;Servizio Sorveglianza della corrispondenza postale e del traffico delle telecomunicazioni&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Microsoft / Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;carta di base: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Ufficio federale di topografia swisstopo&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.li.admin.ch/rm' target='_blank'&gt;Servetsch da surveglianza dal traffic da posta e da telecommunicaziun&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Microsoft / Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Basiskarte: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Bundesamt für Landestopografie&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>nfTrans</t>
@@ -1610,22 +1586,70 @@
     <t>Auch Funkzellenabfrage oder Rasterfahndung genannt, erfasst alle Mobiltelefone in einem Gebiet.</t>
   </si>
   <si>
-    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden.&lt;br&gt;</t>
-  </si>
-  <si>
     <t>Swiss Lawful Interception Report 2015</t>
   </si>
   <si>
-    <t>Die Digitale Gesellschaft ist ein offener Zusammenschluss netzpolitisch interessierter Kreise. Dem Bündnis angeschlossen sind rund 50 Einzelpersonen und 15 Gruppierungen. Dazu gehören Grundrechtsorganisationen, Parteien, KünstlerInnen-Kollektive, BetreiberInnen von Netzwerkdiensten und weiteren Gruppen, die sich der kritischen, digitalen Zivilgesellschaft verpflichtet fühlen. &lt;br&gt;&lt;br&gt;Weitere Informationen zu netzpolitischen Themen sind im Blog zu finden: &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;&lt;br&gt;&lt;br&gt;Programmierung: Ueli Kunz, &lt;a href='http://ideadapt.net'&gt;ideadapt.net&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Delicts Gravant</t>
   </si>
   <si>
     <t>sämtliche Handlungen, welche geeignet sind, die Ermittlung der Herkunft, die Auffindung oder die Einziehung von Vermögenswerten zu vereiteln.</t>
   </si>
   <si>
-    <t>Menschen anwerben, anbieten, vermitteln oder beherbergen durch Anwendung unerlaubternMittel wie Täuschung, Drohung oder Nötigung zum Zwecke der Ausbeutung.</t>
+    <t>Schwere Straftaten sind Delikte die hervorgehoben sind, da diese immer wieder ins Feld geführt werden, um Überwachung zu rechtfertigen.</t>
+  </si>
+  <si>
+    <t>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>En plus de cette visualisation de la surveillance la société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>In aggiunta a questa visualizzazione della sorveglianza. La società digitale pubblica una relazione annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Le Swiss Lawful Interception Report può essere scaricato qui. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Menschen anwerben, anbieten, vermitteln oder beherbergen durch Anwendung unerlaubter Mittel wie Täuschung, Drohung oder Nötigung zum Zwecke der Ausbeutung.</t>
+  </si>
+  <si>
+    <t>betroffene Facebook Accounts. Diese Liste der Facebook Daten zeigt den Umfang auf.</t>
+  </si>
+  <si>
+    <t>betroffene Microsoft/Skype Accounts</t>
+  </si>
+  <si>
+    <t>Die Digitale Gesellschaft ist ein offener Zusammenschluss netzpolitisch interessierter Kreise. Dem Bündnis angeschlossen sind rund 50 Einzelpersonen und 15 Gruppierungen. Dazu gehören Grundrechts- organisationen, Parteien, KünstlerInnen-Kollektive, BetreiberInnen von Netzwerkdiensten und weiteren Gruppen, die sich der kritischen, digitalen Zivilgesellschaft verpflichtet fühlen. &lt;br&gt;&lt;br&gt;Weitere Informationen zu netzpolitischen Themen sind im Blog zu finden: &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;&lt;br&gt;&lt;br&gt;Programmierung: Ueli Kunz, &lt;a href='http://ideadapt.net'&gt;ideadapt.net&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>Normale Telefonüberwachung</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/de' target='_blank'&gt;Dienst Überwachung Post- und Fernmeldeverkehr&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Microsoft / Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Basiskarte: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Bundesamt für Landestopografie&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/fr' target='_blank'&gt;Service Surveillance de la correspondance par poste et télécommunication&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Microsoft/Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;plan de base: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Office fédéral de topographie swisstopo&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/en' target='_blank'&gt;Post and Telecommunications Surveillance Service&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Microsoft/Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Base map: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Federal Office of Topography swisstopo &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/it' target='_blank'&gt;Servizio Sorveglianza della corrispondenza postale e del traffico delle telecomunicazioni&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt; Microsoft/Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;carta di base: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Ufficio federale di topografia swisstopo&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/rm' target='_blank'&gt;Servetsch da surveglianza dal traffic da posta e da telecommunicaziun&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Microsoft/Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Basiskarte: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Bundesamt für Landestopografie&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Strukturierte Gruppe, welche mittels Gewaltverbrechen oder sich durch verbrecherische Mittel</t>
+  </si>
+  <si>
+    <t>Einkünfte bereichert, wie Mafia oder Djihad</t>
+  </si>
+  <si>
+    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.&lt;br&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1685,7 +1709,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="195">
+  <cellStyleXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1876,6 +1900,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1906,7 +1940,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="195">
+  <cellStyles count="205">
     <cellStyle name="Besuchter Link" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
@@ -2012,6 +2046,11 @@
     <cellStyle name="Besuchter Link" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
@@ -2101,6 +2140,11 @@
     <cellStyle name="Link" xfId="188" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -2170,9 +2214,21 @@
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="slirv_translations" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="slirv_translations_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="slirv_translations_2" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:J116" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J116"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:J117" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J117">
+    <filterColumn colId="9">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="10">
     <tableColumn id="1" name="group" dataDxfId="9"/>
     <tableColumn id="2" name="typ" dataDxfId="8"/>
@@ -2511,10 +2567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I110" sqref="I110"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2553,10 +2609,10 @@
         <v>175</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2752,7 +2808,7 @@
         <v>414</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="1"/>
@@ -2768,19 +2824,19 @@
         <v>112</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="1"/>
@@ -2838,7 +2894,7 @@
         <v>389</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="1"/>
@@ -2966,19 +3022,19 @@
         <v>417</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>433</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="1"/>
@@ -3006,7 +3062,7 @@
         <v>298</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="1"/>
@@ -3047,22 +3103,22 @@
         <v>55</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>436</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="1"/>
@@ -3103,22 +3159,22 @@
         <v>55</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>427</v>
       </c>
       <c r="I20" s="6">
         <v>1</v>
@@ -3133,22 +3189,22 @@
         <v>55</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>447</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="1"/>
@@ -3191,22 +3247,22 @@
         <v>55</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>476</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="I23" s="6">
         <v>1</v>
@@ -3221,22 +3277,22 @@
         <v>55</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>472</v>
-      </c>
       <c r="E24" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>480</v>
       </c>
       <c r="I24" s="6">
         <v>1</v>
@@ -3251,22 +3307,22 @@
         <v>55</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>473</v>
-      </c>
       <c r="E25" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>484</v>
       </c>
       <c r="I25" s="6">
         <v>1</v>
@@ -4186,7 +4242,7 @@
         <v>284</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I56" s="6"/>
       <c r="J56" s="1"/>
@@ -4214,7 +4270,7 @@
         <v>285</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="1"/>
@@ -4270,7 +4326,7 @@
         <v>286</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I59" s="6"/>
       <c r="J59" s="1"/>
@@ -4326,7 +4382,7 @@
         <v>280</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I61" s="6"/>
       <c r="J61" s="1"/>
@@ -4398,7 +4454,7 @@
         <v>86</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>327</v>
@@ -4438,7 +4494,7 @@
         <v>343</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I65" s="6"/>
       <c r="J65" s="1"/>
@@ -4510,7 +4566,7 @@
         <v>90</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>134</v>
@@ -4522,7 +4578,7 @@
         <v>278</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I68" s="6"/>
       <c r="J68" s="1"/>
@@ -4566,19 +4622,7 @@
         <v>92</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>330</v>
+        <v>509</v>
       </c>
       <c r="I70" s="6"/>
       <c r="J70" s="1"/>
@@ -4622,16 +4666,16 @@
         <v>63</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="G72" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>456</v>
       </c>
       <c r="I72" s="6"/>
       <c r="J72" s="1"/>
@@ -4815,7 +4859,7 @@
         <v>103</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>416</v>
@@ -4843,19 +4887,7 @@
         <v>97</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>420</v>
+        <v>510</v>
       </c>
       <c r="I80" s="6"/>
       <c r="J80" s="1"/>
@@ -4871,7 +4903,7 @@
         <v>100</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>416</v>
@@ -5207,7 +5239,7 @@
         <v>64</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>402</v>
@@ -5219,7 +5251,7 @@
         <v>404</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I93" s="6"/>
       <c r="J93" s="1"/>
@@ -5235,44 +5267,44 @@
         <v>59</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>405</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="I94" s="6"/>
       <c r="J94" s="1"/>
     </row>
-    <row r="95" spans="1:10" ht="45">
+    <row r="95" spans="1:10" ht="45" hidden="1">
       <c r="A95" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>310</v>
       </c>
       <c r="D95" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="G95" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="H95" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
@@ -5296,12 +5328,12 @@
         <v>310</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>491</v>
+        <v>522</v>
       </c>
       <c r="I96" s="6"/>
       <c r="J96" s="1"/>
     </row>
-    <row r="97" spans="1:10" ht="30">
+    <row r="97" spans="1:10">
       <c r="A97" s="4" t="s">
         <v>0</v>
       </c>
@@ -5312,7 +5344,7 @@
         <v>311</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>485</v>
+        <v>523</v>
       </c>
       <c r="I97" s="6"/>
       <c r="J97" s="1"/>
@@ -5457,32 +5489,23 @@
       <c r="I102" s="6"/>
       <c r="J102" s="1"/>
     </row>
-    <row r="103" spans="1:10" ht="60">
+    <row r="103" spans="1:10">
       <c r="A103" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>459</v>
+        <v>526</v>
       </c>
       <c r="I103" s="6"/>
       <c r="J103" s="1"/>
     </row>
-    <row r="104" spans="1:10" ht="45">
+    <row r="104" spans="1:10" ht="60">
       <c r="A104" s="4" t="s">
         <v>113</v>
       </c>
@@ -5490,47 +5513,44 @@
         <v>63</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>460</v>
+        <v>512</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="I104" s="6"/>
       <c r="J104" s="1"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" ht="45">
       <c r="A105" s="4" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>71</v>
+        <v>458</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>400</v>
+        <v>459</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>265</v>
+        <v>460</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="H105" s="1" t="s">
-        <v>363</v>
+        <v>461</v>
       </c>
       <c r="I105" s="6"/>
       <c r="J105" s="1"/>
@@ -5543,22 +5563,22 @@
         <v>55</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>68</v>
+        <v>400</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>68</v>
+        <v>265</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>68</v>
+        <v>295</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>68</v>
+        <v>363</v>
       </c>
       <c r="I106" s="6"/>
       <c r="J106" s="1"/>
@@ -5571,22 +5591,22 @@
         <v>55</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>401</v>
+        <v>68</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>264</v>
+        <v>68</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>296</v>
+        <v>68</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>364</v>
+        <v>68</v>
       </c>
       <c r="I107" s="6"/>
       <c r="J107" s="1"/>
@@ -5599,140 +5619,152 @@
         <v>55</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>70</v>
+        <v>401</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I108" s="6"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109" spans="1:10" s="1" customFormat="1">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:10">
+      <c r="A109" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="I109" s="6"/>
+      <c r="J109" s="1"/>
+    </row>
+    <row r="110" spans="1:10" s="1" customFormat="1">
+      <c r="A110" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C109" s="1" t="s">
+      <c r="B110" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="E109" s="1" t="str">
+      <c r="D110" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E110" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
         <v>Swiss Lawful Interception Report 2015</v>
       </c>
-      <c r="F109" s="1" t="str">
+      <c r="F110" s="1" t="str">
         <f>Tabelle2[[#This Row],[en]]</f>
         <v>Swiss Lawful Interception Report 2015</v>
       </c>
-      <c r="G109" s="1" t="str">
+      <c r="G110" s="1" t="str">
         <f>Tabelle2[[#This Row],[fr]]</f>
         <v>Swiss Lawful Interception Report 2015</v>
       </c>
-      <c r="H109" s="1" t="str">
+      <c r="H110" s="1" t="str">
         <f>Tabelle2[[#This Row],[it]]</f>
         <v>Swiss Lawful Interception Report 2015</v>
       </c>
-      <c r="I109" s="1">
+      <c r="I110" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="45">
-      <c r="A110" s="4" t="s">
+    <row r="111" spans="1:10" ht="45">
+      <c r="A111" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C111" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="E110" s="1" t="str">
+      <c r="D111" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E111" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
         <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
-      <c r="F110" s="1" t="str">
+      <c r="F111" s="1" t="str">
         <f>Tabelle2[[#This Row],[en]]</f>
         <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
-      <c r="G110" s="1" t="str">
+      <c r="G111" s="1" t="str">
         <f>Tabelle2[[#This Row],[fr]]</f>
         <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
-      <c r="H110" s="1" t="str">
+      <c r="H111" s="1" t="str">
         <f>Tabelle2[[#This Row],[it]]</f>
         <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
-      <c r="I110" s="6">
-        <v>1</v>
-      </c>
-      <c r="J110" s="1"/>
-    </row>
-    <row r="111" spans="1:10" ht="330">
-      <c r="A111" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>497</v>
-      </c>
       <c r="I111" s="6">
         <v>1</v>
       </c>
       <c r="J111" s="1"/>
     </row>
-    <row r="112" spans="1:10" ht="270">
-      <c r="A112" s="4" t="s">
+    <row r="112" spans="1:10" ht="409">
+      <c r="A112" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C112" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="I112" s="6"/>
+      <c r="C112" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="I112" s="6">
+        <v>1</v>
+      </c>
       <c r="J112" s="1"/>
     </row>
-    <row r="113" spans="1:10" ht="120">
+    <row r="113" spans="1:10" ht="270">
       <c r="A113" s="4" t="s">
         <v>318</v>
       </c>
@@ -5740,29 +5772,15 @@
         <v>63</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>514</v>
+        <v>319</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="H113" s="1" t="s">
         <v>506</v>
       </c>
       <c r="I113" s="6"/>
-      <c r="J113" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" ht="105">
+      <c r="J113" s="1"/>
+    </row>
+    <row r="114" spans="1:10" ht="120" hidden="1">
       <c r="A114" s="4" t="s">
         <v>318</v>
       </c>
@@ -5772,30 +5790,27 @@
       <c r="C114" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="D114" s="1" t="str">
-        <f>CONCATENATE("&lt;a href='",D110,"' title='",D109,"' target='_blank'&gt;",D109,"&lt;/a&gt;")</f>
-        <v>&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
+      <c r="D114" s="1" t="s">
+        <v>525</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="I114" s="6">
-        <v>1</v>
-      </c>
+        <v>497</v>
+      </c>
+      <c r="I114" s="6"/>
       <c r="J114" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="210">
+    <row r="115" spans="1:10" ht="105" hidden="1">
       <c r="A115" s="4" t="s">
         <v>318</v>
       </c>
@@ -5803,63 +5818,96 @@
         <v>63</v>
       </c>
       <c r="C115" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D115" s="1" t="str">
+        <f>CONCATENATE("&lt;a href='",D111,"' title='",D110,"' target='_blank'&gt;",D110,"&lt;/a&gt;")</f>
+        <v>&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="I115" s="6">
+        <v>1</v>
+      </c>
+      <c r="J115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="210">
+      <c r="A116" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C116" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="D115" s="1" t="str">
-        <f>CONCATENATE(D113,D114)</f>
-        <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden.&lt;br&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
-      </c>
-      <c r="E115" s="1" t="str">
-        <f>CONCATENATE(E113,E114)</f>
+      <c r="D116" s="1" t="str">
+        <f>CONCATENATE(D114,D115)</f>
+        <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.&lt;br&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
+      </c>
+      <c r="E116" s="1" t="str">
+        <f>CONCATENATE(E114,E115)</f>
         <v>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</v>
       </c>
-      <c r="F115" s="1" t="str">
-        <f t="shared" ref="F115:H115" si="0">CONCATENATE(F113,F114)</f>
+      <c r="F116" s="1" t="str">
+        <f t="shared" ref="F116:H116" si="0">CONCATENATE(F114,F115)</f>
         <v>En plus de cette visualisation de la surveillance la société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</v>
       </c>
-      <c r="G115" s="1" t="str">
+      <c r="G116" s="1" t="str">
         <f t="shared" si="0"/>
         <v>In aggiunta a questa visualizzazione della sorveglianza. La società digitale pubblica una relazione annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Le Swiss Lawful Interception Report può essere scaricato qui. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</v>
       </c>
-      <c r="H115" s="1" t="str">
+      <c r="H116" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
-      <c r="I115" s="6">
+      <c r="I116" s="6">
         <v>1</v>
       </c>
-      <c r="J115" s="1"/>
-    </row>
-    <row r="116" spans="1:10" ht="300">
-      <c r="A116" s="4" t="s">
+      <c r="J116" s="1"/>
+    </row>
+    <row r="117" spans="1:10" ht="300">
+      <c r="A117" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C117" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="E116" s="1" t="s">
+      <c r="E117" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="H117" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="G116" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="I116" s="6"/>
-      <c r="J116" s="1"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I108 I110:I1048576">
+  <conditionalFormatting sqref="I1:I109 I111:I1048576">
     <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",I1)))</formula>
     </cfRule>
@@ -5875,4 +5923,2912 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G5" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" t="s">
+        <v>412</v>
+      </c>
+      <c r="F7" t="s">
+        <v>413</v>
+      </c>
+      <c r="G7" t="s">
+        <v>414</v>
+      </c>
+      <c r="H7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" t="s">
+        <v>441</v>
+      </c>
+      <c r="E8" t="s">
+        <v>440</v>
+      </c>
+      <c r="F8" t="s">
+        <v>439</v>
+      </c>
+      <c r="G8" t="s">
+        <v>438</v>
+      </c>
+      <c r="H8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>375</v>
+      </c>
+      <c r="E9" t="s">
+        <v>374</v>
+      </c>
+      <c r="F9" t="s">
+        <v>374</v>
+      </c>
+      <c r="G9" t="s">
+        <v>374</v>
+      </c>
+      <c r="H9" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F10" t="s">
+        <v>387</v>
+      </c>
+      <c r="G10" t="s">
+        <v>389</v>
+      </c>
+      <c r="H10" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" t="s">
+        <v>335</v>
+      </c>
+      <c r="F11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H11" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" t="s">
+        <v>336</v>
+      </c>
+      <c r="F12" t="s">
+        <v>392</v>
+      </c>
+      <c r="G12" t="s">
+        <v>393</v>
+      </c>
+      <c r="H12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>325</v>
+      </c>
+      <c r="D13" t="s">
+        <v>383</v>
+      </c>
+      <c r="E13" t="s">
+        <v>383</v>
+      </c>
+      <c r="F13" t="s">
+        <v>383</v>
+      </c>
+      <c r="G13" t="s">
+        <v>383</v>
+      </c>
+      <c r="H13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>326</v>
+      </c>
+      <c r="D14" t="s">
+        <v>384</v>
+      </c>
+      <c r="E14" t="s">
+        <v>385</v>
+      </c>
+      <c r="F14" t="s">
+        <v>386</v>
+      </c>
+      <c r="G14" t="s">
+        <v>388</v>
+      </c>
+      <c r="H14" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>417</v>
+      </c>
+      <c r="D15" t="s">
+        <v>428</v>
+      </c>
+      <c r="E15" t="s">
+        <v>429</v>
+      </c>
+      <c r="F15" t="s">
+        <v>430</v>
+      </c>
+      <c r="G15" t="s">
+        <v>431</v>
+      </c>
+      <c r="H15" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" t="s">
+        <v>338</v>
+      </c>
+      <c r="F16" t="s">
+        <v>297</v>
+      </c>
+      <c r="G16" t="s">
+        <v>298</v>
+      </c>
+      <c r="H16" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" t="s">
+        <v>266</v>
+      </c>
+      <c r="G17" t="s">
+        <v>299</v>
+      </c>
+      <c r="H17" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>433</v>
+      </c>
+      <c r="D18" t="s">
+        <v>434</v>
+      </c>
+      <c r="E18" t="s">
+        <v>434</v>
+      </c>
+      <c r="F18" t="s">
+        <v>433</v>
+      </c>
+      <c r="G18" t="s">
+        <v>435</v>
+      </c>
+      <c r="H18" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>334</v>
+      </c>
+      <c r="F19" t="s">
+        <v>267</v>
+      </c>
+      <c r="G19" t="s">
+        <v>300</v>
+      </c>
+      <c r="H19" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>427</v>
+      </c>
+      <c r="D20" t="s">
+        <v>422</v>
+      </c>
+      <c r="E20" t="s">
+        <v>423</v>
+      </c>
+      <c r="F20" t="s">
+        <v>424</v>
+      </c>
+      <c r="G20" t="s">
+        <v>425</v>
+      </c>
+      <c r="H20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>442</v>
+      </c>
+      <c r="D21" t="s">
+        <v>494</v>
+      </c>
+      <c r="E21" t="s">
+        <v>443</v>
+      </c>
+      <c r="F21" t="s">
+        <v>444</v>
+      </c>
+      <c r="G21" t="s">
+        <v>445</v>
+      </c>
+      <c r="H21" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>406</v>
+      </c>
+      <c r="D22" t="s">
+        <v>407</v>
+      </c>
+      <c r="E22" t="s">
+        <v>411</v>
+      </c>
+      <c r="F22" t="s">
+        <v>408</v>
+      </c>
+      <c r="G22" t="s">
+        <v>409</v>
+      </c>
+      <c r="H22" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>467</v>
+      </c>
+      <c r="D23" t="s">
+        <v>472</v>
+      </c>
+      <c r="E23" t="s">
+        <v>472</v>
+      </c>
+      <c r="F23" t="s">
+        <v>474</v>
+      </c>
+      <c r="G23" t="s">
+        <v>473</v>
+      </c>
+      <c r="H23" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>468</v>
+      </c>
+      <c r="D24" t="s">
+        <v>470</v>
+      </c>
+      <c r="E24" t="s">
+        <v>475</v>
+      </c>
+      <c r="F24" t="s">
+        <v>476</v>
+      </c>
+      <c r="G24" t="s">
+        <v>477</v>
+      </c>
+      <c r="H24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>469</v>
+      </c>
+      <c r="D25" t="s">
+        <v>471</v>
+      </c>
+      <c r="E25" t="s">
+        <v>479</v>
+      </c>
+      <c r="F25" t="s">
+        <v>480</v>
+      </c>
+      <c r="G25" t="s">
+        <v>481</v>
+      </c>
+      <c r="H25" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" t="s">
+        <v>236</v>
+      </c>
+      <c r="G26" t="s">
+        <v>237</v>
+      </c>
+      <c r="H26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>320</v>
+      </c>
+      <c r="D27" t="s">
+        <v>321</v>
+      </c>
+      <c r="E27" t="s">
+        <v>322</v>
+      </c>
+      <c r="F27" t="s">
+        <v>323</v>
+      </c>
+      <c r="G27" t="s">
+        <v>324</v>
+      </c>
+      <c r="H27" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
+        <v>189</v>
+      </c>
+      <c r="G28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H28" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" t="s">
+        <v>186</v>
+      </c>
+      <c r="G29" t="s">
+        <v>201</v>
+      </c>
+      <c r="H29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" t="s">
+        <v>187</v>
+      </c>
+      <c r="G30" t="s">
+        <v>202</v>
+      </c>
+      <c r="H30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" t="s">
+        <v>188</v>
+      </c>
+      <c r="G31" t="s">
+        <v>203</v>
+      </c>
+      <c r="H31" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" t="s">
+        <v>145</v>
+      </c>
+      <c r="G32" t="s">
+        <v>204</v>
+      </c>
+      <c r="H32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" t="s">
+        <v>149</v>
+      </c>
+      <c r="F33" t="s">
+        <v>190</v>
+      </c>
+      <c r="G33" t="s">
+        <v>205</v>
+      </c>
+      <c r="H33" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" t="s">
+        <v>191</v>
+      </c>
+      <c r="G34" t="s">
+        <v>206</v>
+      </c>
+      <c r="H34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" t="s">
+        <v>150</v>
+      </c>
+      <c r="F35" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" t="s">
+        <v>207</v>
+      </c>
+      <c r="H35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" t="s">
+        <v>208</v>
+      </c>
+      <c r="H36" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F37" t="s">
+        <v>151</v>
+      </c>
+      <c r="G37" t="s">
+        <v>209</v>
+      </c>
+      <c r="H37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" t="s">
+        <v>152</v>
+      </c>
+      <c r="G38" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" t="s">
+        <v>192</v>
+      </c>
+      <c r="G39" t="s">
+        <v>210</v>
+      </c>
+      <c r="H39" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" t="s">
+        <v>193</v>
+      </c>
+      <c r="G40" t="s">
+        <v>211</v>
+      </c>
+      <c r="H40" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" t="s">
+        <v>194</v>
+      </c>
+      <c r="G41" t="s">
+        <v>212</v>
+      </c>
+      <c r="H41" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
+        <v>195</v>
+      </c>
+      <c r="G42" t="s">
+        <v>213</v>
+      </c>
+      <c r="H42" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>196</v>
+      </c>
+      <c r="G43" t="s">
+        <v>214</v>
+      </c>
+      <c r="H43" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" t="s">
+        <v>197</v>
+      </c>
+      <c r="G44" t="s">
+        <v>215</v>
+      </c>
+      <c r="H44" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" t="s">
+        <v>198</v>
+      </c>
+      <c r="G45" t="s">
+        <v>216</v>
+      </c>
+      <c r="H45" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" t="s">
+        <v>48</v>
+      </c>
+      <c r="E46" t="s">
+        <v>153</v>
+      </c>
+      <c r="F46" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" t="s">
+        <v>153</v>
+      </c>
+      <c r="H46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" t="s">
+        <v>49</v>
+      </c>
+      <c r="G47" t="s">
+        <v>49</v>
+      </c>
+      <c r="H47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" t="s">
+        <v>154</v>
+      </c>
+      <c r="F48" t="s">
+        <v>154</v>
+      </c>
+      <c r="G48" t="s">
+        <v>154</v>
+      </c>
+      <c r="H48" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" t="s">
+        <v>155</v>
+      </c>
+      <c r="F49" t="s">
+        <v>155</v>
+      </c>
+      <c r="G49" t="s">
+        <v>217</v>
+      </c>
+      <c r="H49" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" t="s">
+        <v>199</v>
+      </c>
+      <c r="G50" t="s">
+        <v>218</v>
+      </c>
+      <c r="H50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" t="s">
+        <v>156</v>
+      </c>
+      <c r="F51" t="s">
+        <v>156</v>
+      </c>
+      <c r="G51" t="s">
+        <v>219</v>
+      </c>
+      <c r="H51" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" t="s">
+        <v>248</v>
+      </c>
+      <c r="G52" t="s">
+        <v>248</v>
+      </c>
+      <c r="H52" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" t="s">
+        <v>131</v>
+      </c>
+      <c r="F53" t="s">
+        <v>249</v>
+      </c>
+      <c r="G53" t="s">
+        <v>282</v>
+      </c>
+      <c r="H53" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" t="s">
+        <v>132</v>
+      </c>
+      <c r="F54" t="s">
+        <v>250</v>
+      </c>
+      <c r="G54" t="s">
+        <v>283</v>
+      </c>
+      <c r="H54" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F55" t="s">
+        <v>251</v>
+      </c>
+      <c r="G55" t="s">
+        <v>276</v>
+      </c>
+      <c r="H55" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" t="s">
+        <v>137</v>
+      </c>
+      <c r="F56" t="s">
+        <v>252</v>
+      </c>
+      <c r="G56" t="s">
+        <v>284</v>
+      </c>
+      <c r="H56" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" t="s">
+        <v>79</v>
+      </c>
+      <c r="E57" t="s">
+        <v>136</v>
+      </c>
+      <c r="F57" t="s">
+        <v>253</v>
+      </c>
+      <c r="G57" t="s">
+        <v>285</v>
+      </c>
+      <c r="H57" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" t="s">
+        <v>106</v>
+      </c>
+      <c r="E58" t="s">
+        <v>134</v>
+      </c>
+      <c r="F58" t="s">
+        <v>244</v>
+      </c>
+      <c r="G58" t="s">
+        <v>278</v>
+      </c>
+      <c r="H58" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" t="s">
+        <v>135</v>
+      </c>
+      <c r="F59" t="s">
+        <v>254</v>
+      </c>
+      <c r="G59" t="s">
+        <v>286</v>
+      </c>
+      <c r="H59" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" t="s">
+        <v>138</v>
+      </c>
+      <c r="F60" t="s">
+        <v>246</v>
+      </c>
+      <c r="G60" t="s">
+        <v>279</v>
+      </c>
+      <c r="H60" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" t="s">
+        <v>81</v>
+      </c>
+      <c r="E61" t="s">
+        <v>139</v>
+      </c>
+      <c r="F61" t="s">
+        <v>247</v>
+      </c>
+      <c r="G61" t="s">
+        <v>280</v>
+      </c>
+      <c r="H61" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" t="s">
+        <v>314</v>
+      </c>
+      <c r="E62" t="s">
+        <v>315</v>
+      </c>
+      <c r="F62" t="s">
+        <v>316</v>
+      </c>
+      <c r="G62" t="s">
+        <v>317</v>
+      </c>
+      <c r="H62" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" t="s">
+        <v>416</v>
+      </c>
+      <c r="E63" t="s">
+        <v>416</v>
+      </c>
+      <c r="F63" t="s">
+        <v>416</v>
+      </c>
+      <c r="G63" t="s">
+        <v>416</v>
+      </c>
+      <c r="H63" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" t="s">
+        <v>507</v>
+      </c>
+      <c r="E64" t="s">
+        <v>327</v>
+      </c>
+      <c r="F64" t="s">
+        <v>328</v>
+      </c>
+      <c r="G64" t="s">
+        <v>329</v>
+      </c>
+      <c r="H64" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65" t="s">
+        <v>339</v>
+      </c>
+      <c r="E65" t="s">
+        <v>340</v>
+      </c>
+      <c r="F65" t="s">
+        <v>341</v>
+      </c>
+      <c r="G65" t="s">
+        <v>343</v>
+      </c>
+      <c r="H65" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" t="s">
+        <v>88</v>
+      </c>
+      <c r="D66" t="s">
+        <v>169</v>
+      </c>
+      <c r="E66" t="s">
+        <v>170</v>
+      </c>
+      <c r="F66" t="s">
+        <v>242</v>
+      </c>
+      <c r="G66" t="s">
+        <v>342</v>
+      </c>
+      <c r="H66" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" t="s">
+        <v>89</v>
+      </c>
+      <c r="D67" t="s">
+        <v>167</v>
+      </c>
+      <c r="E67" t="s">
+        <v>168</v>
+      </c>
+      <c r="F67" t="s">
+        <v>243</v>
+      </c>
+      <c r="G67" t="s">
+        <v>277</v>
+      </c>
+      <c r="H67" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" t="s">
+        <v>508</v>
+      </c>
+      <c r="E68" t="s">
+        <v>134</v>
+      </c>
+      <c r="F68" t="s">
+        <v>244</v>
+      </c>
+      <c r="G68" t="s">
+        <v>278</v>
+      </c>
+      <c r="H68" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" t="s">
+        <v>165</v>
+      </c>
+      <c r="E69" t="s">
+        <v>166</v>
+      </c>
+      <c r="F69" t="s">
+        <v>245</v>
+      </c>
+      <c r="G69" t="s">
+        <v>166</v>
+      </c>
+      <c r="H69" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" t="s">
+        <v>93</v>
+      </c>
+      <c r="D71" t="s">
+        <v>353</v>
+      </c>
+      <c r="E71" t="s">
+        <v>354</v>
+      </c>
+      <c r="F71" t="s">
+        <v>355</v>
+      </c>
+      <c r="G71" t="s">
+        <v>356</v>
+      </c>
+      <c r="H71" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" t="s">
+        <v>516</v>
+      </c>
+      <c r="E72" t="s">
+        <v>452</v>
+      </c>
+      <c r="F72" t="s">
+        <v>453</v>
+      </c>
+      <c r="G72" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>94</v>
+      </c>
+      <c r="B73" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" t="s">
+        <v>102</v>
+      </c>
+      <c r="E73" t="s">
+        <v>395</v>
+      </c>
+      <c r="F73" t="s">
+        <v>258</v>
+      </c>
+      <c r="G73" t="s">
+        <v>290</v>
+      </c>
+      <c r="H73" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74" t="s">
+        <v>97</v>
+      </c>
+      <c r="D74" t="s">
+        <v>96</v>
+      </c>
+      <c r="E74" t="s">
+        <v>396</v>
+      </c>
+      <c r="F74" t="s">
+        <v>259</v>
+      </c>
+      <c r="G74" t="s">
+        <v>291</v>
+      </c>
+      <c r="H74" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" t="s">
+        <v>100</v>
+      </c>
+      <c r="D75" t="s">
+        <v>99</v>
+      </c>
+      <c r="E75" t="s">
+        <v>397</v>
+      </c>
+      <c r="F75" t="s">
+        <v>260</v>
+      </c>
+      <c r="G75" t="s">
+        <v>292</v>
+      </c>
+      <c r="H75" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" t="s">
+        <v>101</v>
+      </c>
+      <c r="D76" t="s">
+        <v>171</v>
+      </c>
+      <c r="E76" t="s">
+        <v>398</v>
+      </c>
+      <c r="F76" t="s">
+        <v>261</v>
+      </c>
+      <c r="G76" t="s">
+        <v>293</v>
+      </c>
+      <c r="H76" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" t="s">
+        <v>95</v>
+      </c>
+      <c r="D77" t="s">
+        <v>104</v>
+      </c>
+      <c r="E77" t="s">
+        <v>140</v>
+      </c>
+      <c r="F77" t="s">
+        <v>262</v>
+      </c>
+      <c r="G77" t="s">
+        <v>140</v>
+      </c>
+      <c r="H77" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>94</v>
+      </c>
+      <c r="B78" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78" t="s">
+        <v>98</v>
+      </c>
+      <c r="D78" t="s">
+        <v>107</v>
+      </c>
+      <c r="E78" t="s">
+        <v>399</v>
+      </c>
+      <c r="F78" t="s">
+        <v>263</v>
+      </c>
+      <c r="G78" t="s">
+        <v>294</v>
+      </c>
+      <c r="H78" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79" t="s">
+        <v>63</v>
+      </c>
+      <c r="C79" t="s">
+        <v>103</v>
+      </c>
+      <c r="D79" t="s">
+        <v>515</v>
+      </c>
+      <c r="E79" t="s">
+        <v>416</v>
+      </c>
+      <c r="F79" t="s">
+        <v>416</v>
+      </c>
+      <c r="G79" t="s">
+        <v>416</v>
+      </c>
+      <c r="H79" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80" t="s">
+        <v>63</v>
+      </c>
+      <c r="C80" t="s">
+        <v>97</v>
+      </c>
+      <c r="D80" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="D81" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" t="s">
+        <v>63</v>
+      </c>
+      <c r="C82" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" t="s">
+        <v>521</v>
+      </c>
+      <c r="E82" t="s">
+        <v>416</v>
+      </c>
+      <c r="F82" t="s">
+        <v>416</v>
+      </c>
+      <c r="G82" t="s">
+        <v>416</v>
+      </c>
+      <c r="H82" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" t="s">
+        <v>63</v>
+      </c>
+      <c r="C83" t="s">
+        <v>101</v>
+      </c>
+      <c r="D83" t="s">
+        <v>161</v>
+      </c>
+      <c r="E83" t="s">
+        <v>162</v>
+      </c>
+      <c r="F83" t="s">
+        <v>255</v>
+      </c>
+      <c r="G83" t="s">
+        <v>287</v>
+      </c>
+      <c r="H83" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" t="s">
+        <v>63</v>
+      </c>
+      <c r="C84" t="s">
+        <v>95</v>
+      </c>
+      <c r="D84" t="s">
+        <v>159</v>
+      </c>
+      <c r="E84" t="s">
+        <v>160</v>
+      </c>
+      <c r="F84" t="s">
+        <v>256</v>
+      </c>
+      <c r="G84" t="s">
+        <v>288</v>
+      </c>
+      <c r="H84" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" t="s">
+        <v>63</v>
+      </c>
+      <c r="C85" t="s">
+        <v>98</v>
+      </c>
+      <c r="D85" t="s">
+        <v>163</v>
+      </c>
+      <c r="E85" t="s">
+        <v>164</v>
+      </c>
+      <c r="F85" t="s">
+        <v>257</v>
+      </c>
+      <c r="G85" t="s">
+        <v>289</v>
+      </c>
+      <c r="H85" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" t="s">
+        <v>58</v>
+      </c>
+      <c r="D86" t="s">
+        <v>61</v>
+      </c>
+      <c r="E86" t="s">
+        <v>142</v>
+      </c>
+      <c r="F86" t="s">
+        <v>269</v>
+      </c>
+      <c r="G86" t="s">
+        <v>302</v>
+      </c>
+      <c r="H86" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" t="s">
+        <v>60</v>
+      </c>
+      <c r="D87" t="s">
+        <v>367</v>
+      </c>
+      <c r="E87" t="s">
+        <v>368</v>
+      </c>
+      <c r="F87" t="s">
+        <v>369</v>
+      </c>
+      <c r="G87" t="s">
+        <v>370</v>
+      </c>
+      <c r="H87" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" t="s">
+        <v>64</v>
+      </c>
+      <c r="D88" t="s">
+        <v>65</v>
+      </c>
+      <c r="E88" t="s">
+        <v>143</v>
+      </c>
+      <c r="F88" t="s">
+        <v>270</v>
+      </c>
+      <c r="G88" t="s">
+        <v>303</v>
+      </c>
+      <c r="H88" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C89" t="s">
+        <v>59</v>
+      </c>
+      <c r="D89" t="s">
+        <v>62</v>
+      </c>
+      <c r="E89" t="s">
+        <v>172</v>
+      </c>
+      <c r="F89" t="s">
+        <v>271</v>
+      </c>
+      <c r="G89" t="s">
+        <v>304</v>
+      </c>
+      <c r="H89" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" t="s">
+        <v>55</v>
+      </c>
+      <c r="C90" t="s">
+        <v>310</v>
+      </c>
+      <c r="D90" t="s">
+        <v>312</v>
+      </c>
+      <c r="E90" t="s">
+        <v>312</v>
+      </c>
+      <c r="F90" t="s">
+        <v>312</v>
+      </c>
+      <c r="G90" t="s">
+        <v>312</v>
+      </c>
+      <c r="H90" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" t="s">
+        <v>55</v>
+      </c>
+      <c r="C91" t="s">
+        <v>311</v>
+      </c>
+      <c r="D91" t="s">
+        <v>313</v>
+      </c>
+      <c r="E91" t="s">
+        <v>313</v>
+      </c>
+      <c r="F91" t="s">
+        <v>313</v>
+      </c>
+      <c r="G91" t="s">
+        <v>313</v>
+      </c>
+      <c r="H91" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" t="s">
+        <v>63</v>
+      </c>
+      <c r="C92" t="s">
+        <v>58</v>
+      </c>
+      <c r="D92" t="s">
+        <v>376</v>
+      </c>
+      <c r="E92" t="s">
+        <v>158</v>
+      </c>
+      <c r="F92" t="s">
+        <v>268</v>
+      </c>
+      <c r="G92" t="s">
+        <v>301</v>
+      </c>
+      <c r="H92" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
+        <v>63</v>
+      </c>
+      <c r="C93" t="s">
+        <v>60</v>
+      </c>
+      <c r="D93" t="s">
+        <v>377</v>
+      </c>
+      <c r="E93" t="s">
+        <v>379</v>
+      </c>
+      <c r="F93" t="s">
+        <v>380</v>
+      </c>
+      <c r="G93" t="s">
+        <v>381</v>
+      </c>
+      <c r="H93" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" t="s">
+        <v>63</v>
+      </c>
+      <c r="C94" t="s">
+        <v>64</v>
+      </c>
+      <c r="D94" t="s">
+        <v>511</v>
+      </c>
+      <c r="E94" t="s">
+        <v>402</v>
+      </c>
+      <c r="F94" t="s">
+        <v>403</v>
+      </c>
+      <c r="G94" t="s">
+        <v>404</v>
+      </c>
+      <c r="H94" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>63</v>
+      </c>
+      <c r="C95" t="s">
+        <v>59</v>
+      </c>
+      <c r="D95" t="s">
+        <v>490</v>
+      </c>
+      <c r="E95" t="s">
+        <v>491</v>
+      </c>
+      <c r="F95" t="s">
+        <v>492</v>
+      </c>
+      <c r="G95" t="s">
+        <v>405</v>
+      </c>
+      <c r="H95" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" t="s">
+        <v>63</v>
+      </c>
+      <c r="C96" t="s">
+        <v>310</v>
+      </c>
+      <c r="D96" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>63</v>
+      </c>
+      <c r="C97" t="s">
+        <v>311</v>
+      </c>
+      <c r="D97" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" t="s">
+        <v>113</v>
+      </c>
+      <c r="B98" t="s">
+        <v>55</v>
+      </c>
+      <c r="C98" t="s">
+        <v>120</v>
+      </c>
+      <c r="D98" t="s">
+        <v>124</v>
+      </c>
+      <c r="E98" t="s">
+        <v>126</v>
+      </c>
+      <c r="F98" t="s">
+        <v>238</v>
+      </c>
+      <c r="G98" t="s">
+        <v>272</v>
+      </c>
+      <c r="H98" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>113</v>
+      </c>
+      <c r="B99" t="s">
+        <v>55</v>
+      </c>
+      <c r="C99" t="s">
+        <v>68</v>
+      </c>
+      <c r="D99" t="s">
+        <v>72</v>
+      </c>
+      <c r="E99" t="s">
+        <v>68</v>
+      </c>
+      <c r="F99" t="s">
+        <v>68</v>
+      </c>
+      <c r="G99" t="s">
+        <v>68</v>
+      </c>
+      <c r="H99" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>113</v>
+      </c>
+      <c r="B100" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" t="s">
+        <v>122</v>
+      </c>
+      <c r="E100" t="s">
+        <v>127</v>
+      </c>
+      <c r="F100" t="s">
+        <v>239</v>
+      </c>
+      <c r="G100" t="s">
+        <v>273</v>
+      </c>
+      <c r="H100" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>113</v>
+      </c>
+      <c r="B101" t="s">
+        <v>55</v>
+      </c>
+      <c r="C101" t="s">
+        <v>70</v>
+      </c>
+      <c r="D101" t="s">
+        <v>74</v>
+      </c>
+      <c r="E101" t="s">
+        <v>129</v>
+      </c>
+      <c r="F101" t="s">
+        <v>240</v>
+      </c>
+      <c r="G101" t="s">
+        <v>68</v>
+      </c>
+      <c r="H101" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>113</v>
+      </c>
+      <c r="B102" t="s">
+        <v>55</v>
+      </c>
+      <c r="C102" t="s">
+        <v>119</v>
+      </c>
+      <c r="D102" t="s">
+        <v>123</v>
+      </c>
+      <c r="E102" t="s">
+        <v>128</v>
+      </c>
+      <c r="F102" t="s">
+        <v>241</v>
+      </c>
+      <c r="G102" t="s">
+        <v>275</v>
+      </c>
+      <c r="H102" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>113</v>
+      </c>
+      <c r="B103" t="s">
+        <v>55</v>
+      </c>
+      <c r="C103" t="s">
+        <v>119</v>
+      </c>
+      <c r="D103" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>113</v>
+      </c>
+      <c r="B104" t="s">
+        <v>63</v>
+      </c>
+      <c r="C104" t="s">
+        <v>120</v>
+      </c>
+      <c r="D104" t="s">
+        <v>512</v>
+      </c>
+      <c r="E104" t="s">
+        <v>455</v>
+      </c>
+      <c r="F104" t="s">
+        <v>456</v>
+      </c>
+      <c r="G104" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" t="s">
+        <v>63</v>
+      </c>
+      <c r="C105" t="s">
+        <v>121</v>
+      </c>
+      <c r="D105" t="s">
+        <v>458</v>
+      </c>
+      <c r="E105" t="s">
+        <v>459</v>
+      </c>
+      <c r="F105" t="s">
+        <v>460</v>
+      </c>
+      <c r="G105" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>66</v>
+      </c>
+      <c r="B106" t="s">
+        <v>55</v>
+      </c>
+      <c r="C106" t="s">
+        <v>67</v>
+      </c>
+      <c r="D106" t="s">
+        <v>71</v>
+      </c>
+      <c r="E106" t="s">
+        <v>400</v>
+      </c>
+      <c r="F106" t="s">
+        <v>265</v>
+      </c>
+      <c r="G106" t="s">
+        <v>295</v>
+      </c>
+      <c r="H106" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>66</v>
+      </c>
+      <c r="B107" t="s">
+        <v>55</v>
+      </c>
+      <c r="C107" t="s">
+        <v>68</v>
+      </c>
+      <c r="D107" t="s">
+        <v>72</v>
+      </c>
+      <c r="E107" t="s">
+        <v>68</v>
+      </c>
+      <c r="F107" t="s">
+        <v>68</v>
+      </c>
+      <c r="G107" t="s">
+        <v>68</v>
+      </c>
+      <c r="H107" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>66</v>
+      </c>
+      <c r="B108" t="s">
+        <v>55</v>
+      </c>
+      <c r="C108" t="s">
+        <v>69</v>
+      </c>
+      <c r="D108" t="s">
+        <v>73</v>
+      </c>
+      <c r="E108" t="s">
+        <v>401</v>
+      </c>
+      <c r="F108" t="s">
+        <v>264</v>
+      </c>
+      <c r="G108" t="s">
+        <v>296</v>
+      </c>
+      <c r="H108" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" t="s">
+        <v>66</v>
+      </c>
+      <c r="B109" t="s">
+        <v>55</v>
+      </c>
+      <c r="C109" t="s">
+        <v>70</v>
+      </c>
+      <c r="D109" t="s">
+        <v>74</v>
+      </c>
+      <c r="E109" t="s">
+        <v>70</v>
+      </c>
+      <c r="F109" t="s">
+        <v>240</v>
+      </c>
+      <c r="G109" t="s">
+        <v>274</v>
+      </c>
+      <c r="H109" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" t="s">
+        <v>418</v>
+      </c>
+      <c r="B110" t="s">
+        <v>55</v>
+      </c>
+      <c r="C110" t="s">
+        <v>325</v>
+      </c>
+      <c r="D110" t="s">
+        <v>513</v>
+      </c>
+      <c r="E110" t="s">
+        <v>513</v>
+      </c>
+      <c r="F110" t="s">
+        <v>513</v>
+      </c>
+      <c r="G110" t="s">
+        <v>513</v>
+      </c>
+      <c r="H110" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" t="s">
+        <v>418</v>
+      </c>
+      <c r="B111" t="s">
+        <v>419</v>
+      </c>
+      <c r="C111" t="s">
+        <v>325</v>
+      </c>
+      <c r="D111" t="s">
+        <v>447</v>
+      </c>
+      <c r="E111" t="s">
+        <v>447</v>
+      </c>
+      <c r="F111" t="s">
+        <v>447</v>
+      </c>
+      <c r="G111" t="s">
+        <v>447</v>
+      </c>
+      <c r="H111" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
+        <v>318</v>
+      </c>
+      <c r="B112" t="s">
+        <v>63</v>
+      </c>
+      <c r="C112" t="s">
+        <v>417</v>
+      </c>
+      <c r="D112" t="s">
+        <v>527</v>
+      </c>
+      <c r="E112" t="s">
+        <v>529</v>
+      </c>
+      <c r="F112" t="s">
+        <v>528</v>
+      </c>
+      <c r="G112" t="s">
+        <v>530</v>
+      </c>
+      <c r="H112" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" t="s">
+        <v>318</v>
+      </c>
+      <c r="B113" t="s">
+        <v>63</v>
+      </c>
+      <c r="C113" t="s">
+        <v>319</v>
+      </c>
+      <c r="D113" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>318</v>
+      </c>
+      <c r="B114" t="s">
+        <v>63</v>
+      </c>
+      <c r="C114" t="s">
+        <v>325</v>
+      </c>
+      <c r="D114" t="s">
+        <v>534</v>
+      </c>
+      <c r="E114" t="s">
+        <v>517</v>
+      </c>
+      <c r="F114" t="s">
+        <v>518</v>
+      </c>
+      <c r="G114" t="s">
+        <v>519</v>
+      </c>
+      <c r="H114" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
+        <v>318</v>
+      </c>
+      <c r="B115" t="s">
+        <v>63</v>
+      </c>
+      <c r="C115" t="s">
+        <v>326</v>
+      </c>
+      <c r="D115" t="s">
+        <v>524</v>
+      </c>
+      <c r="E115" t="s">
+        <v>462</v>
+      </c>
+      <c r="F115" t="s">
+        <v>463</v>
+      </c>
+      <c r="G115" t="s">
+        <v>464</v>
+      </c>
+      <c r="H115" t="s">
+        <v>465</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Translations Update: Excelfile der Übersetzungen
</commit_message>
<xml_diff>
--- a/_specs/slirv_translations.xlsx
+++ b/_specs/slirv_translations.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Blatt2" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="slirv_translations" localSheetId="0">Blatt1!$A$2:$H$117</definedName>
+    <definedName name="slirv_translations" localSheetId="0">Blatt1!$A$2:$H$118</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="534">
   <si>
     <t>typ</t>
   </si>
@@ -1535,27 +1535,15 @@
     <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden.</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</t>
-  </si>
-  <si>
     <t>En plus de cette visualisation de la surveillance la société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici.</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</t>
-  </si>
-  <si>
     <t>In aggiunta a questa visualizzazione della sorveglianza. La società digitale pubblica una relazione annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Le Swiss Lawful Interception Report può essere scaricato qui.</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</t>
-  </si>
-  <si>
     <t>slir_intro</t>
   </si>
   <si>
@@ -1586,18 +1574,6 @@
     <t>Schwere Straftaten sind Delikte die hervorgehoben sind, da diese immer wieder ins Feld geführt werden, um Überwachung zu rechtfertigen.</t>
   </si>
   <si>
-    <t>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>En plus de cette visualisation de la surveillance la société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>In aggiunta a questa visualizzazione della sorveglianza. La società digitale pubblica una relazione annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Le Swiss Lawful Interception Report può essere scaricato qui. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Menschen anwerben, anbieten, vermitteln oder beherbergen durch Anwendung unerlaubter Mittel wie Täuschung, Drohung oder Nötigung zum Zwecke der Ausbeutung.</t>
   </si>
   <si>
@@ -1625,9 +1601,6 @@
     <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/rm' target='_blank'&gt;Servetsch da surveglianza dal traffic da posta e da telecommunicaziun&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Microsoft/Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Basiskarte: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Bundesamt für Landestopografie&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.&lt;br&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Geldwäscherei bedeutet, die Ermittlung der Herkunft, die Auffindung oder die Einziehung von Vermögenswerten zu vereiteln.</t>
   </si>
   <si>
@@ -1641,6 +1614,36 @@
   </si>
   <si>
     <t>Microsoft &amp; Skype</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>nur_deutsch</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Nur in Deutsch verfügbar</t>
+  </si>
+  <si>
+    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>En plus de cette visualisation de la surveillance la société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>In aggiunta a questa visualizzazione della sorveglianza. La società digitale pubblica una relazione annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Le Swiss Lawful Interception Report può essere scaricato qui.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;Nur in Deutsch verfügbar</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1730,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="209">
+  <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1918,6 +1921,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1965,7 +1976,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="209">
+  <cellStyles count="217">
     <cellStyle name="Besuchter Link" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
@@ -2078,6 +2089,10 @@
     <cellStyle name="Besuchter Link" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
@@ -2174,9 +2189,23 @@
     <cellStyle name="Link" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2224,16 +2253,6 @@
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -2244,23 +2263,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:J117" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:J118" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:J118">
     <filterColumn colId="9">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="group" dataDxfId="9"/>
-    <tableColumn id="2" name="typ" dataDxfId="8"/>
-    <tableColumn id="3" name="detail" dataDxfId="7"/>
-    <tableColumn id="4" name="de" dataDxfId="6"/>
-    <tableColumn id="5" name="en" dataDxfId="5"/>
-    <tableColumn id="6" name="fr" dataDxfId="4"/>
-    <tableColumn id="7" name="it" dataDxfId="3"/>
-    <tableColumn id="8" name="rm" dataDxfId="2"/>
-    <tableColumn id="9" name="nfTrans" dataDxfId="1"/>
-    <tableColumn id="10" name="notEXport" dataDxfId="0"/>
+    <tableColumn id="1" name="group" dataDxfId="10"/>
+    <tableColumn id="2" name="typ" dataDxfId="9"/>
+    <tableColumn id="3" name="detail" dataDxfId="8"/>
+    <tableColumn id="4" name="de" dataDxfId="7"/>
+    <tableColumn id="5" name="en" dataDxfId="6"/>
+    <tableColumn id="6" name="fr" dataDxfId="5"/>
+    <tableColumn id="7" name="it" dataDxfId="4"/>
+    <tableColumn id="8" name="rm" dataDxfId="3"/>
+    <tableColumn id="9" name="nfTrans" dataDxfId="2"/>
+    <tableColumn id="10" name="notEXport" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2588,10 +2607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J117"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="H117" sqref="A1:H117"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2915,7 +2934,7 @@
         <v>388</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="1"/>
@@ -4475,7 +4494,7 @@
         <v>86</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>326</v>
@@ -4587,7 +4606,7 @@
         <v>90</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>134</v>
@@ -4643,7 +4662,7 @@
         <v>92</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="I70" s="6"/>
       <c r="J70" s="1"/>
@@ -4687,7 +4706,7 @@
         <v>63</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>451</v>
@@ -4880,7 +4899,7 @@
         <v>103</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>415</v>
@@ -4908,7 +4927,7 @@
         <v>97</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="I80" s="6"/>
       <c r="J80" s="1"/>
@@ -4924,7 +4943,7 @@
         <v>100</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>415</v>
@@ -5176,7 +5195,7 @@
         <v>311</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="E90" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
@@ -5264,7 +5283,7 @@
         <v>64</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>401</v>
@@ -5353,7 +5372,7 @@
         <v>310</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="I96" s="6"/>
       <c r="J96" s="1"/>
@@ -5369,19 +5388,19 @@
         <v>311</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="I97" s="6"/>
       <c r="J97" s="1"/>
@@ -5537,7 +5556,7 @@
         <v>119</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="I103" s="6"/>
       <c r="J103" s="1"/>
@@ -5553,7 +5572,7 @@
         <v>120</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>454</v>
@@ -5704,7 +5723,7 @@
       <c r="I109" s="6"/>
       <c r="J109" s="1"/>
     </row>
-    <row r="110" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="110" spans="1:10" s="1" customFormat="1">
       <c r="A110" s="1" t="s">
         <v>417</v>
       </c>
@@ -5715,7 +5734,7 @@
         <v>324</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="E110" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
@@ -5782,19 +5801,19 @@
         <v>416</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="I112" s="6">
         <v>1</v>
@@ -5812,7 +5831,7 @@
         <v>318</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="I113" s="6"/>
       <c r="J113" s="1"/>
@@ -5825,19 +5844,19 @@
         <v>63</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="E114" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="F114" s="1" t="s">
-        <v>500</v>
-      </c>
       <c r="G114" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>496</v>
@@ -5847,7 +5866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="105" hidden="1">
+    <row r="115" spans="1:10" ht="30" hidden="1">
       <c r="A115" s="4" t="s">
         <v>317</v>
       </c>
@@ -5855,32 +5874,29 @@
         <v>63</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>495</v>
-      </c>
-      <c r="D115" s="1" t="str">
-        <f>CONCATENATE("&lt;a href='",D111,"' title='",D110,"' target='_blank'&gt;",D110,"&lt;/a&gt;")</f>
-        <v>&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
+        <v>526</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>528</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>499</v>
+        <v>524</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>501</v>
+        <v>527</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>503</v>
+        <v>525</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="I115" s="6">
-        <v>1</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="I115" s="6"/>
       <c r="J115" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="210">
+    <row r="116" spans="1:10" ht="135" hidden="1">
       <c r="A116" s="4" t="s">
         <v>317</v>
       </c>
@@ -5888,34 +5904,36 @@
         <v>63</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>324</v>
+        <v>495</v>
       </c>
       <c r="D116" s="1" t="str">
-        <f>CONCATENATE(D114,D115)</f>
-        <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.&lt;br&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
+        <f>CONCATENATE("&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='",D111,"' title='",D110,"' target='_blank'&gt;",D110,"&lt;/a&gt;")</f>
+        <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
       <c r="E116" s="1" t="str">
-        <f>CONCATENATE(E114,E115)</f>
-        <v>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</v>
+        <f t="shared" ref="E116:H116" si="0">CONCATENATE("&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='",E111,"' title='",E110,"' target='_blank'&gt;",E110,"&lt;/a&gt;")</f>
+        <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f t="shared" ref="F116:H116" si="0">CONCATENATE(F114,F115)</f>
-        <v>En plus de cette visualisation de la surveillance la société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
       <c r="G116" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>In aggiunta a questa visualizzazione della sorveglianza. La società digitale pubblica una relazione annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Le Swiss Lawful Interception Report può essere scaricato qui. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</v>
+        <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
       <c r="H116" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden. &lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' &gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
+        <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
       <c r="I116" s="6">
         <v>1</v>
       </c>
-      <c r="J116" s="1"/>
-    </row>
-    <row r="117" spans="1:10" ht="300">
+      <c r="J116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="285">
       <c r="A117" s="4" t="s">
         <v>317</v>
       </c>
@@ -5923,29 +5941,64 @@
         <v>63</v>
       </c>
       <c r="C117" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D117" s="1" t="str">
+        <f>CONCATENATE(D114,D116)</f>
+        <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
+      </c>
+      <c r="E117" s="1" t="str">
+        <f t="shared" ref="E117:H117" si="1">CONCATENATE(E114,E116,E115)</f>
+        <v>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</v>
+      </c>
+      <c r="F117" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>En plus de cette visualisation de la surveillance la société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</v>
+      </c>
+      <c r="G117" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>In aggiunta a questa visualizzazione della sorveglianza. La società digitale pubblica una relazione annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Le Swiss Lawful Interception Report può essere scaricato qui.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</v>
+      </c>
+      <c r="H117" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;Nur in Deutsch verfügbar</v>
+      </c>
+      <c r="I117" s="6">
+        <v>1</v>
+      </c>
+      <c r="J117" s="1"/>
+    </row>
+    <row r="118" spans="1:10" ht="300">
+      <c r="A118" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C118" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="E117" s="1" t="s">
+      <c r="D118" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="F118" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="G118" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="H117" s="1" t="s">
+      <c r="H118" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="I117" s="6"/>
-      <c r="J117" s="1"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I109 I111:I1048576">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6229,7 +6282,7 @@
         <v>388</v>
       </c>
       <c r="H10" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -7621,7 +7674,7 @@
         <v>86</v>
       </c>
       <c r="D64" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="E64" t="s">
         <v>326</v>
@@ -7725,7 +7778,7 @@
         <v>90</v>
       </c>
       <c r="D68" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="E68" t="s">
         <v>134</v>
@@ -7777,7 +7830,7 @@
         <v>92</v>
       </c>
       <c r="D70" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -7817,7 +7870,7 @@
         <v>63</v>
       </c>
       <c r="D72" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E72" t="s">
         <v>451</v>
@@ -7996,7 +8049,7 @@
         <v>103</v>
       </c>
       <c r="D79" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="E79" t="s">
         <v>415</v>
@@ -8022,7 +8075,7 @@
         <v>97</v>
       </c>
       <c r="D80" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -8036,7 +8089,7 @@
         <v>100</v>
       </c>
       <c r="D81" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="E81" t="s">
         <v>415</v>
@@ -8270,19 +8323,19 @@
         <v>311</v>
       </c>
       <c r="D90" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="E90" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="F90" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="G90" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="H90" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -8348,7 +8401,7 @@
         <v>64</v>
       </c>
       <c r="D93" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E93" t="s">
         <v>401</v>
@@ -8400,7 +8453,7 @@
         <v>310</v>
       </c>
       <c r="D95" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -8414,19 +8467,19 @@
         <v>311</v>
       </c>
       <c r="D96" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="E96" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="F96" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="G96" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="H96" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -8570,7 +8623,7 @@
         <v>119</v>
       </c>
       <c r="D102" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -8584,7 +8637,7 @@
         <v>120</v>
       </c>
       <c r="D103" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="E103" t="s">
         <v>454</v>
@@ -8734,19 +8787,19 @@
         <v>324</v>
       </c>
       <c r="D109" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="E109" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F109" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="G109" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="H109" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -8786,19 +8839,19 @@
         <v>416</v>
       </c>
       <c r="D111" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="E111" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="F111" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="G111" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="H111" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -8812,7 +8865,7 @@
         <v>318</v>
       </c>
       <c r="D112" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -8826,19 +8879,19 @@
         <v>324</v>
       </c>
       <c r="D113" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E113" t="s">
-        <v>514</v>
+        <v>530</v>
       </c>
       <c r="F113" t="s">
-        <v>515</v>
+        <v>531</v>
       </c>
       <c r="G113" t="s">
-        <v>516</v>
+        <v>532</v>
       </c>
       <c r="H113" t="s">
-        <v>517</v>
+        <v>533</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -8852,7 +8905,7 @@
         <v>325</v>
       </c>
       <c r="D114" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="E114" t="s">
         <v>461</v>

</xml_diff>

<commit_message>
Ordner für Original Translations, wird am Ende wieder gelöscht. Update Master Translations
</commit_message>
<xml_diff>
--- a/_specs/slirv_translations.xlsx
+++ b/_specs/slirv_translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="10000" windowWidth="30940" windowHeight="18560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3260" yWindow="2540" windowWidth="28640" windowHeight="19080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="trans" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="slirv_translations" localSheetId="1">Blatt3!$A$2:$H$117</definedName>
-    <definedName name="slirv_translations" localSheetId="0">trans!$A$2:$H$117</definedName>
+    <definedName name="slirv_translations" localSheetId="0">trans!$A$2:$H$118</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="559">
   <si>
     <t>typ</t>
   </si>
@@ -1696,6 +1696,30 @@
   </si>
   <si>
     <t>Il Digital Society Switzerland pubblica annualmente l'intercettazione legale Relazione svizzera sui cantoni della Svizzera. Questa visualizzazione completa il rapporto interattivo e mostra in dettaglio, quante persone sono interessate nei Cantoni. Scopri quali crimini stanno limitando le vostre libertà fondamentali. &lt;br&gt;&lt;small&gt;I dati di queste statistiche includono soltanto misure di vigilanza in conformità con il codice di procedura penale. Fatta eccezione per le operazioni di cacciatori IMSI, trojan governative o di sorveglianza delle agenzie di intelligence.&lt;/small&gt;</t>
+  </si>
+  <si>
+    <t>Visualisierung zur staatlichen Überwachung in der Schweiz</t>
+  </si>
+  <si>
+    <t>Die Digitale Gesellschaft ist ein offener Zusammenschluss netzpolitisch interessierter Kreise. Dem Bündnis angeschlossen sind rund 50 Einzelpersonen und 15 Gruppierungen. Dazu gehören Grundrechtsorganisationen, Parteien, KünstlerInnen-Kollektive, BetreiberInnen von Netzwerkdiensten und weiteren Gruppen, die sich der kritischen, digitalen Zivilgesellschaft verpflichtet fühlen. &lt;br&gt;&lt;br&gt;Weitere Informationen zu netzpolitischen Themen sind im Blog zu finden: &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;&lt;br&gt;&lt;br&gt;Programmierung: Ueli Kunz, &lt;a href='http://ideadapt.net'&gt;ideadapt.net&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Schwere Straftaten sind als Delikte hervorgehoben, da diese immer wieder ins Feld geführt werden, um Überwachung zu rechtfertigen.</t>
+  </si>
+  <si>
+    <t>fullscreen</t>
+  </si>
+  <si>
+    <t>in den Vollbildmodus wechseln</t>
+  </si>
+  <si>
+    <t>switch to full screen mode</t>
+  </si>
+  <si>
+    <t>passer en mode plein écran</t>
+  </si>
+  <si>
+    <t>passare alla modalità a schermo intero</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1806,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="223">
+  <cellStyleXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1973,6 +1997,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2034,7 +2062,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="223">
+  <cellStyles count="227">
     <cellStyle name="Besuchter Link" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
@@ -2154,6 +2182,8 @@
     <cellStyle name="Besuchter Link" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
@@ -2257,6 +2287,8 @@
     <cellStyle name="Link" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -2331,12 +2363,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:J117" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:J117">
-    <filterColumn colId="9">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:J118" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:J118"/>
   <tableColumns count="10">
     <tableColumn id="1" name="group" dataDxfId="10"/>
     <tableColumn id="2" name="typ" dataDxfId="9"/>
@@ -2675,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J117"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="H117" sqref="A1:H117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2960,7 +2988,7 @@
         <v>111</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>370</v>
+        <v>551</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>369</v>
@@ -3231,7 +3259,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" hidden="1">
+    <row r="19" spans="1:10">
       <c r="A19" s="4" t="s">
         <v>55</v>
       </c>
@@ -3261,127 +3289,122 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1">
-      <c r="A20" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="5" t="s">
+    <row r="20" spans="1:10" ht="30">
+      <c r="A20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I21" s="6">
         <v>1</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J21" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="4" t="s">
+    <row r="22" spans="1:10">
+      <c r="A22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" ht="45" hidden="1">
-      <c r="A22" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="I22" s="6"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="45">
+      <c r="A23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="I22" s="6">
-        <v>1</v>
-      </c>
-      <c r="J22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>467</v>
       </c>
       <c r="I23" s="6">
         <v>1</v>
       </c>
-      <c r="J23" s="7"/>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="5" t="s">
@@ -3391,22 +3414,22 @@
         <v>55</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="I24" s="6">
         <v>1</v>
@@ -3421,57 +3444,59 @@
         <v>55</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I25" s="6">
         <v>1</v>
       </c>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="1:10" ht="30">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="I26" s="6"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="B26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="I26" s="6">
+        <v>1</v>
+      </c>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" ht="30">
       <c r="A27" s="4" t="s">
         <v>2</v>
       </c>
@@ -3479,54 +3504,52 @@
         <v>55</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>315</v>
+        <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>316</v>
+        <v>29</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>317</v>
+        <v>142</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>318</v>
+        <v>234</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>319</v>
+        <v>235</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="I28" s="6">
-        <v>1</v>
-      </c>
+      <c r="B28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="I28" s="6"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10">
@@ -3537,22 +3560,22 @@
         <v>55</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>145</v>
+        <v>33</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="I29" s="6">
         <v>1</v>
@@ -3567,22 +3590,22 @@
         <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I30" s="6">
         <v>1</v>
@@ -3597,22 +3620,22 @@
         <v>55</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>302</v>
+        <v>219</v>
       </c>
       <c r="I31" s="6">
         <v>1</v>
@@ -3627,22 +3650,22 @@
         <v>55</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>143</v>
+        <v>186</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>220</v>
+        <v>302</v>
       </c>
       <c r="I32" s="6">
         <v>1</v>
@@ -3657,22 +3680,22 @@
         <v>55</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>188</v>
+        <v>143</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I33" s="6">
         <v>1</v>
@@ -3687,22 +3710,22 @@
         <v>55</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>36</v>
+        <v>147</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I34" s="6">
         <v>1</v>
@@ -3717,22 +3740,22 @@
         <v>55</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>148</v>
+        <v>36</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I35" s="6">
         <v>1</v>
@@ -3747,22 +3770,22 @@
         <v>55</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="I36" s="6">
         <v>1</v>
@@ -3777,22 +3800,22 @@
         <v>55</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>149</v>
+        <v>38</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>149</v>
+        <v>38</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I37" s="6">
         <v>1</v>
@@ -3807,22 +3830,22 @@
         <v>55</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="I38" s="6">
         <v>1</v>
@@ -3837,22 +3860,22 @@
         <v>55</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>41</v>
+        <v>150</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I39" s="6">
         <v>1</v>
@@ -3867,22 +3890,22 @@
         <v>55</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I40" s="6">
         <v>1</v>
@@ -3897,22 +3920,22 @@
         <v>55</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I41" s="6">
         <v>1</v>
@@ -3927,22 +3950,22 @@
         <v>55</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I42" s="6">
         <v>1</v>
@@ -3957,22 +3980,22 @@
         <v>55</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I43" s="6">
         <v>1</v>
@@ -3987,22 +4010,22 @@
         <v>55</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I44" s="6">
         <v>1</v>
@@ -4017,22 +4040,22 @@
         <v>55</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="I45" s="6">
         <v>1</v>
@@ -4047,22 +4070,22 @@
         <v>55</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>48</v>
+        <v>196</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>48</v>
+        <v>214</v>
       </c>
       <c r="I46" s="6">
         <v>1</v>
@@ -4077,22 +4100,22 @@
         <v>55</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I47" s="6">
         <v>1</v>
@@ -4107,22 +4130,22 @@
         <v>55</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>231</v>
+        <v>49</v>
       </c>
       <c r="I48" s="6">
         <v>1</v>
@@ -4137,22 +4160,22 @@
         <v>55</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>215</v>
+        <v>152</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I49" s="6">
         <v>1</v>
@@ -4167,22 +4190,22 @@
         <v>55</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>52</v>
+        <v>153</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>52</v>
+        <v>232</v>
       </c>
       <c r="I50" s="6">
         <v>1</v>
@@ -4197,22 +4220,22 @@
         <v>55</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>154</v>
+        <v>52</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>154</v>
+        <v>197</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>233</v>
+        <v>52</v>
       </c>
       <c r="I51" s="6">
         <v>1</v>
@@ -4221,28 +4244,28 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="5" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>245</v>
+        <v>154</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
       <c r="I52" s="6">
         <v>1</v>
@@ -4250,31 +4273,33 @@
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="I53" s="6"/>
+      <c r="B53" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I53" s="6">
+        <v>1</v>
+      </c>
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10">
@@ -4285,22 +4310,22 @@
         <v>55</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>410</v>
+        <v>246</v>
       </c>
       <c r="I54" s="6"/>
       <c r="J54" s="1"/>
@@ -4313,22 +4338,22 @@
         <v>55</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>326</v>
+        <v>410</v>
       </c>
       <c r="I55" s="6"/>
       <c r="J55" s="1"/>
@@ -4341,22 +4366,22 @@
         <v>55</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>443</v>
+        <v>326</v>
       </c>
       <c r="I56" s="6"/>
       <c r="J56" s="1"/>
@@ -4369,22 +4394,22 @@
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="1"/>
@@ -4397,22 +4422,22 @@
         <v>55</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>345</v>
+        <v>444</v>
       </c>
       <c r="I58" s="6"/>
       <c r="J58" s="1"/>
@@ -4425,22 +4450,22 @@
         <v>55</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>445</v>
+        <v>345</v>
       </c>
       <c r="I59" s="6"/>
       <c r="J59" s="1"/>
@@ -4453,22 +4478,22 @@
         <v>55</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>325</v>
+        <v>445</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="1"/>
@@ -4481,55 +4506,55 @@
         <v>55</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>446</v>
+        <v>325</v>
       </c>
       <c r="I61" s="6"/>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="1:10" ht="30">
+    <row r="62" spans="1:10">
       <c r="A62" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>309</v>
+        <v>81</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>310</v>
+        <v>137</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>311</v>
+        <v>244</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>312</v>
+        <v>276</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>344</v>
+        <v>446</v>
       </c>
       <c r="I62" s="6"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" ht="30">
       <c r="A63" s="4" t="s">
         <v>75</v>
       </c>
@@ -4537,27 +4562,27 @@
         <v>63</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>411</v>
+        <v>309</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>411</v>
+        <v>310</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>411</v>
+        <v>311</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>411</v>
+        <v>312</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>411</v>
+        <v>344</v>
       </c>
       <c r="I63" s="6"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10" ht="30">
+    <row r="64" spans="1:10">
       <c r="A64" s="4" t="s">
         <v>75</v>
       </c>
@@ -4565,22 +4590,22 @@
         <v>63</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>497</v>
+        <v>411</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>322</v>
+        <v>411</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>323</v>
+        <v>411</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>324</v>
+        <v>411</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>346</v>
+        <v>411</v>
       </c>
       <c r="I64" s="6"/>
       <c r="J64" s="1"/>
@@ -4593,27 +4618,27 @@
         <v>63</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>334</v>
+        <v>497</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>460</v>
+        <v>346</v>
       </c>
       <c r="I65" s="6"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:10" ht="45">
+    <row r="66" spans="1:10" ht="30">
       <c r="A66" s="4" t="s">
         <v>75</v>
       </c>
@@ -4621,22 +4646,22 @@
         <v>63</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>167</v>
+        <v>334</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>168</v>
+        <v>335</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>239</v>
+        <v>336</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>341</v>
+        <v>460</v>
       </c>
       <c r="I66" s="6"/>
       <c r="J66" s="1"/>
@@ -4649,27 +4674,27 @@
         <v>63</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>273</v>
+        <v>337</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I67" s="6"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="1:10" ht="60">
+    <row r="68" spans="1:10" ht="45">
       <c r="A68" s="4" t="s">
         <v>75</v>
       </c>
@@ -4677,27 +4702,27 @@
         <v>63</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>498</v>
+        <v>165</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>416</v>
+        <v>342</v>
       </c>
       <c r="I68" s="6"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="1:10" ht="30">
+    <row r="69" spans="1:10" ht="60">
       <c r="A69" s="4" t="s">
         <v>75</v>
       </c>
@@ -4705,27 +4730,27 @@
         <v>63</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>163</v>
+        <v>498</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>164</v>
+        <v>274</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>347</v>
+        <v>416</v>
       </c>
       <c r="I69" s="6"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="1:10" ht="60">
+    <row r="70" spans="1:10" ht="30">
       <c r="A70" s="4" t="s">
         <v>75</v>
       </c>
@@ -4733,24 +4758,27 @@
         <v>63</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>499</v>
+        <v>163</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>530</v>
+        <v>164</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>531</v>
+        <v>242</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>532</v>
+        <v>164</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="I70" s="6"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="1:10" ht="30">
+    <row r="71" spans="1:10" ht="60">
       <c r="A71" s="4" t="s">
         <v>75</v>
       </c>
@@ -4758,75 +4786,72 @@
         <v>63</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>348</v>
+        <v>499</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>349</v>
+        <v>530</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>350</v>
+        <v>531</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>352</v>
+        <v>532</v>
       </c>
       <c r="I71" s="6"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="1:10" ht="60">
+    <row r="72" spans="1:10" ht="30">
       <c r="A72" s="4" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>503</v>
+        <v>348</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>447</v>
+        <v>349</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>448</v>
+        <v>350</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>449</v>
+        <v>351</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="I72" s="6"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" ht="60">
       <c r="A73" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>102</v>
+        <v>553</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>390</v>
+        <v>447</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>255</v>
+        <v>448</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>340</v>
+        <v>449</v>
       </c>
       <c r="I73" s="6"/>
       <c r="J73" s="1"/>
@@ -4839,22 +4864,22 @@
         <v>55</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="I74" s="6"/>
       <c r="J74" s="1"/>
@@ -4867,22 +4892,22 @@
         <v>55</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>339</v>
+        <v>355</v>
       </c>
       <c r="I75" s="6"/>
       <c r="J75" s="1"/>
@@ -4895,22 +4920,22 @@
         <v>55</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>169</v>
+        <v>99</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>386</v>
+        <v>339</v>
       </c>
       <c r="I76" s="6"/>
       <c r="J76" s="1"/>
@@ -4923,22 +4948,22 @@
         <v>55</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>104</v>
+        <v>169</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>138</v>
+        <v>393</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>138</v>
+        <v>289</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
       <c r="I77" s="6"/>
       <c r="J77" s="1"/>
@@ -4951,55 +4976,55 @@
         <v>55</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>394</v>
+        <v>138</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>290</v>
+        <v>138</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I78" s="6"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="1:10" ht="60">
+    <row r="79" spans="1:10">
       <c r="A79" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>513</v>
+        <v>107</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>533</v>
+        <v>394</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>534</v>
+        <v>260</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>535</v>
+        <v>290</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>411</v>
+        <v>357</v>
       </c>
       <c r="I79" s="6"/>
       <c r="J79" s="1"/>
     </row>
-    <row r="80" spans="1:10" ht="75">
+    <row r="80" spans="1:10" ht="60">
       <c r="A80" s="4" t="s">
         <v>94</v>
       </c>
@@ -5007,19 +5032,22 @@
         <v>63</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>411</v>
       </c>
       <c r="I80" s="6"/>
       <c r="J80" s="1"/>
@@ -5032,27 +5060,24 @@
         <v>63</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>411</v>
+        <v>538</v>
       </c>
       <c r="I81" s="6"/>
       <c r="J81" s="1"/>
     </row>
-    <row r="82" spans="1:10" ht="45">
+    <row r="82" spans="1:10" ht="75">
       <c r="A82" s="4" t="s">
         <v>94</v>
       </c>
@@ -5060,27 +5085,27 @@
         <v>63</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>159</v>
+        <v>504</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>160</v>
+        <v>539</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>252</v>
+        <v>540</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>283</v>
+        <v>541</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>354</v>
+        <v>411</v>
       </c>
       <c r="I82" s="6"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83" spans="1:10" ht="30">
+    <row r="83" spans="1:10" ht="45">
       <c r="A83" s="4" t="s">
         <v>94</v>
       </c>
@@ -5088,22 +5113,22 @@
         <v>63</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="I83" s="6"/>
       <c r="J83" s="1"/>
@@ -5116,50 +5141,50 @@
         <v>63</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="I84" s="6"/>
       <c r="J84" s="1"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" ht="30">
       <c r="A85" s="4" t="s">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>61</v>
+        <v>161</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>305</v>
+        <v>360</v>
       </c>
       <c r="I85" s="6"/>
       <c r="J85" s="1"/>
@@ -5172,22 +5197,22 @@
         <v>55</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>362</v>
+        <v>61</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>363</v>
+        <v>140</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>364</v>
+        <v>266</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>365</v>
+        <v>298</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>366</v>
+        <v>305</v>
       </c>
       <c r="I86" s="6"/>
       <c r="J86" s="1"/>
@@ -5200,22 +5225,22 @@
         <v>55</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>65</v>
+        <v>362</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>141</v>
+        <v>363</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>267</v>
+        <v>364</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>299</v>
+        <v>365</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>304</v>
+        <v>366</v>
       </c>
       <c r="I87" s="6"/>
       <c r="J87" s="1"/>
@@ -5228,22 +5253,22 @@
         <v>55</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I88" s="6"/>
       <c r="J88" s="1"/>
@@ -5256,22 +5281,22 @@
         <v>55</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>306</v>
+        <v>59</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>308</v>
+        <v>62</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>308</v>
+        <v>170</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>308</v>
+        <v>268</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="I89" s="6"/>
       <c r="J89" s="1"/>
@@ -5284,59 +5309,59 @@
         <v>55</v>
       </c>
       <c r="C90" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="I90" s="6"/>
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="E90" s="1" t="str">
+      <c r="E91" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
         <v>Microsoft &amp; Skype</v>
       </c>
-      <c r="F90" s="1" t="str">
+      <c r="F91" s="1" t="str">
         <f>Tabelle2[[#This Row],[en]]</f>
         <v>Microsoft &amp; Skype</v>
       </c>
-      <c r="G90" s="1" t="str">
+      <c r="G91" s="1" t="str">
         <f>Tabelle2[[#This Row],[fr]]</f>
         <v>Microsoft &amp; Skype</v>
       </c>
-      <c r="H90" s="1" t="str">
+      <c r="H91" s="1" t="str">
         <f>Tabelle2[[#This Row],[it]]</f>
         <v>Microsoft &amp; Skype</v>
       </c>
-      <c r="I90" s="6"/>
-      <c r="J90" s="1"/>
-    </row>
-    <row r="91" spans="1:10" ht="45">
-      <c r="A91" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="I91" s="6"/>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:10" ht="30">
+    <row r="92" spans="1:10" ht="45">
       <c r="A92" s="4" t="s">
         <v>0</v>
       </c>
@@ -5344,27 +5369,27 @@
         <v>63</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>374</v>
+        <v>156</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>375</v>
+        <v>265</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>376</v>
+        <v>297</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="I92" s="6"/>
       <c r="J92" s="1"/>
     </row>
-    <row r="93" spans="1:10" ht="45">
+    <row r="93" spans="1:10" ht="30">
       <c r="A93" s="4" t="s">
         <v>0</v>
       </c>
@@ -5372,27 +5397,27 @@
         <v>63</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>500</v>
+        <v>372</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>415</v>
+        <v>373</v>
       </c>
       <c r="I93" s="6"/>
       <c r="J93" s="1"/>
     </row>
-    <row r="94" spans="1:10" ht="60">
+    <row r="94" spans="1:10" ht="45">
       <c r="A94" s="4" t="s">
         <v>0</v>
       </c>
@@ -5400,85 +5425,88 @@
         <v>63</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>484</v>
+        <v>500</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>485</v>
+        <v>397</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>486</v>
+        <v>398</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>487</v>
+        <v>415</v>
       </c>
       <c r="I94" s="6"/>
       <c r="J94" s="1"/>
     </row>
-    <row r="95" spans="1:10" ht="45" hidden="1">
+    <row r="95" spans="1:10" ht="60">
       <c r="A95" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>477</v>
+        <v>63</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>478</v>
+        <v>59</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>484</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="H95" s="1" t="str">
-        <f>Tabelle2[[#This Row],[de]]</f>
-        <v>https://de-de.facebook.com/help/405183566203254</v>
-      </c>
-      <c r="I95" s="6">
-        <v>1</v>
-      </c>
-      <c r="J95" s="1">
-        <v>1</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="I95" s="6"/>
+      <c r="J95" s="1"/>
     </row>
     <row r="96" spans="1:10" ht="45">
       <c r="A96" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>63</v>
+        <v>477</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>515</v>
+      <c r="D96" s="4" t="s">
+        <v>478</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>542</v>
+        <v>479</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>543</v>
+        <v>481</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="I96" s="6"/>
-      <c r="J96" s="1"/>
-    </row>
-    <row r="97" spans="1:10" ht="30">
+        <v>480</v>
+      </c>
+      <c r="H96" s="1" t="str">
+        <f>Tabelle2[[#This Row],[de]]</f>
+        <v>https://de-de.facebook.com/help/405183566203254</v>
+      </c>
+      <c r="I96" s="6">
+        <v>1</v>
+      </c>
+      <c r="J96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="45">
       <c r="A97" s="4" t="s">
         <v>0</v>
       </c>
@@ -5486,55 +5514,52 @@
         <v>63</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>516</v>
+        <v>542</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="G97" s="8" t="s">
-        <v>516</v>
-      </c>
-      <c r="H97" s="8" t="s">
-        <v>516</v>
+        <v>543</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>544</v>
       </c>
       <c r="I97" s="6"/>
       <c r="J97" s="1"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" ht="30">
       <c r="A98" s="4" t="s">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>120</v>
+        <v>307</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>123</v>
+        <v>516</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>125</v>
+        <v>516</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>301</v>
+        <v>516</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="H98" s="8" t="s">
+        <v>516</v>
       </c>
       <c r="I98" s="6"/>
       <c r="J98" s="1"/>
     </row>
-    <row r="99" spans="1:10" hidden="1">
+    <row r="99" spans="1:10">
       <c r="A99" s="4" t="s">
         <v>113</v>
       </c>
@@ -5542,27 +5567,25 @@
         <v>55</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>68</v>
+        <v>236</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>68</v>
+        <v>269</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>68</v>
+        <v>301</v>
       </c>
       <c r="I99" s="6"/>
-      <c r="J99" s="1">
-        <v>1</v>
-      </c>
+      <c r="J99" s="1"/>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="4" t="s">
@@ -5572,27 +5595,29 @@
         <v>55</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>237</v>
+        <v>68</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>270</v>
+        <v>68</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>343</v>
+        <v>68</v>
       </c>
       <c r="I100" s="6"/>
-      <c r="J100" s="1"/>
-    </row>
-    <row r="101" spans="1:10" hidden="1">
+      <c r="J100" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" s="4" t="s">
         <v>113</v>
       </c>
@@ -5600,29 +5625,27 @@
         <v>55</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>361</v>
+        <v>270</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="I101" s="6"/>
-      <c r="J101" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" hidden="1">
+      <c r="J101" s="1"/>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="4" t="s">
         <v>113</v>
       </c>
@@ -5630,51 +5653,56 @@
         <v>55</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>507</v>
+        <v>74</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>545</v>
+        <v>127</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>547</v>
+        <v>238</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>546</v>
+        <v>361</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>361</v>
       </c>
       <c r="I102" s="6"/>
       <c r="J102" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="60">
+    <row r="103" spans="1:10">
       <c r="A103" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>528</v>
+        <v>507</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>450</v>
+        <v>545</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>451</v>
+        <v>547</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>452</v>
+        <v>546</v>
       </c>
       <c r="I103" s="6"/>
-      <c r="J103" s="1"/>
-    </row>
-    <row r="104" spans="1:10" ht="45">
+      <c r="J103" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="60">
       <c r="A104" s="4" t="s">
         <v>113</v>
       </c>
@@ -5682,47 +5710,44 @@
         <v>63</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="I104" s="6"/>
       <c r="J104" s="1"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" ht="45">
       <c r="A105" s="4" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>71</v>
+        <v>529</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>395</v>
+        <v>453</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>262</v>
+        <v>454</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="H105" s="1" t="s">
-        <v>358</v>
+        <v>455</v>
       </c>
       <c r="I105" s="6"/>
       <c r="J105" s="1"/>
@@ -5735,22 +5760,22 @@
         <v>55</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>68</v>
+        <v>395</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>68</v>
+        <v>262</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>68</v>
+        <v>291</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>68</v>
+        <v>358</v>
       </c>
       <c r="I106" s="6"/>
       <c r="J106" s="1"/>
@@ -5763,22 +5788,22 @@
         <v>55</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>396</v>
+        <v>68</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>261</v>
+        <v>68</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>292</v>
+        <v>68</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>359</v>
+        <v>68</v>
       </c>
       <c r="I107" s="6"/>
       <c r="J107" s="1"/>
@@ -5791,152 +5816,155 @@
         <v>55</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>70</v>
+        <v>396</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>271</v>
+        <v>292</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I108" s="6"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109" spans="1:10" s="1" customFormat="1" hidden="1">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:10">
+      <c r="A109" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="I109" s="6"/>
+      <c r="J109" s="1"/>
+    </row>
+    <row r="110" spans="1:10" s="1" customFormat="1">
+      <c r="A110" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C109" s="1" t="s">
+      <c r="B110" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="E109" s="1" t="str">
+      <c r="E110" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
         <v>Swiss Lawful Interception Report 2015</v>
       </c>
-      <c r="F109" s="1" t="str">
+      <c r="F110" s="1" t="str">
         <f>Tabelle2[[#This Row],[en]]</f>
         <v>Swiss Lawful Interception Report 2015</v>
       </c>
-      <c r="G109" s="1" t="str">
+      <c r="G110" s="1" t="str">
         <f>Tabelle2[[#This Row],[fr]]</f>
         <v>Swiss Lawful Interception Report 2015</v>
       </c>
-      <c r="H109" s="1" t="str">
+      <c r="H110" s="1" t="str">
         <f>Tabelle2[[#This Row],[it]]</f>
         <v>Swiss Lawful Interception Report 2015</v>
       </c>
-      <c r="I109" s="1">
+      <c r="I110" s="1">
         <v>1</v>
       </c>
-      <c r="J109" s="1">
+      <c r="J110" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="45">
-      <c r="A110" s="4" t="s">
+    <row r="111" spans="1:10" ht="45">
+      <c r="A111" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C111" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="E110" s="1" t="str">
+      <c r="E111" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
         <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
-      <c r="F110" s="1" t="str">
+      <c r="F111" s="1" t="str">
         <f>Tabelle2[[#This Row],[en]]</f>
         <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
-      <c r="G110" s="1" t="str">
+      <c r="G111" s="1" t="str">
         <f>Tabelle2[[#This Row],[fr]]</f>
         <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
-      <c r="H110" s="1" t="str">
+      <c r="H111" s="1" t="str">
         <f>Tabelle2[[#This Row],[it]]</f>
         <v>https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf</v>
       </c>
-      <c r="I110" s="6">
-        <v>1</v>
-      </c>
-      <c r="J110" s="1"/>
-    </row>
-    <row r="111" spans="1:10" ht="409">
-      <c r="A111" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>512</v>
-      </c>
       <c r="I111" s="6">
         <v>1</v>
       </c>
       <c r="J111" s="1"/>
     </row>
-    <row r="112" spans="1:10" ht="270">
-      <c r="A112" s="4" t="s">
+    <row r="112" spans="1:10" ht="409">
+      <c r="A112" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C112" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="I112" s="6"/>
+      <c r="C112" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="I112" s="6">
+        <v>1</v>
+      </c>
       <c r="J112" s="1"/>
     </row>
-    <row r="113" spans="1:10" ht="120" hidden="1">
+    <row r="113" spans="1:10" ht="270">
       <c r="A113" s="4" t="s">
         <v>313</v>
       </c>
@@ -5944,29 +5972,24 @@
         <v>63</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>495</v>
+        <v>314</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>492</v>
+        <v>548</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>493</v>
+        <v>549</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>491</v>
+        <v>550</v>
       </c>
       <c r="I113" s="6"/>
-      <c r="J113" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" ht="30" hidden="1">
+      <c r="J113" s="1"/>
+    </row>
+    <row r="114" spans="1:10" ht="120">
       <c r="A114" s="4" t="s">
         <v>313</v>
       </c>
@@ -5974,29 +5997,29 @@
         <v>63</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>520</v>
+        <v>495</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>518</v>
+        <v>492</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>521</v>
+        <v>493</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>519</v>
+        <v>494</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>522</v>
+        <v>491</v>
       </c>
       <c r="I114" s="6"/>
       <c r="J114" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="135" hidden="1">
+    <row r="115" spans="1:10" ht="30">
       <c r="A115" s="4" t="s">
         <v>313</v>
       </c>
@@ -6004,100 +6027,130 @@
         <v>63</v>
       </c>
       <c r="C115" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="I115" s="6"/>
+      <c r="J115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="135">
+      <c r="A116" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C116" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="D115" s="1" t="str">
-        <f>CONCATENATE("&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='",D110,"' title='",D109,"' target='_blank'&gt;",D109,"&lt;/a&gt;")</f>
+      <c r="D116" s="1" t="str">
+        <f>CONCATENATE("&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='",D111,"' title='",D110,"' target='_blank'&gt;",D110,"&lt;/a&gt;")</f>
         <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
-      <c r="E115" s="1" t="str">
-        <f t="shared" ref="E115:H115" si="0">CONCATENATE("&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='",E110,"' title='",E109,"' target='_blank'&gt;",E109,"&lt;/a&gt;")</f>
+      <c r="E116" s="1" t="str">
+        <f t="shared" ref="E116:H116" si="0">CONCATENATE("&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='",E111,"' title='",E110,"' target='_blank'&gt;",E110,"&lt;/a&gt;")</f>
         <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
-      <c r="F115" s="1" t="str">
+      <c r="F116" s="1" t="str">
         <f t="shared" si="0"/>
         <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
-      <c r="G115" s="1" t="str">
+      <c r="G116" s="1" t="str">
         <f t="shared" si="0"/>
         <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
-      <c r="H115" s="1" t="str">
+      <c r="H116" s="1" t="str">
         <f t="shared" si="0"/>
         <v>&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
-      <c r="I115" s="6">
+      <c r="I116" s="6">
         <v>1</v>
       </c>
-      <c r="J115" s="1">
+      <c r="J116" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="270">
-      <c r="A116" s="4" t="s">
+    <row r="117" spans="1:10" ht="270">
+      <c r="A117" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C117" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="D116" s="1" t="str">
-        <f>CONCATENATE(D113,D115)</f>
+      <c r="D117" s="1" t="str">
+        <f>CONCATENATE(D114,D116)</f>
         <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</v>
       </c>
-      <c r="E116" s="1" t="str">
-        <f t="shared" ref="E116:H116" si="1">CONCATENATE(E113,E115,E114)</f>
+      <c r="E117" s="1" t="str">
+        <f t="shared" ref="E117:H117" si="1">CONCATENATE(E114,E116,E115)</f>
         <v>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</v>
       </c>
-      <c r="F116" s="1" t="str">
+      <c r="F117" s="1" t="str">
         <f t="shared" si="1"/>
         <v>En plus de cette visualisation de la surveillance la société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</v>
       </c>
-      <c r="G116" s="1" t="str">
+      <c r="G117" s="1" t="str">
         <f t="shared" si="1"/>
         <v>In aggiunta a questa visualizzazione della sorveglianza. La società digitale pubblica una relazione annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Le Swiss Lawful Interception Report può essere scaricato qui.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</v>
       </c>
-      <c r="H116" s="1" t="str">
+      <c r="H117" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Swiss Lawful Interception Report kann hier heruntergeladen werden.&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2014/03/SLIR_2014.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;Nur in Deutsch verfügbar</v>
       </c>
-      <c r="I116" s="6">
+      <c r="I117" s="6">
         <v>1</v>
       </c>
-      <c r="J116" s="1"/>
-    </row>
-    <row r="117" spans="1:10" ht="300">
-      <c r="A117" s="4" t="s">
+      <c r="J117" s="1"/>
+    </row>
+    <row r="118" spans="1:10" ht="300">
+      <c r="A118" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C118" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="E117" s="1" t="s">
+      <c r="D118" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="F118" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="G118" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="H117" s="1" t="s">
+      <c r="H118" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="I117" s="6"/>
-      <c r="J117" s="1"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I110:I1048576 I1:I108">
+  <conditionalFormatting sqref="I111:I1048576 I1:I109">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",I1)))</formula>
     </cfRule>
@@ -6119,8 +6172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H106"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
nicht alle Spalten im CSV. sorry my bad!
</commit_message>
<xml_diff>
--- a/_specs/slirv_translations.xlsx
+++ b/_specs/slirv_translations.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="800" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7400" yWindow="800" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="trans" sheetId="3" r:id="rId1"/>
-    <sheet name="Blatt1" sheetId="7" r:id="rId2"/>
+    <sheet name="Blatt1" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="slirv_translations" localSheetId="0">trans!$A$2:$H$117</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="566">
   <si>
     <t>typ</t>
   </si>
@@ -1575,10 +1575,6 @@
     <t>Die Digitale Gesellschaft ist ein offener Zusammenschluss netzpolitisch interessierter Kreise. Dem Bündnis angeschlossen sind rund 50 Einzelpersonen und 15 Gruppierungen. Dazu gehören Grundrechtsorganisationen, Parteien, KünstlerInnen-Kollektive, BetreiberInnen von Netzwerkdiensten und weiteren Gruppen, die sich der kritischen, digitalen Zivilgesellschaft verpflichtet fühlen. &lt;br&gt;&lt;br&gt;Weitere Informationen zu netzpolitischen Themen sind im Blog zu finden: &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">midar an modi maletg antir
-</t>
-  </si>
-  <si>
     <t>tradiment da la patria, desarar malsongas humanas, abus d'uffezi,
 servetsch d'infurmaziun scumando</t>
   </si>
@@ -1735,6 +1731,18 @@
   </si>
   <si>
     <t>midar an modi maletg antir</t>
+  </si>
+  <si>
+    <t>tradiment da la patria, desarar malsongas humanas, abus d'uffezi,</t>
+  </si>
+  <si>
+    <t>servetsch d'infurmaziun scumando</t>
+  </si>
+  <si>
+    <t>La Societad Digitala Svizzra publitgescha annual igl “Swiss Lawfull Interception Report” tgi sa tracta sur la survigilaziun digl stadi en Svizzra. La visualisaziun cumplettescha igl report interactiv e mossa detaglià, scu tgi igl Cantuns survigileschan. Chatta or, per tge delicts igls voss dretgs fundamentals reivan restranschia. &lt;br&gt;&lt;br&gt;&lt;small&gt;Las datas ainten quella statistica cuntignan sulettamain mesiras da survigilaziun siva urdan da process penal. Exceptà en missiuns digl IMSI-Catcher, trojan digl stadi ni mesiras da survigilaziun digl servetsch da spiunadi.&lt;/small&gt;</t>
+  </si>
+  <si>
+    <t>La Societad Digitala è ena averta uniun da cres tgi sa interesseschan per la politica da reits per la informatica. Alla coaliziun totgan vetiers radond 50 persungas singulas et 15 gruppaziuns. Vetiers totgan organisaziuns da dretg fundamental, manaders per services da reits, parteidas politicas, collectivs d'artists et otras gruppadas, tgi sa sentan obligà per las criticas dalla societad civila. &lt;br&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Ulteriuras informatziuns sur da temas dalla politica da reits per la informatica chattez en igl blog : &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1831,7 +1839,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="261">
+  <cellStyleXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2022,6 +2030,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2133,7 +2143,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="261">
+  <cellStyles count="263">
     <cellStyle name="Besuchter Link" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
@@ -2272,6 +2282,7 @@
     <cellStyle name="Besuchter Link" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
@@ -2394,6 +2405,7 @@
     <cellStyle name="Link" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -2808,11 +2820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3044,7 +3055,7 @@
         <v>369</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>370</v>
@@ -3106,7 +3117,7 @@
         <v>338</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="1"/>
@@ -3128,7 +3139,7 @@
         <v>306</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>348</v>
@@ -3184,7 +3195,7 @@
         <v>305</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>351</v>
@@ -3386,7 +3397,7 @@
         <v>482</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="1"/>
@@ -3440,7 +3451,7 @@
         <v>395</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>396</v>
@@ -4536,7 +4547,7 @@
         <v>130</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>257</v>
@@ -4592,7 +4603,7 @@
         <v>134</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>258</v>
@@ -4620,7 +4631,7 @@
         <v>135</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>259</v>
@@ -4648,7 +4659,7 @@
         <v>289</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>290</v>
@@ -4704,7 +4715,7 @@
         <v>300</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>301</v>
@@ -4760,7 +4771,7 @@
         <v>166</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>311</v>
@@ -4788,7 +4799,7 @@
         <v>164</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>256</v>
@@ -4816,7 +4827,7 @@
         <v>130</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>257</v>
@@ -4844,7 +4855,7 @@
         <v>162</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>162</v>
@@ -4872,13 +4883,13 @@
         <v>462</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>463</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I70" s="6"/>
       <c r="J70" s="1"/>
@@ -4928,7 +4939,7 @@
         <v>399</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>400</v>
@@ -4956,7 +4967,7 @@
         <v>353</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>269</v>
@@ -5040,7 +5051,7 @@
         <v>356</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>272</v>
@@ -5124,7 +5135,7 @@
         <v>464</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>465</v>
@@ -5152,13 +5163,13 @@
         <v>466</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>467</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I80" s="6"/>
       <c r="J80" s="1"/>
@@ -5180,13 +5191,13 @@
         <v>468</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>469</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I81" s="6"/>
       <c r="J81" s="1"/>
@@ -5208,7 +5219,7 @@
         <v>158</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>266</v>
@@ -5236,7 +5247,7 @@
         <v>156</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>267</v>
@@ -5264,7 +5275,7 @@
         <v>160</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>268</v>
@@ -5320,7 +5331,7 @@
         <v>333</v>
       </c>
       <c r="F86" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>334</v>
@@ -5464,7 +5475,7 @@
         <v>154</v>
       </c>
       <c r="F91" s="12" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>279</v>
@@ -5520,13 +5531,13 @@
         <v>360</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>361</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I93" s="6"/>
       <c r="J93" s="1"/>
@@ -5548,7 +5559,7 @@
         <v>430</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>362</v>
@@ -5609,13 +5620,13 @@
         <v>470</v>
       </c>
       <c r="F96" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>471</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I96" s="6"/>
       <c r="J96" s="1"/>
@@ -5637,7 +5648,7 @@
         <v>453</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>453</v>
@@ -5665,13 +5676,13 @@
         <v>123</v>
       </c>
       <c r="F98" s="12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>252</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I98" s="6"/>
       <c r="J98" s="1">
@@ -5723,7 +5734,7 @@
         <v>124</v>
       </c>
       <c r="F100" s="12" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>253</v>
@@ -5779,7 +5790,7 @@
         <v>472</v>
       </c>
       <c r="F102" s="12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>473</v>
@@ -5807,13 +5818,13 @@
         <v>401</v>
       </c>
       <c r="F103" s="12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>402</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I103" s="6"/>
       <c r="J103" s="1"/>
@@ -5835,7 +5846,7 @@
         <v>403</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>404</v>
@@ -6075,7 +6086,7 @@
         <v>474</v>
       </c>
       <c r="F112" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>475</v>
@@ -6103,7 +6114,7 @@
         <v>434</v>
       </c>
       <c r="F113" s="12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>435</v>
@@ -6232,10 +6243,10 @@
         <v>509</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I117" s="6"/>
       <c r="J117" s="1"/>
@@ -6261,43 +6272,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>169</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>170</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>178</v>
-      </c>
-      <c r="B2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" t="s">
-        <v>173</v>
       </c>
       <c r="D2" t="s">
         <v>173</v>
@@ -6308,16 +6325,22 @@
       <c r="F2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>179</v>
-      </c>
-      <c r="B3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" t="s">
-        <v>174</v>
       </c>
       <c r="D3" t="s">
         <v>174</v>
@@ -6328,16 +6351,22 @@
       <c r="F3" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" t="s">
-        <v>175</v>
       </c>
       <c r="D4" t="s">
         <v>175</v>
@@ -6348,16 +6377,22 @@
       <c r="F4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>180</v>
-      </c>
-      <c r="B5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" t="s">
-        <v>176</v>
       </c>
       <c r="D5" t="s">
         <v>176</v>
@@ -6368,16 +6403,22 @@
       <c r="F5" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
         <v>181</v>
-      </c>
-      <c r="B6" t="s">
-        <v>177</v>
-      </c>
-      <c r="C6" t="s">
-        <v>177</v>
       </c>
       <c r="D6" t="s">
         <v>177</v>
@@ -6388,136 +6429,178 @@
       <c r="F6" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
         <v>73</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>153</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>369</v>
       </c>
-      <c r="D7" t="s">
-        <v>524</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>523</v>
+      </c>
+      <c r="G7" t="s">
         <v>370</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
         <v>110</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>393</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>392</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>391</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>390</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>109</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>476</v>
-      </c>
-      <c r="C9" t="s">
-        <v>338</v>
-      </c>
-      <c r="D9" t="s">
-        <v>338</v>
       </c>
       <c r="E9" t="s">
         <v>338</v>
       </c>
       <c r="F9" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>338</v>
+      </c>
+      <c r="G9" t="s">
+        <v>338</v>
+      </c>
+      <c r="H9" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
         <v>92</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>114</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>306</v>
       </c>
-      <c r="D10" t="s">
-        <v>525</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>524</v>
+      </c>
+      <c r="G10" t="s">
         <v>348</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
         <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" t="s">
-        <v>304</v>
       </c>
       <c r="D11" t="s">
         <v>113</v>
       </c>
       <c r="E11" t="s">
+        <v>304</v>
+      </c>
+      <c r="F11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G11" t="s">
         <v>349</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>112</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>305</v>
       </c>
-      <c r="D12" t="s">
-        <v>526</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>525</v>
+      </c>
+      <c r="G12" t="s">
         <v>351</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
         <v>298</v>
-      </c>
-      <c r="B13" t="s">
-        <v>344</v>
-      </c>
-      <c r="C13" t="s">
-        <v>344</v>
       </c>
       <c r="D13" t="s">
         <v>344</v>
@@ -6528,616 +6611,802 @@
       <c r="F13" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H13" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
         <v>299</v>
-      </c>
-      <c r="B14" t="s">
-        <v>345</v>
-      </c>
-      <c r="C14" t="s">
-        <v>346</v>
       </c>
       <c r="D14" t="s">
         <v>345</v>
       </c>
       <c r="E14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F14" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="s">
+        <v>347</v>
+      </c>
+      <c r="H14" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
         <v>372</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>381</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>382</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>383</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>384</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
         <v>116</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>115</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>307</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>276</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>277</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>106</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>107</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>137</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>248</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>278</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
         <v>386</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>387</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>387</v>
-      </c>
-      <c r="D18" t="s">
-        <v>386</v>
-      </c>
-      <c r="E18" t="s">
-        <v>388</v>
       </c>
       <c r="F18" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="s">
+        <v>388</v>
+      </c>
+      <c r="H18" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
         <v>478</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>479</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>480</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>481</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>482</v>
       </c>
-      <c r="F19" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="H19" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
         <v>394</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>431</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>395</v>
       </c>
-      <c r="D20" t="s">
-        <v>527</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>526</v>
+      </c>
+      <c r="G20" t="s">
         <v>396</v>
       </c>
-      <c r="F20" t="s">
+      <c r="H20" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
         <v>406</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>411</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>411</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>413</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>412</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
         <v>407</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>409</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>414</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
         <v>415</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>416</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
         <v>408</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>410</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>418</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>419</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>420</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>29</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>140</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>232</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>233</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
         <v>293</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>294</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>295</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>296</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>297</v>
       </c>
-      <c r="F25" t="s">
+      <c r="H25" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>33</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>33</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>185</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>196</v>
       </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>31</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>143</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
         <v>182</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
         <v>197</v>
       </c>
-      <c r="F27" t="s">
+      <c r="H27" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
         <v>5</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>32</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>144</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>183</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>198</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>142</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>184</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>199</v>
       </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
         <v>6</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>34</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>141</v>
       </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
         <v>141</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>200</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
         <v>7</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>35</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>145</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>186</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>201</v>
       </c>
-      <c r="F31" t="s">
+      <c r="H31" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
         <v>8</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>36</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>36</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
         <v>187</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>202</v>
       </c>
-      <c r="F32" t="s">
+      <c r="H32" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
         <v>9</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>37</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>146</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" t="s">
         <v>146</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>203</v>
       </c>
-      <c r="F33" t="s">
+      <c r="H33" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s">
         <v>10</v>
-      </c>
-      <c r="B34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" t="s">
-        <v>38</v>
       </c>
       <c r="D34" t="s">
         <v>38</v>
       </c>
       <c r="E34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" t="s">
         <v>204</v>
       </c>
-      <c r="F34" t="s">
+      <c r="H34" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
         <v>11</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>39</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
         <v>147</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35" t="s">
         <v>147</v>
       </c>
-      <c r="E35" t="s">
+      <c r="G35" t="s">
         <v>205</v>
       </c>
-      <c r="F35" t="s">
+      <c r="H35" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
         <v>12</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>40</v>
-      </c>
-      <c r="C36" t="s">
-        <v>148</v>
-      </c>
-      <c r="D36" t="s">
-        <v>148</v>
       </c>
       <c r="E36" t="s">
         <v>148</v>
       </c>
       <c r="F36" t="s">
+        <v>148</v>
+      </c>
+      <c r="G36" t="s">
+        <v>148</v>
+      </c>
+      <c r="H36" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" t="s">
         <v>13</v>
       </c>
-      <c r="B37" t="s">
+      <c r="D37" t="s">
         <v>41</v>
       </c>
-      <c r="C37" t="s">
+      <c r="E37" t="s">
         <v>41</v>
       </c>
-      <c r="D37" t="s">
+      <c r="F37" t="s">
         <v>188</v>
       </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>206</v>
       </c>
-      <c r="F37" t="s">
+      <c r="H37" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
         <v>14</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>42</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>42</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F38" t="s">
         <v>189</v>
       </c>
-      <c r="E38" t="s">
+      <c r="G38" t="s">
         <v>207</v>
       </c>
-      <c r="F38" t="s">
+      <c r="H38" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
         <v>15</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>43</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
         <v>43</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39" t="s">
         <v>190</v>
       </c>
-      <c r="E39" t="s">
+      <c r="G39" t="s">
         <v>208</v>
       </c>
-      <c r="F39" t="s">
+      <c r="H39" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
         <v>16</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" t="s">
         <v>44</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>44</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F40" t="s">
         <v>191</v>
       </c>
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>209</v>
       </c>
-      <c r="F40" t="s">
+      <c r="H40" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
         <v>18</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>45</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" t="s">
         <v>45</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F41" t="s">
         <v>192</v>
       </c>
-      <c r="E41" t="s">
+      <c r="G41" t="s">
         <v>210</v>
       </c>
-      <c r="F41" t="s">
+      <c r="H41" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
         <v>17</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
         <v>46</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E42" t="s">
         <v>46</v>
       </c>
-      <c r="D42" t="s">
+      <c r="F42" t="s">
         <v>193</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42" t="s">
         <v>211</v>
       </c>
-      <c r="F42" t="s">
+      <c r="H42" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
         <v>19</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>47</v>
       </c>
-      <c r="C43" t="s">
+      <c r="E43" t="s">
         <v>47</v>
       </c>
-      <c r="D43" t="s">
+      <c r="F43" t="s">
         <v>194</v>
       </c>
-      <c r="E43" t="s">
+      <c r="G43" t="s">
         <v>212</v>
       </c>
-      <c r="F43" t="s">
+      <c r="H43" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
         <v>20</v>
-      </c>
-      <c r="B44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" t="s">
-        <v>149</v>
       </c>
       <c r="D44" t="s">
         <v>48</v>
@@ -7148,16 +7417,22 @@
       <c r="F44" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44" t="s">
+        <v>149</v>
+      </c>
+      <c r="H44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
         <v>21</v>
-      </c>
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" t="s">
-        <v>49</v>
       </c>
       <c r="D45" t="s">
         <v>49</v>
@@ -7168,316 +7443,412 @@
       <c r="F45" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45" t="s">
+        <v>49</v>
+      </c>
+      <c r="H45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>50</v>
-      </c>
-      <c r="C46" t="s">
-        <v>150</v>
-      </c>
-      <c r="D46" t="s">
-        <v>150</v>
       </c>
       <c r="E46" t="s">
         <v>150</v>
       </c>
       <c r="F46" t="s">
+        <v>150</v>
+      </c>
+      <c r="G46" t="s">
+        <v>150</v>
+      </c>
+      <c r="H46" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
         <v>23</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" t="s">
         <v>51</v>
       </c>
-      <c r="C47" t="s">
+      <c r="E47" t="s">
         <v>151</v>
       </c>
-      <c r="D47" t="s">
+      <c r="F47" t="s">
         <v>151</v>
       </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
         <v>213</v>
       </c>
-      <c r="F47" t="s">
+      <c r="H47" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
         <v>24</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>52</v>
       </c>
-      <c r="C48" t="s">
+      <c r="E48" t="s">
         <v>52</v>
       </c>
-      <c r="D48" t="s">
+      <c r="F48" t="s">
         <v>195</v>
       </c>
-      <c r="E48" t="s">
+      <c r="G48" t="s">
         <v>214</v>
       </c>
-      <c r="F48" t="s">
+      <c r="H48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" t="s">
         <v>25</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D49" t="s">
         <v>30</v>
       </c>
-      <c r="C49" t="s">
+      <c r="E49" t="s">
         <v>152</v>
       </c>
-      <c r="D49" t="s">
+      <c r="F49" t="s">
         <v>152</v>
       </c>
-      <c r="E49" t="s">
+      <c r="G49" t="s">
         <v>215</v>
       </c>
-      <c r="F49" t="s">
+      <c r="H49" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
         <v>82</v>
       </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
         <v>74</v>
       </c>
-      <c r="C50" t="s">
+      <c r="E50" t="s">
         <v>126</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F50" t="s">
         <v>235</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>235</v>
       </c>
-      <c r="F50" t="s">
+      <c r="H50" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
         <v>83</v>
       </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
         <v>75</v>
       </c>
-      <c r="C51" t="s">
+      <c r="E51" t="s">
         <v>127</v>
-      </c>
-      <c r="D51" t="s">
-        <v>236</v>
-      </c>
-      <c r="E51" t="s">
-        <v>261</v>
       </c>
       <c r="F51" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" t="s">
+        <v>261</v>
+      </c>
+      <c r="H51" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
         <v>84</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>80</v>
       </c>
-      <c r="C52" t="s">
+      <c r="E52" t="s">
         <v>128</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F52" t="s">
         <v>237</v>
       </c>
-      <c r="E52" t="s">
+      <c r="G52" t="s">
         <v>262</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" t="s">
         <v>85</v>
       </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>81</v>
       </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
         <v>129</v>
       </c>
-      <c r="D53" t="s">
+      <c r="F53" t="s">
         <v>238</v>
       </c>
-      <c r="E53" t="s">
+      <c r="G53" t="s">
         <v>255</v>
       </c>
-      <c r="F53" t="s">
+      <c r="H53" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" t="s">
         <v>86</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>76</v>
       </c>
-      <c r="C54" t="s">
+      <c r="E54" t="s">
         <v>133</v>
       </c>
-      <c r="D54" t="s">
+      <c r="F54" t="s">
         <v>239</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
         <v>263</v>
       </c>
-      <c r="F54" t="s">
+      <c r="H54" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" t="s">
         <v>87</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
         <v>77</v>
       </c>
-      <c r="C55" t="s">
+      <c r="E55" t="s">
         <v>132</v>
       </c>
-      <c r="D55" t="s">
+      <c r="F55" t="s">
         <v>240</v>
       </c>
-      <c r="E55" t="s">
+      <c r="G55" t="s">
         <v>264</v>
       </c>
-      <c r="F55" t="s">
+      <c r="H55" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" t="s">
         <v>88</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>104</v>
       </c>
-      <c r="C56" t="s">
+      <c r="E56" t="s">
         <v>130</v>
       </c>
-      <c r="D56" t="s">
+      <c r="F56" t="s">
+        <v>527</v>
+      </c>
+      <c r="G56" t="s">
+        <v>257</v>
+      </c>
+      <c r="H56" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" t="s">
+        <v>131</v>
+      </c>
+      <c r="F57" t="s">
+        <v>241</v>
+      </c>
+      <c r="G57" t="s">
+        <v>265</v>
+      </c>
+      <c r="H57" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" t="s">
+        <v>103</v>
+      </c>
+      <c r="E58" t="s">
+        <v>134</v>
+      </c>
+      <c r="F58" t="s">
         <v>528</v>
       </c>
-      <c r="E56" t="s">
-        <v>257</v>
-      </c>
-      <c r="F56" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>89</v>
-      </c>
-      <c r="B57" t="s">
-        <v>78</v>
-      </c>
-      <c r="C57" t="s">
-        <v>131</v>
-      </c>
-      <c r="D57" t="s">
-        <v>241</v>
-      </c>
-      <c r="E57" t="s">
-        <v>265</v>
-      </c>
-      <c r="F57" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
-        <v>90</v>
-      </c>
-      <c r="B58" t="s">
-        <v>103</v>
-      </c>
-      <c r="C58" t="s">
-        <v>134</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="G58" t="s">
+        <v>258</v>
+      </c>
+      <c r="H58" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" t="s">
+        <v>79</v>
+      </c>
+      <c r="E59" t="s">
+        <v>135</v>
+      </c>
+      <c r="F59" t="s">
         <v>529</v>
       </c>
-      <c r="E58" t="s">
-        <v>258</v>
-      </c>
-      <c r="F58" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>91</v>
-      </c>
-      <c r="B59" t="s">
-        <v>79</v>
-      </c>
-      <c r="C59" t="s">
-        <v>135</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="G59" t="s">
+        <v>259</v>
+      </c>
+      <c r="H59" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" t="s">
+        <v>288</v>
+      </c>
+      <c r="E60" t="s">
+        <v>289</v>
+      </c>
+      <c r="F60" t="s">
         <v>530</v>
       </c>
-      <c r="E59" t="s">
-        <v>259</v>
-      </c>
-      <c r="F59" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" t="s">
-        <v>288</v>
-      </c>
-      <c r="C60" t="s">
-        <v>289</v>
-      </c>
-      <c r="D60" t="s">
-        <v>531</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="G60" t="s">
         <v>290</v>
       </c>
-      <c r="F60" t="s">
+      <c r="H60" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" t="s">
         <v>83</v>
-      </c>
-      <c r="B61" t="s">
-        <v>371</v>
-      </c>
-      <c r="C61" t="s">
-        <v>371</v>
       </c>
       <c r="D61" t="s">
         <v>371</v>
@@ -7488,959 +7859,1258 @@
       <c r="F61" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61" t="s">
+        <v>371</v>
+      </c>
+      <c r="H61" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" t="s">
         <v>84</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
         <v>438</v>
       </c>
-      <c r="C62" t="s">
+      <c r="E62" t="s">
         <v>300</v>
       </c>
-      <c r="D62" t="s">
+      <c r="F62" t="s">
+        <v>531</v>
+      </c>
+      <c r="G62" t="s">
+        <v>301</v>
+      </c>
+      <c r="H62" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" t="s">
+        <v>308</v>
+      </c>
+      <c r="E63" t="s">
+        <v>309</v>
+      </c>
+      <c r="F63" t="s">
+        <v>310</v>
+      </c>
+      <c r="G63" t="s">
+        <v>312</v>
+      </c>
+      <c r="H63" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" t="s">
+        <v>165</v>
+      </c>
+      <c r="E64" t="s">
+        <v>166</v>
+      </c>
+      <c r="F64" t="s">
         <v>532</v>
       </c>
-      <c r="E62" t="s">
-        <v>301</v>
-      </c>
-      <c r="F62" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" t="s">
-        <v>308</v>
-      </c>
-      <c r="C63" t="s">
-        <v>309</v>
-      </c>
-      <c r="D63" t="s">
-        <v>310</v>
-      </c>
-      <c r="E63" t="s">
-        <v>312</v>
-      </c>
-      <c r="F63" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>86</v>
-      </c>
-      <c r="B64" t="s">
-        <v>165</v>
-      </c>
-      <c r="C64" t="s">
-        <v>166</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="G64" t="s">
+        <v>311</v>
+      </c>
+      <c r="H64" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65" t="s">
+        <v>163</v>
+      </c>
+      <c r="E65" t="s">
+        <v>164</v>
+      </c>
+      <c r="F65" t="s">
         <v>533</v>
       </c>
-      <c r="E64" t="s">
-        <v>311</v>
-      </c>
-      <c r="F64" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>87</v>
-      </c>
-      <c r="B65" t="s">
-        <v>163</v>
-      </c>
-      <c r="C65" t="s">
-        <v>164</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="G65" t="s">
+        <v>256</v>
+      </c>
+      <c r="H65" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" t="s">
+        <v>88</v>
+      </c>
+      <c r="D66" t="s">
+        <v>439</v>
+      </c>
+      <c r="E66" t="s">
+        <v>130</v>
+      </c>
+      <c r="F66" t="s">
         <v>534</v>
       </c>
-      <c r="E65" t="s">
-        <v>256</v>
-      </c>
-      <c r="F65" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>88</v>
-      </c>
-      <c r="B66" t="s">
-        <v>439</v>
-      </c>
-      <c r="C66" t="s">
-        <v>130</v>
-      </c>
-      <c r="D66" t="s">
-        <v>535</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="G66" t="s">
         <v>257</v>
       </c>
-      <c r="F66" t="s">
+      <c r="H66" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" t="s">
         <v>89</v>
       </c>
-      <c r="B67" t="s">
+      <c r="D67" t="s">
         <v>161</v>
-      </c>
-      <c r="C67" t="s">
-        <v>162</v>
-      </c>
-      <c r="D67" t="s">
-        <v>536</v>
       </c>
       <c r="E67" t="s">
         <v>162</v>
       </c>
       <c r="F67" t="s">
+        <v>535</v>
+      </c>
+      <c r="G67" t="s">
+        <v>162</v>
+      </c>
+      <c r="H67" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:8" ht="120" customHeight="1">
       <c r="A68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" t="s">
         <v>90</v>
       </c>
-      <c r="B68" t="s">
+      <c r="D68" t="s">
         <v>440</v>
       </c>
-      <c r="C68" t="s">
+      <c r="E68" t="s">
         <v>462</v>
       </c>
-      <c r="D68" t="s">
+      <c r="F68" t="s">
+        <v>536</v>
+      </c>
+      <c r="G68" t="s">
+        <v>463</v>
+      </c>
+      <c r="H68" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="H69" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" t="s">
+        <v>91</v>
+      </c>
+      <c r="D70" t="s">
+        <v>319</v>
+      </c>
+      <c r="E70" t="s">
+        <v>320</v>
+      </c>
+      <c r="F70" t="s">
+        <v>321</v>
+      </c>
+      <c r="G70" t="s">
+        <v>322</v>
+      </c>
+      <c r="H70" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" t="s">
+        <v>477</v>
+      </c>
+      <c r="E71" t="s">
+        <v>399</v>
+      </c>
+      <c r="F71" t="s">
         <v>537</v>
       </c>
-      <c r="E68" t="s">
-        <v>463</v>
-      </c>
-      <c r="F68" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
-        <v>91</v>
-      </c>
-      <c r="B69" t="s">
-        <v>319</v>
-      </c>
-      <c r="C69" t="s">
-        <v>320</v>
-      </c>
-      <c r="D69" t="s">
-        <v>321</v>
-      </c>
-      <c r="E69" t="s">
-        <v>322</v>
-      </c>
-      <c r="F69" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
+      <c r="G71" t="s">
+        <v>400</v>
+      </c>
+      <c r="H71" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C72" t="s">
+        <v>101</v>
+      </c>
+      <c r="D72" t="s">
+        <v>100</v>
+      </c>
+      <c r="E72" t="s">
+        <v>353</v>
+      </c>
+      <c r="F72" t="s">
+        <v>538</v>
+      </c>
+      <c r="G72" t="s">
+        <v>269</v>
+      </c>
+      <c r="H72" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73" t="s">
+        <v>95</v>
+      </c>
+      <c r="D73" t="s">
+        <v>94</v>
+      </c>
+      <c r="E73" t="s">
+        <v>354</v>
+      </c>
+      <c r="F73" t="s">
+        <v>242</v>
+      </c>
+      <c r="G73" t="s">
+        <v>270</v>
+      </c>
+      <c r="H73" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74" t="s">
+        <v>98</v>
+      </c>
+      <c r="D74" t="s">
+        <v>97</v>
+      </c>
+      <c r="E74" t="s">
+        <v>355</v>
+      </c>
+      <c r="F74" t="s">
+        <v>243</v>
+      </c>
+      <c r="G74" t="s">
+        <v>271</v>
+      </c>
+      <c r="H74" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" t="s">
+        <v>167</v>
+      </c>
+      <c r="E75" t="s">
+        <v>356</v>
+      </c>
+      <c r="F75" t="s">
+        <v>539</v>
+      </c>
+      <c r="G75" t="s">
+        <v>272</v>
+      </c>
+      <c r="H75" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" t="s">
+        <v>93</v>
+      </c>
+      <c r="D76" t="s">
+        <v>102</v>
+      </c>
+      <c r="E76" t="s">
+        <v>136</v>
+      </c>
+      <c r="F76" t="s">
+        <v>244</v>
+      </c>
+      <c r="G76" t="s">
+        <v>136</v>
+      </c>
+      <c r="H76" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" t="s">
+        <v>105</v>
+      </c>
+      <c r="E77" t="s">
+        <v>357</v>
+      </c>
+      <c r="F77" t="s">
+        <v>245</v>
+      </c>
+      <c r="G77" t="s">
+        <v>273</v>
+      </c>
+      <c r="H77" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>92</v>
+      </c>
+      <c r="B78" t="s">
         <v>61</v>
       </c>
-      <c r="B70" t="s">
-        <v>477</v>
-      </c>
-      <c r="C70" t="s">
-        <v>399</v>
-      </c>
-      <c r="D70" t="s">
-        <v>538</v>
-      </c>
-      <c r="E70" t="s">
-        <v>400</v>
-      </c>
-      <c r="F70" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" t="s">
+      <c r="C78" t="s">
         <v>101</v>
       </c>
-      <c r="B71" t="s">
-        <v>100</v>
-      </c>
-      <c r="C71" t="s">
-        <v>353</v>
-      </c>
-      <c r="D71" t="s">
-        <v>539</v>
-      </c>
-      <c r="E71" t="s">
-        <v>269</v>
-      </c>
-      <c r="F71" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" t="s">
+      <c r="D78" t="s">
+        <v>451</v>
+      </c>
+      <c r="E78" t="s">
+        <v>464</v>
+      </c>
+      <c r="F78" t="s">
+        <v>540</v>
+      </c>
+      <c r="G78" t="s">
+        <v>465</v>
+      </c>
+      <c r="H78" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>92</v>
+      </c>
+      <c r="B79" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79" t="s">
         <v>95</v>
       </c>
-      <c r="B72" t="s">
-        <v>94</v>
-      </c>
-      <c r="C72" t="s">
-        <v>354</v>
-      </c>
-      <c r="D72" t="s">
-        <v>242</v>
-      </c>
-      <c r="E72" t="s">
-        <v>270</v>
-      </c>
-      <c r="F72" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" t="s">
+      <c r="D79" t="s">
+        <v>508</v>
+      </c>
+      <c r="E79" t="s">
+        <v>466</v>
+      </c>
+      <c r="F79" t="s">
+        <v>541</v>
+      </c>
+      <c r="G79" t="s">
+        <v>467</v>
+      </c>
+      <c r="H79" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" t="s">
+        <v>61</v>
+      </c>
+      <c r="C80" t="s">
         <v>98</v>
       </c>
-      <c r="B73" t="s">
-        <v>97</v>
-      </c>
-      <c r="C73" t="s">
-        <v>355</v>
-      </c>
-      <c r="D73" t="s">
-        <v>243</v>
-      </c>
-      <c r="E73" t="s">
-        <v>271</v>
-      </c>
-      <c r="F73" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" t="s">
+      <c r="D80" t="s">
+        <v>443</v>
+      </c>
+      <c r="E80" t="s">
+        <v>468</v>
+      </c>
+      <c r="F80" t="s">
+        <v>542</v>
+      </c>
+      <c r="G80" t="s">
+        <v>469</v>
+      </c>
+      <c r="H80" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" t="s">
+        <v>61</v>
+      </c>
+      <c r="C81" t="s">
         <v>99</v>
       </c>
-      <c r="B74" t="s">
-        <v>167</v>
-      </c>
-      <c r="C74" t="s">
-        <v>356</v>
-      </c>
-      <c r="D74" t="s">
-        <v>540</v>
-      </c>
-      <c r="E74" t="s">
-        <v>272</v>
-      </c>
-      <c r="F74" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" t="s">
+      <c r="D81" t="s">
+        <v>157</v>
+      </c>
+      <c r="E81" t="s">
+        <v>158</v>
+      </c>
+      <c r="F81" t="s">
+        <v>543</v>
+      </c>
+      <c r="G81" t="s">
+        <v>266</v>
+      </c>
+      <c r="H81" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>92</v>
+      </c>
+      <c r="B82" t="s">
+        <v>61</v>
+      </c>
+      <c r="C82" t="s">
         <v>93</v>
       </c>
-      <c r="B75" t="s">
-        <v>102</v>
-      </c>
-      <c r="C75" t="s">
-        <v>136</v>
-      </c>
-      <c r="D75" t="s">
-        <v>244</v>
-      </c>
-      <c r="E75" t="s">
-        <v>136</v>
-      </c>
-      <c r="F75" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" t="s">
+      <c r="D82" t="s">
+        <v>155</v>
+      </c>
+      <c r="E82" t="s">
+        <v>156</v>
+      </c>
+      <c r="F82" t="s">
+        <v>544</v>
+      </c>
+      <c r="G82" t="s">
+        <v>267</v>
+      </c>
+      <c r="H82" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" t="s">
+        <v>61</v>
+      </c>
+      <c r="C83" t="s">
         <v>96</v>
       </c>
-      <c r="B76" t="s">
-        <v>105</v>
-      </c>
-      <c r="C76" t="s">
-        <v>357</v>
-      </c>
-      <c r="D76" t="s">
-        <v>245</v>
-      </c>
-      <c r="E76" t="s">
-        <v>273</v>
-      </c>
-      <c r="F76" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" t="s">
-        <v>101</v>
-      </c>
-      <c r="B77" t="s">
-        <v>451</v>
-      </c>
-      <c r="C77" t="s">
-        <v>464</v>
-      </c>
-      <c r="D77" t="s">
-        <v>541</v>
-      </c>
-      <c r="E77" t="s">
-        <v>465</v>
-      </c>
-      <c r="F77" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" t="s">
-        <v>95</v>
-      </c>
-      <c r="B78" t="s">
-        <v>508</v>
-      </c>
-      <c r="C78" t="s">
-        <v>466</v>
-      </c>
-      <c r="D78" t="s">
-        <v>542</v>
-      </c>
-      <c r="E78" t="s">
-        <v>467</v>
-      </c>
-      <c r="F78" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" t="s">
-        <v>98</v>
-      </c>
-      <c r="B79" t="s">
-        <v>443</v>
-      </c>
-      <c r="C79" t="s">
-        <v>468</v>
-      </c>
-      <c r="D79" t="s">
-        <v>543</v>
-      </c>
-      <c r="E79" t="s">
-        <v>469</v>
-      </c>
-      <c r="F79" t="s">
+      <c r="D83" t="s">
+        <v>159</v>
+      </c>
+      <c r="E83" t="s">
+        <v>160</v>
+      </c>
+      <c r="F83" t="s">
+        <v>545</v>
+      </c>
+      <c r="G83" t="s">
+        <v>268</v>
+      </c>
+      <c r="H83" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" t="s">
+        <v>55</v>
+      </c>
+      <c r="C84" t="s">
+        <v>56</v>
+      </c>
+      <c r="D84" t="s">
+        <v>59</v>
+      </c>
+      <c r="E84" t="s">
+        <v>138</v>
+      </c>
+      <c r="F84" t="s">
+        <v>249</v>
+      </c>
+      <c r="G84" t="s">
+        <v>280</v>
+      </c>
+      <c r="H84" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" t="s">
+        <v>58</v>
+      </c>
+      <c r="D85" t="s">
+        <v>332</v>
+      </c>
+      <c r="E85" t="s">
+        <v>333</v>
+      </c>
+      <c r="F85" t="s">
+        <v>546</v>
+      </c>
+      <c r="G85" t="s">
+        <v>334</v>
+      </c>
+      <c r="H85" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" t="s">
+        <v>62</v>
+      </c>
+      <c r="D86" t="s">
+        <v>63</v>
+      </c>
+      <c r="E86" t="s">
+        <v>139</v>
+      </c>
+      <c r="F86" t="s">
+        <v>250</v>
+      </c>
+      <c r="G86" t="s">
+        <v>281</v>
+      </c>
+      <c r="H86" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" t="s">
+        <v>57</v>
+      </c>
+      <c r="D87" t="s">
+        <v>60</v>
+      </c>
+      <c r="E87" t="s">
+        <v>168</v>
+      </c>
+      <c r="F87" t="s">
+        <v>251</v>
+      </c>
+      <c r="G87" t="s">
+        <v>282</v>
+      </c>
+      <c r="H87" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" t="s">
+        <v>285</v>
+      </c>
+      <c r="D88" t="s">
+        <v>287</v>
+      </c>
+      <c r="E88" t="s">
+        <v>287</v>
+      </c>
+      <c r="F88" t="s">
+        <v>287</v>
+      </c>
+      <c r="G88" t="s">
+        <v>287</v>
+      </c>
+      <c r="H88" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C89" t="s">
+        <v>286</v>
+      </c>
+      <c r="D89" t="s">
+        <v>454</v>
+      </c>
+      <c r="E89" t="s">
+        <v>454</v>
+      </c>
+      <c r="F89" t="s">
+        <v>454</v>
+      </c>
+      <c r="G89" t="s">
+        <v>454</v>
+      </c>
+      <c r="H89" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" t="s">
+        <v>61</v>
+      </c>
+      <c r="C90" t="s">
+        <v>56</v>
+      </c>
+      <c r="D90" t="s">
+        <v>339</v>
+      </c>
+      <c r="E90" t="s">
+        <v>154</v>
+      </c>
+      <c r="F90" t="s">
+        <v>547</v>
+      </c>
+      <c r="G90" t="s">
+        <v>279</v>
+      </c>
+      <c r="H90" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" t="s">
+        <v>61</v>
+      </c>
+      <c r="C91" t="s">
+        <v>58</v>
+      </c>
+      <c r="D91" t="s">
+        <v>340</v>
+      </c>
+      <c r="E91" t="s">
+        <v>341</v>
+      </c>
+      <c r="F91" t="s">
+        <v>342</v>
+      </c>
+      <c r="G91" t="s">
+        <v>343</v>
+      </c>
+      <c r="H91" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" t="s">
+        <v>61</v>
+      </c>
+      <c r="C92" t="s">
+        <v>62</v>
+      </c>
+      <c r="D92" t="s">
+        <v>441</v>
+      </c>
+      <c r="E92" t="s">
+        <v>360</v>
+      </c>
+      <c r="F92" t="s">
+        <v>548</v>
+      </c>
+      <c r="G92" t="s">
+        <v>361</v>
+      </c>
+      <c r="H92" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
+        <v>61</v>
+      </c>
+      <c r="C93" t="s">
+        <v>57</v>
+      </c>
+      <c r="D93" t="s">
+        <v>429</v>
+      </c>
+      <c r="E93" t="s">
+        <v>430</v>
+      </c>
+      <c r="F93" t="s">
+        <v>549</v>
+      </c>
+      <c r="G93" t="s">
+        <v>362</v>
+      </c>
+      <c r="H93" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" t="s">
+        <v>61</v>
+      </c>
+      <c r="C94" t="s">
+        <v>285</v>
+      </c>
+      <c r="D94" t="s">
+        <v>452</v>
+      </c>
+      <c r="E94" t="s">
+        <v>470</v>
+      </c>
+      <c r="F94" t="s">
+        <v>559</v>
+      </c>
+      <c r="G94" t="s">
+        <v>471</v>
+      </c>
+      <c r="H94" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
-      <c r="A80" t="s">
-        <v>99</v>
-      </c>
-      <c r="B80" t="s">
-        <v>157</v>
-      </c>
-      <c r="C80" t="s">
-        <v>158</v>
-      </c>
-      <c r="D80" t="s">
-        <v>544</v>
-      </c>
-      <c r="E80" t="s">
-        <v>266</v>
-      </c>
-      <c r="F80" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" t="s">
-        <v>93</v>
-      </c>
-      <c r="B81" t="s">
-        <v>155</v>
-      </c>
-      <c r="C81" t="s">
-        <v>156</v>
-      </c>
-      <c r="D81" t="s">
-        <v>545</v>
-      </c>
-      <c r="E81" t="s">
-        <v>267</v>
-      </c>
-      <c r="F81" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" t="s">
-        <v>96</v>
-      </c>
-      <c r="B82" t="s">
-        <v>159</v>
-      </c>
-      <c r="C82" t="s">
-        <v>160</v>
-      </c>
-      <c r="D82" t="s">
-        <v>546</v>
-      </c>
-      <c r="E82" t="s">
-        <v>268</v>
-      </c>
-      <c r="F82" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" t="s">
-        <v>56</v>
-      </c>
-      <c r="B83" t="s">
-        <v>59</v>
-      </c>
-      <c r="C83" t="s">
-        <v>138</v>
-      </c>
-      <c r="D83" t="s">
-        <v>249</v>
-      </c>
-      <c r="E83" t="s">
-        <v>280</v>
-      </c>
-      <c r="F83" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" t="s">
-        <v>58</v>
-      </c>
-      <c r="B84" t="s">
-        <v>332</v>
-      </c>
-      <c r="C84" t="s">
-        <v>333</v>
-      </c>
-      <c r="D84" t="s">
-        <v>547</v>
-      </c>
-      <c r="E84" t="s">
-        <v>334</v>
-      </c>
-      <c r="F84" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" t="s">
-        <v>62</v>
-      </c>
-      <c r="B85" t="s">
-        <v>63</v>
-      </c>
-      <c r="C85" t="s">
-        <v>139</v>
-      </c>
-      <c r="D85" t="s">
-        <v>250</v>
-      </c>
-      <c r="E85" t="s">
-        <v>281</v>
-      </c>
-      <c r="F85" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" t="s">
-        <v>57</v>
-      </c>
-      <c r="B86" t="s">
-        <v>60</v>
-      </c>
-      <c r="C86" t="s">
-        <v>168</v>
-      </c>
-      <c r="D86" t="s">
-        <v>251</v>
-      </c>
-      <c r="E86" t="s">
-        <v>282</v>
-      </c>
-      <c r="F86" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" t="s">
-        <v>285</v>
-      </c>
-      <c r="B87" t="s">
-        <v>287</v>
-      </c>
-      <c r="C87" t="s">
-        <v>287</v>
-      </c>
-      <c r="D87" t="s">
-        <v>287</v>
-      </c>
-      <c r="E87" t="s">
-        <v>287</v>
-      </c>
-      <c r="F87" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" t="s">
+    <row r="95" spans="1:8">
+      <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>61</v>
+      </c>
+      <c r="C95" t="s">
         <v>286</v>
       </c>
-      <c r="B88" t="s">
-        <v>454</v>
-      </c>
-      <c r="C88" t="s">
-        <v>454</v>
-      </c>
-      <c r="D88" t="s">
-        <v>454</v>
-      </c>
-      <c r="E88" t="s">
-        <v>454</v>
-      </c>
-      <c r="F88" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" t="s">
-        <v>56</v>
-      </c>
-      <c r="B89" t="s">
-        <v>339</v>
-      </c>
-      <c r="C89" t="s">
-        <v>154</v>
-      </c>
-      <c r="D89" t="s">
-        <v>548</v>
-      </c>
-      <c r="E89" t="s">
-        <v>279</v>
-      </c>
-      <c r="F89" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" t="s">
-        <v>58</v>
-      </c>
-      <c r="B90" t="s">
-        <v>340</v>
-      </c>
-      <c r="C90" t="s">
-        <v>341</v>
-      </c>
-      <c r="D90" t="s">
-        <v>342</v>
-      </c>
-      <c r="E90" t="s">
-        <v>343</v>
-      </c>
-      <c r="F90" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" t="s">
-        <v>62</v>
-      </c>
-      <c r="B91" t="s">
-        <v>441</v>
-      </c>
-      <c r="C91" t="s">
-        <v>360</v>
-      </c>
-      <c r="D91" t="s">
-        <v>549</v>
-      </c>
-      <c r="E91" t="s">
-        <v>361</v>
-      </c>
-      <c r="F91" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" t="s">
-        <v>57</v>
-      </c>
-      <c r="B92" t="s">
-        <v>429</v>
-      </c>
-      <c r="C92" t="s">
-        <v>430</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="D95" t="s">
+        <v>453</v>
+      </c>
+      <c r="E95" t="s">
+        <v>453</v>
+      </c>
+      <c r="F95" t="s">
         <v>550</v>
       </c>
-      <c r="E92" t="s">
-        <v>362</v>
-      </c>
-      <c r="F92" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" t="s">
-        <v>285</v>
-      </c>
-      <c r="B93" t="s">
-        <v>452</v>
-      </c>
-      <c r="C93" t="s">
-        <v>470</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="G95" t="s">
+        <v>453</v>
+      </c>
+      <c r="H95" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>111</v>
+      </c>
+      <c r="B96" t="s">
+        <v>55</v>
+      </c>
+      <c r="C96" t="s">
+        <v>66</v>
+      </c>
+      <c r="D96" t="s">
+        <v>70</v>
+      </c>
+      <c r="E96" t="s">
+        <v>66</v>
+      </c>
+      <c r="F96" t="s">
+        <v>66</v>
+      </c>
+      <c r="G96" t="s">
+        <v>66</v>
+      </c>
+      <c r="H96" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" t="s">
+        <v>111</v>
+      </c>
+      <c r="B97" t="s">
+        <v>55</v>
+      </c>
+      <c r="C97" t="s">
+        <v>119</v>
+      </c>
+      <c r="D97" t="s">
+        <v>120</v>
+      </c>
+      <c r="E97" t="s">
+        <v>124</v>
+      </c>
+      <c r="F97" t="s">
+        <v>552</v>
+      </c>
+      <c r="G97" t="s">
+        <v>253</v>
+      </c>
+      <c r="H97" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" t="s">
+        <v>111</v>
+      </c>
+      <c r="B98" t="s">
+        <v>55</v>
+      </c>
+      <c r="C98" t="s">
+        <v>68</v>
+      </c>
+      <c r="D98" t="s">
+        <v>72</v>
+      </c>
+      <c r="E98" t="s">
+        <v>125</v>
+      </c>
+      <c r="F98" t="s">
+        <v>234</v>
+      </c>
+      <c r="G98" t="s">
+        <v>331</v>
+      </c>
+      <c r="H98" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>111</v>
+      </c>
+      <c r="B99" t="s">
+        <v>61</v>
+      </c>
+      <c r="C99" t="s">
+        <v>117</v>
+      </c>
+      <c r="D99" t="s">
+        <v>445</v>
+      </c>
+      <c r="E99" t="s">
+        <v>472</v>
+      </c>
+      <c r="F99" t="s">
+        <v>553</v>
+      </c>
+      <c r="G99" t="s">
+        <v>473</v>
+      </c>
+      <c r="H99" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100" t="s">
+        <v>61</v>
+      </c>
+      <c r="C100" t="s">
+        <v>118</v>
+      </c>
+      <c r="D100" t="s">
+        <v>460</v>
+      </c>
+      <c r="E100" t="s">
+        <v>401</v>
+      </c>
+      <c r="F100" t="s">
+        <v>554</v>
+      </c>
+      <c r="G100" t="s">
+        <v>402</v>
+      </c>
+      <c r="H100" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>111</v>
+      </c>
+      <c r="B101" t="s">
+        <v>61</v>
+      </c>
+      <c r="C101" t="s">
+        <v>119</v>
+      </c>
+      <c r="D101" t="s">
+        <v>461</v>
+      </c>
+      <c r="E101" t="s">
+        <v>403</v>
+      </c>
+      <c r="F101" t="s">
+        <v>555</v>
+      </c>
+      <c r="G101" t="s">
+        <v>404</v>
+      </c>
+      <c r="H101" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>64</v>
+      </c>
+      <c r="B102" t="s">
+        <v>55</v>
+      </c>
+      <c r="C102" t="s">
+        <v>65</v>
+      </c>
+      <c r="D102" t="s">
+        <v>69</v>
+      </c>
+      <c r="E102" t="s">
+        <v>358</v>
+      </c>
+      <c r="F102" t="s">
+        <v>247</v>
+      </c>
+      <c r="G102" t="s">
+        <v>274</v>
+      </c>
+      <c r="H102" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>64</v>
+      </c>
+      <c r="B103" t="s">
+        <v>55</v>
+      </c>
+      <c r="C103" t="s">
+        <v>66</v>
+      </c>
+      <c r="D103" t="s">
+        <v>70</v>
+      </c>
+      <c r="E103" t="s">
+        <v>66</v>
+      </c>
+      <c r="F103" t="s">
+        <v>66</v>
+      </c>
+      <c r="G103" t="s">
+        <v>66</v>
+      </c>
+      <c r="H103" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>64</v>
+      </c>
+      <c r="B104" t="s">
+        <v>55</v>
+      </c>
+      <c r="C104" t="s">
+        <v>67</v>
+      </c>
+      <c r="D104" t="s">
+        <v>71</v>
+      </c>
+      <c r="E104" t="s">
+        <v>359</v>
+      </c>
+      <c r="F104" t="s">
+        <v>246</v>
+      </c>
+      <c r="G104" t="s">
+        <v>275</v>
+      </c>
+      <c r="H104" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>64</v>
+      </c>
+      <c r="B105" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" t="s">
+        <v>68</v>
+      </c>
+      <c r="D105" t="s">
+        <v>72</v>
+      </c>
+      <c r="E105" t="s">
+        <v>68</v>
+      </c>
+      <c r="F105" t="s">
+        <v>234</v>
+      </c>
+      <c r="G105" t="s">
+        <v>254</v>
+      </c>
+      <c r="H105" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>373</v>
+      </c>
+      <c r="B106" t="s">
+        <v>374</v>
+      </c>
+      <c r="C106" t="s">
+        <v>298</v>
+      </c>
+      <c r="D106" t="s">
+        <v>397</v>
+      </c>
+      <c r="E106" t="s">
+        <v>397</v>
+      </c>
+      <c r="F106" t="s">
+        <v>397</v>
+      </c>
+      <c r="G106" t="s">
+        <v>397</v>
+      </c>
+      <c r="H106" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>291</v>
+      </c>
+      <c r="B107" t="s">
+        <v>61</v>
+      </c>
+      <c r="C107" t="s">
+        <v>372</v>
+      </c>
+      <c r="D107" t="s">
+        <v>446</v>
+      </c>
+      <c r="E107" t="s">
+        <v>448</v>
+      </c>
+      <c r="F107" t="s">
+        <v>447</v>
+      </c>
+      <c r="G107" t="s">
+        <v>449</v>
+      </c>
+      <c r="H107" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>291</v>
+      </c>
+      <c r="B108" t="s">
+        <v>61</v>
+      </c>
+      <c r="C108" t="s">
+        <v>292</v>
+      </c>
+      <c r="D108" t="s">
+        <v>437</v>
+      </c>
+      <c r="E108" t="s">
+        <v>474</v>
+      </c>
+      <c r="F108" t="s">
+        <v>556</v>
+      </c>
+      <c r="G108" t="s">
+        <v>475</v>
+      </c>
+      <c r="H108" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" t="s">
+        <v>291</v>
+      </c>
+      <c r="B109" t="s">
+        <v>61</v>
+      </c>
+      <c r="C109" t="s">
+        <v>298</v>
+      </c>
+      <c r="D109" t="s">
+        <v>512</v>
+      </c>
+      <c r="E109" t="s">
+        <v>513</v>
+      </c>
+      <c r="F109" t="s">
         <v>560</v>
       </c>
-      <c r="E93" t="s">
-        <v>471</v>
-      </c>
-      <c r="F93" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" t="s">
-        <v>286</v>
-      </c>
-      <c r="B94" t="s">
-        <v>453</v>
-      </c>
-      <c r="C94" t="s">
-        <v>453</v>
-      </c>
-      <c r="D94" t="s">
-        <v>551</v>
-      </c>
-      <c r="E94" t="s">
-        <v>453</v>
-      </c>
-      <c r="F94" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" t="s">
-        <v>66</v>
-      </c>
-      <c r="B95" t="s">
-        <v>70</v>
-      </c>
-      <c r="C95" t="s">
-        <v>66</v>
-      </c>
-      <c r="D95" t="s">
-        <v>66</v>
-      </c>
-      <c r="E95" t="s">
-        <v>66</v>
-      </c>
-      <c r="F95" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" t="s">
-        <v>119</v>
-      </c>
-      <c r="B96" t="s">
-        <v>120</v>
-      </c>
-      <c r="C96" t="s">
-        <v>124</v>
-      </c>
-      <c r="D96" t="s">
-        <v>553</v>
-      </c>
-      <c r="E96" t="s">
-        <v>253</v>
-      </c>
-      <c r="F96" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" t="s">
-        <v>68</v>
-      </c>
-      <c r="B97" t="s">
-        <v>72</v>
-      </c>
-      <c r="C97" t="s">
-        <v>125</v>
-      </c>
-      <c r="D97" t="s">
-        <v>234</v>
-      </c>
-      <c r="E97" t="s">
-        <v>331</v>
-      </c>
-      <c r="F97" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" t="s">
-        <v>117</v>
-      </c>
-      <c r="B98" t="s">
-        <v>445</v>
-      </c>
-      <c r="C98" t="s">
-        <v>472</v>
-      </c>
-      <c r="D98" t="s">
-        <v>554</v>
-      </c>
-      <c r="E98" t="s">
-        <v>473</v>
-      </c>
-      <c r="F98" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" t="s">
-        <v>118</v>
-      </c>
-      <c r="B99" t="s">
-        <v>460</v>
-      </c>
-      <c r="C99" t="s">
-        <v>401</v>
-      </c>
-      <c r="D99" t="s">
-        <v>555</v>
-      </c>
-      <c r="E99" t="s">
-        <v>402</v>
-      </c>
-      <c r="F99" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" t="s">
-        <v>119</v>
-      </c>
-      <c r="B100" t="s">
-        <v>461</v>
-      </c>
-      <c r="C100" t="s">
-        <v>403</v>
-      </c>
-      <c r="D100" t="s">
-        <v>556</v>
-      </c>
-      <c r="E100" t="s">
-        <v>404</v>
-      </c>
-      <c r="F100" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" t="s">
-        <v>65</v>
-      </c>
-      <c r="B101" t="s">
-        <v>69</v>
-      </c>
-      <c r="C101" t="s">
-        <v>358</v>
-      </c>
-      <c r="D101" t="s">
-        <v>247</v>
-      </c>
-      <c r="E101" t="s">
-        <v>274</v>
-      </c>
-      <c r="F101" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102" t="s">
-        <v>66</v>
-      </c>
-      <c r="B102" t="s">
-        <v>70</v>
-      </c>
-      <c r="C102" t="s">
-        <v>66</v>
-      </c>
-      <c r="D102" t="s">
-        <v>66</v>
-      </c>
-      <c r="E102" t="s">
-        <v>66</v>
-      </c>
-      <c r="F102" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103" t="s">
-        <v>67</v>
-      </c>
-      <c r="B103" t="s">
-        <v>71</v>
-      </c>
-      <c r="C103" t="s">
-        <v>359</v>
-      </c>
-      <c r="D103" t="s">
-        <v>246</v>
-      </c>
-      <c r="E103" t="s">
-        <v>275</v>
-      </c>
-      <c r="F103" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104" t="s">
-        <v>68</v>
-      </c>
-      <c r="B104" t="s">
-        <v>72</v>
-      </c>
-      <c r="C104" t="s">
-        <v>68</v>
-      </c>
-      <c r="D104" t="s">
-        <v>234</v>
-      </c>
-      <c r="E104" t="s">
-        <v>254</v>
-      </c>
-      <c r="F104" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105" t="s">
-        <v>298</v>
-      </c>
-      <c r="B105" t="s">
-        <v>397</v>
-      </c>
-      <c r="C105" t="s">
-        <v>397</v>
-      </c>
-      <c r="D105" t="s">
-        <v>397</v>
-      </c>
-      <c r="E105" t="s">
-        <v>397</v>
-      </c>
-      <c r="F105" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="A106" t="s">
-        <v>372</v>
-      </c>
-      <c r="B106" t="s">
-        <v>446</v>
-      </c>
-      <c r="C106" t="s">
-        <v>448</v>
-      </c>
-      <c r="D106" t="s">
-        <v>447</v>
-      </c>
-      <c r="E106" t="s">
-        <v>449</v>
-      </c>
-      <c r="F106" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" t="s">
-        <v>292</v>
-      </c>
-      <c r="B107" t="s">
-        <v>437</v>
-      </c>
-      <c r="C107" t="s">
-        <v>474</v>
-      </c>
-      <c r="D107" t="s">
-        <v>557</v>
-      </c>
-      <c r="E107" t="s">
-        <v>475</v>
-      </c>
-      <c r="F107" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108" t="s">
-        <v>298</v>
-      </c>
-      <c r="B108" t="s">
-        <v>513</v>
-      </c>
-      <c r="C108" t="s">
+      <c r="G109" t="s">
         <v>514</v>
       </c>
-      <c r="D108" t="s">
-        <v>561</v>
-      </c>
-      <c r="E108" t="s">
+      <c r="H109" t="s">
         <v>515</v>
       </c>
-      <c r="F108" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109" t="s">
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" t="s">
+        <v>291</v>
+      </c>
+      <c r="B110" t="s">
+        <v>61</v>
+      </c>
+      <c r="C110" t="s">
         <v>299</v>
       </c>
-      <c r="B109" t="s">
+      <c r="D110" t="s">
         <v>509</v>
       </c>
-      <c r="D109" t="s">
-        <v>559</v>
-      </c>
-      <c r="F109" t="s">
-        <v>523</v>
+      <c r="F110" t="s">
+        <v>558</v>
+      </c>
+      <c r="H110" t="s">
+        <v>565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fehler in Franz HTML “ statt ‘
</commit_message>
<xml_diff>
--- a/_specs/slirv_translations.xlsx
+++ b/_specs/slirv_translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="800" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4760" yWindow="320" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="trans" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="571">
   <si>
     <t>typ</t>
   </si>
@@ -1743,6 +1743,21 @@
   </si>
   <si>
     <t>La Societad Digitala è ena averta uniun da cres tgi sa interesseschan per la politica da reits per la informatica. Alla coaliziun totgan vetiers radond 50 persungas singulas et 15 gruppaziuns. Vetiers totgan organisaziuns da dretg fundamental, manaders per services da reits, parteidas politicas, collectivs d'artists et otras gruppadas, tgi sa sentan obligà per las criticas dalla societad civila. &lt;br&gt;&lt;span class="glyphicon glyphicon glyphicon-menu-right" aria-hidden="true"&gt;&lt;/span&gt;Ulteriuras informatziuns sur da temas dalla politica da reits per la informatica chattez en igl blog : &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/de' target='_blank'&gt;Dienst Überwachung Post- und Fernmeldeverkehr&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Microsoft / Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Basiskarte: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Bundesamt für Landestopografie&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/en' target='_blank'&gt;Post and Telecommunications Surveillance Service&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Microsoft/Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Base map: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Federal Office of Topography swisstopo &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/fr' target='_blank'&gt;Service Surveillance de la correspondance par poste et télécommunication&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Microsoft/Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;plan de base: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Office fédéral de topographie swisstopo&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/it' target='_blank'&gt;Servizio Sorveglianza della corrispondenza postale e del traffico delle telecomunicazioni&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt; Microsoft/Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;carta di base: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Ufficio federale di topografia swisstopo&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;ul&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.li.admin.ch/rm' target='_blank'&gt;Servetsch da surveglianza dal traffic da posta e da telecommunicaziun&lt;/a&gt;&lt;/br&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Facebook: &lt;a href='https://govtrequests.facebook.com/country/Switzerland' target='_blank'&gt;Facebook Government Requests&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Microsoft/Skype: &lt;a href='https://www.microsoft.com/about/corporatecitizenship/en-us/reporting/transparency' target='_blank'&gt;Microsoft Transparency Report&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;Basiskarte: &lt;a href='http://www.swisstopo.ch' target='_blank'&gt;Bundesamt für Landestopografie&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -2820,10 +2835,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection sqref="A1:H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6050,19 +6066,19 @@
         <v>372</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>446</v>
+        <v>566</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>448</v>
+        <v>567</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>447</v>
+        <v>568</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>449</v>
+        <v>569</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>450</v>
+        <v>570</v>
       </c>
       <c r="I111" s="6">
         <v>1</v>
@@ -6274,8 +6290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H110"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Update Excel & csv
</commit_message>
<xml_diff>
--- a/_specs/slirv_translations.xlsx
+++ b/_specs/slirv_translations.xlsx
@@ -14,6 +14,7 @@
     <definedName name="slirv_translations" localSheetId="1">Blatt1!$A$2:$H$119</definedName>
     <definedName name="slirv_translations" localSheetId="0">trans!$A$2:$H$119</definedName>
     <definedName name="slirv_translations_1" localSheetId="1">Blatt1!$A$2:$H$119</definedName>
+    <definedName name="slirv_translations_2" localSheetId="1">Blatt1!$A$2:$H$119</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="575">
   <si>
     <t>typ</t>
   </si>
@@ -1868,7 +1869,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="279">
+  <cellStyleXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2147,6 +2148,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
@@ -2188,7 +2193,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="279">
+  <cellStyles count="283">
     <cellStyle name="Besuchter Link" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
@@ -2338,6 +2343,8 @@
     <cellStyle name="Besuchter Link" xfId="276" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="277" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
@@ -2467,6 +2474,8 @@
     <cellStyle name="Link" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="271" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -2537,10 +2546,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="slirv_translations_2" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="slirv_translations" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="slirv_translations_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -2891,8 +2904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H119"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6399,46 +6412,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G111"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>122</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>169</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>170</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>178</v>
-      </c>
-      <c r="C2" t="s">
-        <v>173</v>
       </c>
       <c r="D2" t="s">
         <v>173</v>
@@ -6452,16 +6468,19 @@
       <c r="G2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>179</v>
-      </c>
-      <c r="C3" t="s">
-        <v>174</v>
       </c>
       <c r="D3" t="s">
         <v>174</v>
@@ -6475,16 +6494,19 @@
       <c r="G3" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>175</v>
       </c>
       <c r="D4" t="s">
         <v>175</v>
@@ -6498,16 +6520,19 @@
       <c r="G4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>180</v>
-      </c>
-      <c r="C5" t="s">
-        <v>176</v>
       </c>
       <c r="D5" t="s">
         <v>176</v>
@@ -6521,16 +6546,19 @@
       <c r="G5" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
         <v>181</v>
-      </c>
-      <c r="C6" t="s">
-        <v>177</v>
       </c>
       <c r="D6" t="s">
         <v>177</v>
@@ -6544,154 +6572,175 @@
       <c r="G6" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>153</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>345</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>471</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>346</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
         <v>110</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>368</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>367</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>366</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>365</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>109</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>431</v>
-      </c>
-      <c r="D9" t="s">
-        <v>318</v>
       </c>
       <c r="E9" t="s">
         <v>318</v>
       </c>
       <c r="F9" t="s">
+        <v>318</v>
+      </c>
+      <c r="G9" t="s">
         <v>529</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
         <v>92</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>114</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>288</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>472</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>326</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>113</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>286</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>113</v>
-      </c>
-      <c r="F11" t="s">
-        <v>327</v>
       </c>
       <c r="G11" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
         <v>0</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>112</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>287</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>473</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>329</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
         <v>280</v>
-      </c>
-      <c r="C13" t="s">
-        <v>323</v>
       </c>
       <c r="D13" t="s">
         <v>323</v>
@@ -6705,516 +6754,585 @@
       <c r="G13" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
         <v>281</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>324</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>325</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>324</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>530</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
         <v>347</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>356</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>357</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>358</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>359</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>55</v>
       </c>
       <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
         <v>116</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>115</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>289</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>262</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>263</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>106</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>107</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>137</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>248</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>531</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>55</v>
       </c>
       <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
         <v>361</v>
-      </c>
-      <c r="C18" t="s">
-        <v>362</v>
       </c>
       <c r="D18" t="s">
         <v>362</v>
       </c>
       <c r="E18" t="s">
+        <v>362</v>
+      </c>
+      <c r="F18" t="s">
         <v>361</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>363</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>55</v>
       </c>
       <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
         <v>433</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>434</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>435</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>436</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>437</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>55</v>
       </c>
       <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
         <v>369</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>402</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>370</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>474</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>532</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
         <v>512</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>513</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>515</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>518</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>512</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>514</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>516</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>517</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
         <v>377</v>
-      </c>
-      <c r="C23" t="s">
-        <v>382</v>
       </c>
       <c r="D23" t="s">
         <v>382</v>
       </c>
       <c r="E23" t="s">
+        <v>382</v>
+      </c>
+      <c r="F23" t="s">
         <v>384</v>
-      </c>
-      <c r="F23" t="s">
-        <v>383</v>
       </c>
       <c r="G23" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
         <v>378</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>380</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>385</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>386</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>387</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
         <v>379</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>381</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>389</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>390</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>391</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
         <v>26</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>29</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>140</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>232</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>233</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
         <v>276</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>277</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>278</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>279</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>533</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
         <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>33</v>
       </c>
       <c r="D28" t="s">
         <v>33</v>
       </c>
       <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
         <v>185</v>
-      </c>
-      <c r="F28" t="s">
-        <v>196</v>
       </c>
       <c r="G28" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>31</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>143</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>182</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>197</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
         <v>5</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>32</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>144</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>183</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>198</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>28</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>142</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>184</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>199</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
         <v>6</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>34</v>
-      </c>
-      <c r="D32" t="s">
-        <v>141</v>
       </c>
       <c r="E32" t="s">
         <v>141</v>
       </c>
       <c r="F32" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" t="s">
         <v>200</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
         <v>7</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>35</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>145</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>186</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>201</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s">
         <v>8</v>
-      </c>
-      <c r="C34" t="s">
-        <v>36</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
       </c>
       <c r="E34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" t="s">
         <v>187</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>202</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
         <v>9</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>37</v>
-      </c>
-      <c r="D35" t="s">
-        <v>146</v>
       </c>
       <c r="E35" t="s">
         <v>146</v>
       </c>
       <c r="F35" t="s">
+        <v>146</v>
+      </c>
+      <c r="G35" t="s">
         <v>203</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
         <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>38</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -7223,47 +7341,53 @@
         <v>38</v>
       </c>
       <c r="F36" t="s">
-        <v>204</v>
+        <v>38</v>
       </c>
       <c r="G36" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" t="s">
         <v>11</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>39</v>
-      </c>
-      <c r="D37" t="s">
-        <v>147</v>
       </c>
       <c r="E37" t="s">
         <v>147</v>
       </c>
       <c r="F37" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="G37" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
         <v>12</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>40</v>
-      </c>
-      <c r="D38" t="s">
-        <v>148</v>
       </c>
       <c r="E38" t="s">
         <v>148</v>
@@ -7272,202 +7396,229 @@
         <v>148</v>
       </c>
       <c r="G38" t="s">
+        <v>148</v>
+      </c>
+      <c r="H38" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
         <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>41</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
       </c>
       <c r="E39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" t="s">
         <v>188</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>206</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
         <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>42</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
       </c>
       <c r="E40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" t="s">
         <v>189</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>207</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
         <v>15</v>
-      </c>
-      <c r="C41" t="s">
-        <v>43</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
       </c>
       <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" t="s">
         <v>190</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>208</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
         <v>16</v>
-      </c>
-      <c r="C42" t="s">
-        <v>44</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
       </c>
       <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
         <v>191</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>209</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
         <v>18</v>
-      </c>
-      <c r="C43" t="s">
-        <v>45</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
       </c>
       <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
         <v>192</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>210</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
         <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>46</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
       </c>
       <c r="E44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" t="s">
         <v>193</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>211</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
         <v>19</v>
-      </c>
-      <c r="C45" t="s">
-        <v>47</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
       </c>
       <c r="E45" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" t="s">
         <v>194</v>
-      </c>
-      <c r="F45" t="s">
-        <v>212</v>
       </c>
       <c r="G45" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" t="s">
         <v>20</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>48</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>149</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>48</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>149</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
         <v>21</v>
-      </c>
-      <c r="C47" t="s">
-        <v>49</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -7481,19 +7632,22 @@
       <c r="G47" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
         <v>22</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>50</v>
-      </c>
-      <c r="D48" t="s">
-        <v>150</v>
       </c>
       <c r="E48" t="s">
         <v>150</v>
@@ -7502,938 +7656,1061 @@
         <v>150</v>
       </c>
       <c r="G48" t="s">
+        <v>150</v>
+      </c>
+      <c r="H48" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" t="s">
         <v>23</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>51</v>
-      </c>
-      <c r="D49" t="s">
-        <v>151</v>
       </c>
       <c r="E49" t="s">
         <v>151</v>
       </c>
       <c r="F49" t="s">
+        <v>151</v>
+      </c>
+      <c r="G49" t="s">
         <v>213</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
         <v>24</v>
-      </c>
-      <c r="C50" t="s">
-        <v>52</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
       </c>
       <c r="E50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" t="s">
         <v>195</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>214</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
         <v>25</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>30</v>
-      </c>
-      <c r="D51" t="s">
-        <v>152</v>
       </c>
       <c r="E51" t="s">
         <v>152</v>
       </c>
       <c r="F51" t="s">
+        <v>152</v>
+      </c>
+      <c r="G51" t="s">
         <v>215</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
         <v>82</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>74</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>126</v>
-      </c>
-      <c r="E52" t="s">
-        <v>235</v>
       </c>
       <c r="F52" t="s">
         <v>235</v>
       </c>
       <c r="G52" t="s">
+        <v>235</v>
+      </c>
+      <c r="H52" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" t="s">
         <v>83</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>75</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>127</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>236</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>255</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" t="s">
         <v>84</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>80</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>128</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>237</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>256</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" t="s">
         <v>85</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>81</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>129</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>238</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>534</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" t="s">
         <v>86</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>76</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>133</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>239</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>257</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" t="s">
         <v>87</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>77</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>132</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>240</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>535</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" t="s">
         <v>88</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>104</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>130</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>475</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>536</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" t="s">
         <v>89</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>78</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>131</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>241</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>537</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
         <v>90</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>103</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>134</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>476</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>538</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" t="s">
         <v>91</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>79</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>135</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>477</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>253</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" t="s">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>82</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>272</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>273</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>478</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>539</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63" t="s">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>83</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>75</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>127</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>236</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>255</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" t="s">
         <v>61</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>84</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>407</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>282</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>479</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>283</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" t="s">
         <v>61</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>85</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>290</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>291</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>292</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>293</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" t="s">
         <v>61</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>86</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>165</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>166</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>480</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>540</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" t="s">
         <v>61</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>87</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>163</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>164</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>481</v>
       </c>
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>541</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" t="s">
         <v>61</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>88</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>408</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>130</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>482</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>542</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" t="s">
         <v>61</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>89</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>161</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>162</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>483</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>543</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" t="s">
         <v>61</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>90</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>409</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>424</v>
       </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>484</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>425</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" t="s">
         <v>61</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>91</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>300</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>301</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>302</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>303</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B72" t="s">
         <v>61</v>
       </c>
       <c r="C72" t="s">
+        <v>61</v>
+      </c>
+      <c r="D72" t="s">
         <v>432</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>372</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>485</v>
       </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>373</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73" t="s">
         <v>101</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>100</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>331</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>486</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>544</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74" t="s">
         <v>95</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>94</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>332</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>242</v>
       </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>258</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" t="s">
         <v>98</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>97</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>333</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>243</v>
       </c>
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>545</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" t="s">
         <v>99</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>167</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>334</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
         <v>487</v>
       </c>
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>546</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B77" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" t="s">
         <v>93</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>102</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>136</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>244</v>
       </c>
-      <c r="F77" t="s">
+      <c r="G77" t="s">
         <v>547</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B78" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78" t="s">
         <v>96</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>105</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>335</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>245</v>
       </c>
-      <c r="F78" t="s">
+      <c r="G78" t="s">
         <v>259</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
+        <v>92</v>
+      </c>
+      <c r="B79" t="s">
         <v>61</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>101</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>415</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>426</v>
       </c>
-      <c r="E79" t="s">
+      <c r="F79" t="s">
         <v>488</v>
       </c>
-      <c r="F79" t="s">
+      <c r="G79" t="s">
         <v>548</v>
       </c>
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" t="s">
         <v>61</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>95</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>462</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>427</v>
       </c>
-      <c r="E80" t="s">
+      <c r="F80" t="s">
         <v>489</v>
       </c>
-      <c r="F80" t="s">
+      <c r="G80" t="s">
         <v>549</v>
       </c>
-      <c r="G80" t="s">
+      <c r="H80" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" t="s">
         <v>61</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>98</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>412</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>567</v>
       </c>
-      <c r="E81" t="s">
+      <c r="F81" t="s">
         <v>490</v>
       </c>
-      <c r="F81" t="s">
+      <c r="G81" t="s">
         <v>550</v>
       </c>
-      <c r="G81" t="s">
+      <c r="H81" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
+        <v>92</v>
+      </c>
+      <c r="B82" t="s">
         <v>61</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>99</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>157</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>158</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>491</v>
       </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>551</v>
       </c>
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" t="s">
         <v>61</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>93</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>155</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>156</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>492</v>
       </c>
-      <c r="F83" t="s">
+      <c r="G83" t="s">
         <v>552</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H83" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" t="s">
         <v>61</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>96</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>159</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>160</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
         <v>493</v>
       </c>
-      <c r="F84" t="s">
+      <c r="G84" t="s">
         <v>553</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B85" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" t="s">
         <v>56</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>59</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>138</v>
       </c>
-      <c r="E85" t="s">
+      <c r="F85" t="s">
         <v>249</v>
       </c>
-      <c r="F85" t="s">
+      <c r="G85" t="s">
         <v>264</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" t="s">
         <v>58</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>313</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>314</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F86" t="s">
         <v>494</v>
       </c>
-      <c r="F86" t="s">
+      <c r="G86" t="s">
         <v>554</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B87" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" t="s">
         <v>62</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>63</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>139</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>250</v>
       </c>
-      <c r="F87" t="s">
+      <c r="G87" t="s">
         <v>265</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B88" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" t="s">
         <v>57</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>60</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>168</v>
       </c>
-      <c r="E88" t="s">
+      <c r="F88" t="s">
         <v>251</v>
       </c>
-      <c r="F88" t="s">
+      <c r="G88" t="s">
         <v>266</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C89" t="s">
         <v>269</v>
-      </c>
-      <c r="C89" t="s">
-        <v>271</v>
       </c>
       <c r="D89" t="s">
         <v>271</v>
@@ -8447,16 +8724,19 @@
       <c r="G89" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="H89" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B90" t="s">
+        <v>55</v>
+      </c>
+      <c r="C90" t="s">
         <v>270</v>
-      </c>
-      <c r="C90" t="s">
-        <v>417</v>
       </c>
       <c r="D90" t="s">
         <v>417</v>
@@ -8470,157 +8750,178 @@
       <c r="G90" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="H90" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" t="s">
         <v>61</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>56</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>319</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>154</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F91" t="s">
         <v>495</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>555</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" t="s">
         <v>61</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>58</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>320</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>321</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>322</v>
       </c>
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>556</v>
       </c>
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
         <v>61</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>62</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>410</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>338</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
         <v>496</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>557</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" t="s">
         <v>61</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>57</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>400</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>401</v>
       </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>497</v>
       </c>
-      <c r="F94" t="s">
+      <c r="G94" t="s">
         <v>558</v>
       </c>
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" t="s">
         <v>61</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>269</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>521</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>428</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
         <v>505</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G95" t="s">
         <v>429</v>
       </c>
-      <c r="G95" t="s">
+      <c r="H95" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" t="s">
         <v>61</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>270</v>
-      </c>
-      <c r="C96" t="s">
-        <v>416</v>
       </c>
       <c r="D96" t="s">
         <v>416</v>
       </c>
       <c r="E96" t="s">
+        <v>416</v>
+      </c>
+      <c r="F96" t="s">
         <v>498</v>
       </c>
-      <c r="F96" t="s">
+      <c r="G96" t="s">
         <v>559</v>
       </c>
-      <c r="G96" t="s">
+      <c r="H96" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="B97" t="s">
+        <v>55</v>
+      </c>
+      <c r="C97" t="s">
         <v>66</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>70</v>
-      </c>
-      <c r="D97" t="s">
-        <v>66</v>
       </c>
       <c r="E97" t="s">
         <v>66</v>
@@ -8631,157 +8932,178 @@
       <c r="G97" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="H97" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="B98" t="s">
+        <v>55</v>
+      </c>
+      <c r="C98" t="s">
         <v>119</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>120</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>124</v>
       </c>
-      <c r="E98" t="s">
+      <c r="F98" t="s">
         <v>500</v>
       </c>
-      <c r="F98" t="s">
+      <c r="G98" t="s">
         <v>561</v>
       </c>
-      <c r="G98" t="s">
+      <c r="H98" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="B99" t="s">
+        <v>55</v>
+      </c>
+      <c r="C99" t="s">
         <v>68</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>72</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>125</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
         <v>234</v>
-      </c>
-      <c r="F99" t="s">
-        <v>312</v>
       </c>
       <c r="G99" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="H99" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100" t="s">
         <v>61</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>117</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>414</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>430</v>
       </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
         <v>501</v>
       </c>
-      <c r="F100" t="s">
+      <c r="G100" t="s">
         <v>560</v>
       </c>
-      <c r="G100" t="s">
+      <c r="H100" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
+        <v>111</v>
+      </c>
+      <c r="B101" t="s">
         <v>61</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>118</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>422</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>374</v>
       </c>
-      <c r="E101" t="s">
+      <c r="F101" t="s">
         <v>502</v>
       </c>
-      <c r="F101" t="s">
+      <c r="G101" t="s">
         <v>562</v>
       </c>
-      <c r="G101" t="s">
+      <c r="H101" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
+        <v>111</v>
+      </c>
+      <c r="B102" t="s">
         <v>61</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>119</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>423</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>375</v>
       </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
         <v>503</v>
       </c>
-      <c r="F102" t="s">
+      <c r="G102" t="s">
         <v>563</v>
       </c>
-      <c r="G102" t="s">
+      <c r="H102" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B103" t="s">
+        <v>55</v>
+      </c>
+      <c r="C103" t="s">
         <v>65</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>69</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>336</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>247</v>
       </c>
-      <c r="F103" t="s">
+      <c r="G103" t="s">
         <v>260</v>
       </c>
-      <c r="G103" t="s">
+      <c r="H103" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B104" t="s">
+        <v>55</v>
+      </c>
+      <c r="C104" t="s">
         <v>66</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
         <v>70</v>
-      </c>
-      <c r="D104" t="s">
-        <v>66</v>
       </c>
       <c r="E104" t="s">
         <v>66</v>
@@ -8792,62 +9114,71 @@
       <c r="G104" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="105" spans="1:7">
+      <c r="H104" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B105" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" t="s">
         <v>67</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>71</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>337</v>
       </c>
-      <c r="E105" t="s">
+      <c r="F105" t="s">
         <v>246</v>
       </c>
-      <c r="F105" t="s">
+      <c r="G105" t="s">
         <v>261</v>
       </c>
-      <c r="G105" t="s">
+      <c r="H105" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B106" t="s">
+        <v>55</v>
+      </c>
+      <c r="C106" t="s">
         <v>68</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>72</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E106" t="s">
         <v>68</v>
       </c>
-      <c r="E106" t="s">
+      <c r="F106" t="s">
         <v>234</v>
-      </c>
-      <c r="F106" t="s">
-        <v>312</v>
       </c>
       <c r="G106" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="H106" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
+        <v>348</v>
+      </c>
+      <c r="B107" t="s">
         <v>349</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>280</v>
-      </c>
-      <c r="C107" t="s">
-        <v>568</v>
       </c>
       <c r="D107" t="s">
         <v>568</v>
@@ -8861,96 +9192,111 @@
       <c r="G107" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="108" spans="1:7">
+      <c r="H107" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
+        <v>274</v>
+      </c>
+      <c r="B108" t="s">
         <v>61</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>347</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
         <v>507</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" t="s">
         <v>508</v>
       </c>
-      <c r="E108" t="s">
+      <c r="F108" t="s">
         <v>509</v>
       </c>
-      <c r="F108" t="s">
+      <c r="G108" t="s">
         <v>510</v>
       </c>
-      <c r="G108" t="s">
+      <c r="H108" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
+        <v>274</v>
+      </c>
+      <c r="B109" t="s">
         <v>61</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>275</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>525</v>
       </c>
-      <c r="D109" t="s">
+      <c r="E109" t="s">
         <v>526</v>
       </c>
-      <c r="E109" t="s">
+      <c r="F109" t="s">
         <v>527</v>
       </c>
-      <c r="F109" t="s">
+      <c r="G109" t="s">
         <v>564</v>
       </c>
-      <c r="G109" t="s">
+      <c r="H109" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
+        <v>274</v>
+      </c>
+      <c r="B110" t="s">
         <v>61</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>280</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>570</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E110" t="s">
         <v>571</v>
       </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>572</v>
       </c>
-      <c r="F110" t="s">
+      <c r="G110" t="s">
         <v>573</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
+        <v>274</v>
+      </c>
+      <c r="B111" t="s">
         <v>61</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>281</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>524</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E111" t="s">
         <v>569</v>
       </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
         <v>523</v>
       </c>
-      <c r="F111" t="s">
+      <c r="G111" t="s">
         <v>565</v>
       </c>
-      <c r="G111" t="s">
+      <c r="H111" t="s">
         <v>522</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel, CSV folgt noch.
</commit_message>
<xml_diff>
--- a/_specs/slirv_translations.xlsx
+++ b/_specs/slirv_translations.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24660" yWindow="3500" windowWidth="25220" windowHeight="22500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="34660" yWindow="840" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="trans" sheetId="3" r:id="rId1"/>
-    <sheet name="Blatt1" sheetId="13" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="slirv_translations" localSheetId="0">trans!$A$2:$H$119</definedName>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="571">
   <si>
     <t>typ</t>
   </si>
@@ -1464,9 +1463,6 @@
     <t>localisation d'urgence : activée en cas de recherche de personnes disparues ou en fuite.</t>
   </si>
   <si>
-    <t>En plus de cette visualisation de la surveillance, Société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici.</t>
-  </si>
-  <si>
     <t xml:space="preserve">comptes Facebook : &lt;a href='https://fr-fr.facebook.com/help/405183566203254' target='_blank'&gt;cette liste montre les informations récoltées.&lt;/a&gt; </t>
   </si>
   <si>
@@ -1521,9 +1517,6 @@
     <t>Die Digitale Gesellschaft Schweiz veröffentlicht jährlich den Swiss Lawful Interception Report über die staatliche Überwachung in der Schweiz. Diese Visualiserung ergänzt den Report interaktiv und zeigt detailiert auf, wie in den Kantonen überwacht wird. Finden Sie heraus, für welche Delikte Ihre Grundrechte eingeschränkt werden.&lt;br&gt;&lt;br&gt;Die Daten in dieser Statistik beinhalten nur Überwachungmassnahmen nach Strafprozessordnung. Ausgenommen sind Einsätze von IMSI-Catcher, Staatstrojanern oder Überwachungsmassnahmen des Nachrichtendienstes.</t>
   </si>
   <si>
-    <t>Société numérique Suisse publie annuellement un rapport sur la situation de l'interception légale en Suisse. Cette visualisation interactive complète le rapport et montre en détail la surveillance effectuée dans chaque canton. Découvrez avec quels délits on justifie la limitation de vos libertés fondamentales. &lt;br&gt; &lt;br&gt; Les données de cette statistique ne comprennent que les mesures de surveillance conformes au Code de procédure pénale à l'exclusion des scanners IMSI, des chevaux de Troie gouvernementales ou de la surveillance effectuée par le service de renseignement de la Confédération (SRC).</t>
-  </si>
-  <si>
     <t>La Societad Digitala Svizzra publitgescha annual igl “Swiss Lawfull Interception Report” tgi sa tracta sur la survigilaziun digl stadi en Svizzra. La visualisaziun cumplettescha igl report interactiv e mossa detaglià, scu tgi igl Cantuns survigileschan. Chatta or, per tge delicts igls voss dretgs fundamentals reivan restranschia. &lt;br&gt;&lt;br&gt;&lt;small&gt;Las datas ainten quella statistica cuntignan sulettamain mesiras da survigilaziun siva urdan da process penal. Exceptà en missiuns digl IMSI-Catcher, trojan digl stadi ni mesiras da survigilaziun digl servetsch da spiunadi.</t>
   </si>
   <si>
@@ -1636,9 +1629,6 @@
   </si>
   <si>
     <t>https://www.digitale-gesellschaft.ch/uploads/2015/03/SLIR_2015.pdf</t>
-  </si>
-  <si>
-    <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2015/03/SLIR_2015.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;</t>
   </si>
   <si>
     <t>Visualisation on Lawful Interception in Switzerland</t>
@@ -1752,10 +1742,6 @@
     <t>La Società Digitale è una fusione aperta per tutti interessati in materie di reti. L'alleanza consiste di circa 50 persone e 15 gruppi.  Esse comprendeno organizzazioni di base per i diritti fondamentali, collettivi di artisti, fornitori di servizi internet e altri gruppi che si sentono obbligati alla società civile digitale critica . &lt;br&gt;&lt;br&gt;Piu informazioni su argomenti in materie di reti si possono trovare nel blog: &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">La Societad Digitala è ena averta uniun da cres tgi sa interesseschan per la politica da reits per la informatica. Alla coaliziun totgan vetiers radond 50 persungas singulas et 15 gruppaziuns. Vetiers totgan organisaziuns da dretg fundamental, manaders per services da reits, parteidas politicas, collectivs d'artists et otras gruppadas, tgi sa sentan obligà per las criticas dalla societad civila. &lt;br&gt;&lt;br&gt;Ulteriuras informatziuns sur da temas dalla politica da reits per la informatica chattez en igl blog : &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;
-</t>
-  </si>
-  <si>
     <t>Expensas</t>
   </si>
   <si>
@@ -1810,18 +1796,6 @@
     <t>Neben dieser Visualisierung der Überwachungmassnahmen publiziert die Digitale Gesellschaft jährlich einen detailierten Report, der die Statistiken der Überwachungsmassnahmen noch genauer beleuchtet. Der Report kann hier heruntergeladen werden.</t>
   </si>
   <si>
-    <t>In addition to this visualization of surveillance the Digital Society publishes an annual report, which examines the statistics of surveillance measures in more detail. The Swiss Lawful Interception Report can be downloaded here.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2015/03/SLIR_2015.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;avaliable only in German&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>En plus de cette visualisation de la surveillance, Société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2015/03/SLIR_2015.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>In aggiunta a questa visualizzazione della sorveglianza la Società Digitale pubblica un rapporto annuale, che prende in esame le statistiche di misure di sorveglianza più dettagliato. Il rapporto „Swiss Lawful Interception Report“ può essere scaricato qui.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2015/03/SLIR_2015.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;disponibile solo in tedesco&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>Dasper la visualisaziun dallas mesiras da survigilaziun publitgescha la Societad Digitala en detaglià raport annual, quel che illuminescha las statisticas sur dallas maseiras da survigilaziun anc pli precis. Igl “Swiss Lawful Interception Report” ins sa chargiar giu qua.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2015/03/SLIR_2015.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;Exclusivamain disponibel en tudestg&lt;/strong&gt;</t>
-  </si>
-  <si>
     <t>Strukturierte Gruppe, welche sich mittels Gewaltverbrechen oder sich durch verbrecherische Mittel um Einkünfte bereichert.</t>
   </si>
   <si>
@@ -1835,6 +1809,15 @@
   </si>
   <si>
     <t>Gruppas structuradas, che sa enritgeschan cun crims da violenza ni oter metels criminals .</t>
+  </si>
+  <si>
+    <t>La Societad Digitala è ena averta uniun da cres tgi sa interesseschan per la politica da reits per la informatica. Alla coaliziun totgan vetiers radond 50 persungas singulas et 15 gruppaziuns. Vetiers totgan organisaziuns da dretg fundamental, manaders per services da reits, parteidas politicas, collectivs d'artists et otras gruppadas, tgi sa sentan obligà per las criticas dalla societad civila. &lt;br&gt;&lt;br&gt;Ulteriuras informatziuns sur da temas dalla politica da reits per la informatica chattez en igl blog : &lt;a href='https://www.digitale-gesellschaft.ch'&gt;https://www.digitale-gesellschaft.ch&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Société numérique Suisse publie annuellement un rapport sur la situation de l'interception légale en Suisse. Cette page interactive complète le rapport et montre en détail la surveillance effectuée dans chaque canton. Découvrez avec quels délits on justifie la limitation de vos libertés fondamentales. &lt;br&gt; &lt;br&gt; Les données de cette statistique ne comprennent que les mesures de surveillance conformes au Code de procédure pénale à l'exclusion des scanners IMSI, des chevaux de Troie gouvernementales ou de la surveillance effectuée par le service de renseignement de la Confédération (SRC).</t>
+  </si>
+  <si>
+    <t>En plus de cette visualisation de la surveillance. La Société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici.</t>
   </si>
 </sst>
 </file>
@@ -2878,10 +2861,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H119"/>
+    <sheetView tabSelected="1" topLeftCell="B114" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3138,13 +3122,13 @@
         <v>407</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>308</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>436</v>
@@ -3278,7 +3262,7 @@
         <v>311</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>311</v>
@@ -3356,7 +3340,7 @@
         <v>241</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>275</v>
@@ -3402,7 +3386,7 @@
         <v>410</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>411</v>
@@ -3411,7 +3395,7 @@
         <v>412</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1">
@@ -3463,7 +3447,7 @@
         <v>445</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>415</v>
@@ -3477,22 +3461,22 @@
         <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>482</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>488</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30">
@@ -3503,19 +3487,19 @@
         <v>60</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>486</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H23" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
@@ -3675,7 +3659,7 @@
         <v>269</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>307</v>
@@ -4403,7 +4387,7 @@
         <v>231</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>274</v>
@@ -4455,7 +4439,7 @@
         <v>233</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>418</v>
@@ -4481,7 +4465,7 @@
         <v>446</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>289</v>
@@ -4501,13 +4485,13 @@
         <v>77</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>234</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>357</v>
@@ -4533,7 +4517,7 @@
         <v>447</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>419</v>
@@ -4585,7 +4569,7 @@
         <v>449</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>288</v>
@@ -4688,13 +4672,13 @@
         <v>159</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>451</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>286</v>
@@ -4714,13 +4698,13 @@
         <v>158</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>452</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>421</v>
@@ -4740,13 +4724,13 @@
         <v>391</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>453</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>423</v>
@@ -4772,7 +4756,7 @@
         <v>454</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>422</v>
@@ -4792,7 +4776,7 @@
         <v>392</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>455</v>
@@ -4844,7 +4828,7 @@
         <v>408</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>456</v>
@@ -4876,7 +4860,7 @@
         <v>457</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>285</v>
@@ -4928,7 +4912,7 @@
         <v>236</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>284</v>
@@ -4954,7 +4938,7 @@
         <v>458</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>315</v>
@@ -4980,7 +4964,7 @@
         <v>237</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>297</v>
@@ -5032,7 +5016,7 @@
         <v>459</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>426</v>
@@ -5049,19 +5033,19 @@
         <v>94</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="90">
@@ -5078,13 +5062,13 @@
         <v>394</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>460</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>437</v>
@@ -5110,7 +5094,7 @@
         <v>461</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>427</v>
@@ -5136,7 +5120,7 @@
         <v>462</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>295</v>
@@ -5162,7 +5146,7 @@
         <v>463</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>301</v>
@@ -5179,19 +5163,19 @@
         <v>56</v>
       </c>
       <c r="D87" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="G87" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="F87" s="1" t="s">
+      <c r="H87" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -5214,7 +5198,7 @@
         <v>464</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>305</v>
@@ -5339,19 +5323,19 @@
         <v>56</v>
       </c>
       <c r="D93" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="G93" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="H93" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="30">
@@ -5368,13 +5352,13 @@
         <v>309</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>310</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>430</v>
@@ -5391,16 +5375,16 @@
         <v>61</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>465</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>439</v>
@@ -5417,7 +5401,7 @@
         <v>57</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>384</v>
@@ -5426,7 +5410,7 @@
         <v>466</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>431</v>
@@ -5473,13 +5457,13 @@
         <v>259</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>404</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>405</v>
@@ -5508,7 +5492,7 @@
         <v>467</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>397</v>
@@ -5589,7 +5573,7 @@
         <v>469</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>287</v>
@@ -5609,7 +5593,7 @@
         <v>71</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>227</v>
@@ -5641,7 +5625,7 @@
         <v>470</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>432</v>
@@ -5667,7 +5651,7 @@
         <v>471</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>441</v>
@@ -5693,7 +5677,7 @@
         <v>472</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>433</v>
@@ -5847,7 +5831,7 @@
         <v>270</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E112" s="1" t="str">
         <f>Tabelle2[[#This Row],[de]]</f>
@@ -5877,19 +5861,19 @@
         <v>333</v>
       </c>
       <c r="D113" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="E113" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="F113" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="F113" s="1" t="s">
+      <c r="G113" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="G113" s="1" t="s">
+      <c r="H113" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="270">
@@ -5903,19 +5887,19 @@
         <v>265</v>
       </c>
       <c r="D114" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="H114" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="120" hidden="1">
@@ -5929,16 +5913,16 @@
         <v>389</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>388</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>473</v>
+        <v>570</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>434</v>
@@ -5958,16 +5942,16 @@
         <v>399</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="I116">
         <v>1</v>
@@ -6027,7 +6011,7 @@
       </c>
       <c r="F118" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>En plus de cette visualisation de la surveillance, Société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2015/03/SLIR_2015.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</v>
+        <v>En plus de cette visualisation de la surveillance. La Société numérique publie un rapport annuel, qui examine les statistiques de surveillance plus en détail. Le Swiss Lawful Interception Report peut être téléchargé ici.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2015/03/SLIR_2015.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;disponible uniquement en allemand&lt;/strong&gt;</v>
       </c>
       <c r="G118" s="1" t="str">
         <f t="shared" si="2"/>
@@ -6049,19 +6033,19 @@
         <v>271</v>
       </c>
       <c r="D119" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="G119" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>547</v>
-      </c>
       <c r="H119" s="1" t="s">
-        <v>548</v>
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -6076,2577 +6060,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G111"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G111"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F3" t="s">
-        <v>167</v>
-      </c>
-      <c r="G3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F4" t="s">
-        <v>168</v>
-      </c>
-      <c r="G4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D6" t="s">
-        <v>170</v>
-      </c>
-      <c r="E6" t="s">
-        <v>170</v>
-      </c>
-      <c r="F6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D7" t="s">
-        <v>331</v>
-      </c>
-      <c r="E7" t="s">
-        <v>442</v>
-      </c>
-      <c r="F7" t="s">
-        <v>332</v>
-      </c>
-      <c r="G7" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" t="s">
-        <v>354</v>
-      </c>
-      <c r="D8" t="s">
-        <v>353</v>
-      </c>
-      <c r="E8" t="s">
-        <v>352</v>
-      </c>
-      <c r="F8" t="s">
-        <v>351</v>
-      </c>
-      <c r="G8" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" t="s">
-        <v>407</v>
-      </c>
-      <c r="D9" t="s">
-        <v>532</v>
-      </c>
-      <c r="E9" t="s">
-        <v>308</v>
-      </c>
-      <c r="F9" t="s">
-        <v>494</v>
-      </c>
-      <c r="G9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" t="s">
-        <v>278</v>
-      </c>
-      <c r="E10" t="s">
-        <v>443</v>
-      </c>
-      <c r="F10" t="s">
-        <v>313</v>
-      </c>
-      <c r="G10" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" t="s">
-        <v>276</v>
-      </c>
-      <c r="E11" t="s">
-        <v>112</v>
-      </c>
-      <c r="F11" t="s">
-        <v>314</v>
-      </c>
-      <c r="G11" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" t="s">
-        <v>277</v>
-      </c>
-      <c r="E12" t="s">
-        <v>444</v>
-      </c>
-      <c r="F12" t="s">
-        <v>316</v>
-      </c>
-      <c r="G12" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C13" t="s">
-        <v>393</v>
-      </c>
-      <c r="D13" t="s">
-        <v>393</v>
-      </c>
-      <c r="E13" t="s">
-        <v>393</v>
-      </c>
-      <c r="F13" t="s">
-        <v>393</v>
-      </c>
-      <c r="G13" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" t="s">
-        <v>271</v>
-      </c>
-      <c r="C14" t="s">
-        <v>311</v>
-      </c>
-      <c r="D14" t="s">
-        <v>312</v>
-      </c>
-      <c r="E14" t="s">
-        <v>311</v>
-      </c>
-      <c r="F14" t="s">
-        <v>495</v>
-      </c>
-      <c r="G14" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>333</v>
-      </c>
-      <c r="C15" t="s">
-        <v>342</v>
-      </c>
-      <c r="D15" t="s">
-        <v>343</v>
-      </c>
-      <c r="E15" t="s">
-        <v>344</v>
-      </c>
-      <c r="F15" t="s">
-        <v>345</v>
-      </c>
-      <c r="G15" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" t="s">
-        <v>279</v>
-      </c>
-      <c r="E16" t="s">
-        <v>254</v>
-      </c>
-      <c r="F16" t="s">
-        <v>255</v>
-      </c>
-      <c r="G16" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D17" t="s">
-        <v>134</v>
-      </c>
-      <c r="E17" t="s">
-        <v>241</v>
-      </c>
-      <c r="F17" t="s">
-        <v>496</v>
-      </c>
-      <c r="G17" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" t="s">
-        <v>347</v>
-      </c>
-      <c r="C18" t="s">
-        <v>348</v>
-      </c>
-      <c r="D18" t="s">
-        <v>348</v>
-      </c>
-      <c r="E18" t="s">
-        <v>347</v>
-      </c>
-      <c r="F18" t="s">
-        <v>349</v>
-      </c>
-      <c r="G18" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>409</v>
-      </c>
-      <c r="C19" t="s">
-        <v>410</v>
-      </c>
-      <c r="D19" t="s">
-        <v>533</v>
-      </c>
-      <c r="E19" t="s">
-        <v>411</v>
-      </c>
-      <c r="F19" t="s">
-        <v>412</v>
-      </c>
-      <c r="G19" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>355</v>
-      </c>
-      <c r="C20" t="s">
-        <v>385</v>
-      </c>
-      <c r="D20" t="s">
-        <v>356</v>
-      </c>
-      <c r="E20" t="s">
-        <v>445</v>
-      </c>
-      <c r="F20" t="s">
-        <v>497</v>
-      </c>
-      <c r="G20" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>481</v>
-      </c>
-      <c r="C21" t="s">
-        <v>482</v>
-      </c>
-      <c r="D21" t="s">
-        <v>484</v>
-      </c>
-      <c r="E21" t="s">
-        <v>487</v>
-      </c>
-      <c r="F21" t="s">
-        <v>488</v>
-      </c>
-      <c r="G21" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" t="s">
-        <v>481</v>
-      </c>
-      <c r="C22" t="s">
-        <v>483</v>
-      </c>
-      <c r="D22" t="s">
-        <v>485</v>
-      </c>
-      <c r="E22" t="s">
-        <v>486</v>
-      </c>
-      <c r="F22" t="s">
-        <v>489</v>
-      </c>
-      <c r="G22" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>362</v>
-      </c>
-      <c r="C23" t="s">
-        <v>367</v>
-      </c>
-      <c r="D23" t="s">
-        <v>367</v>
-      </c>
-      <c r="E23" t="s">
-        <v>369</v>
-      </c>
-      <c r="F23" t="s">
-        <v>368</v>
-      </c>
-      <c r="G23" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" t="s">
-        <v>363</v>
-      </c>
-      <c r="C24" t="s">
-        <v>365</v>
-      </c>
-      <c r="D24" t="s">
-        <v>370</v>
-      </c>
-      <c r="E24" t="s">
-        <v>371</v>
-      </c>
-      <c r="F24" t="s">
-        <v>372</v>
-      </c>
-      <c r="G24" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>364</v>
-      </c>
-      <c r="C25" t="s">
-        <v>366</v>
-      </c>
-      <c r="D25" t="s">
-        <v>374</v>
-      </c>
-      <c r="E25" t="s">
-        <v>375</v>
-      </c>
-      <c r="F25" t="s">
-        <v>376</v>
-      </c>
-      <c r="G25" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" t="s">
-        <v>136</v>
-      </c>
-      <c r="E26" t="s">
-        <v>225</v>
-      </c>
-      <c r="F26" t="s">
-        <v>226</v>
-      </c>
-      <c r="G26" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" t="s">
-        <v>266</v>
-      </c>
-      <c r="C27" t="s">
-        <v>267</v>
-      </c>
-      <c r="D27" t="s">
-        <v>268</v>
-      </c>
-      <c r="E27" t="s">
-        <v>269</v>
-      </c>
-      <c r="F27" t="s">
-        <v>498</v>
-      </c>
-      <c r="G27" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" t="s">
-        <v>178</v>
-      </c>
-      <c r="F28" t="s">
-        <v>189</v>
-      </c>
-      <c r="G28" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" t="s">
-        <v>139</v>
-      </c>
-      <c r="E29" t="s">
-        <v>175</v>
-      </c>
-      <c r="F29" t="s">
-        <v>190</v>
-      </c>
-      <c r="G29" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>140</v>
-      </c>
-      <c r="E30" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" t="s">
-        <v>191</v>
-      </c>
-      <c r="G30" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" t="s">
-        <v>138</v>
-      </c>
-      <c r="E31" t="s">
-        <v>177</v>
-      </c>
-      <c r="F31" t="s">
-        <v>192</v>
-      </c>
-      <c r="G31" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" t="s">
-        <v>137</v>
-      </c>
-      <c r="E32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32" t="s">
-        <v>193</v>
-      </c>
-      <c r="G32" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" t="s">
-        <v>141</v>
-      </c>
-      <c r="E33" t="s">
-        <v>179</v>
-      </c>
-      <c r="F33" t="s">
-        <v>194</v>
-      </c>
-      <c r="G33" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" t="s">
-        <v>180</v>
-      </c>
-      <c r="F34" t="s">
-        <v>195</v>
-      </c>
-      <c r="G34" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" t="s">
-        <v>142</v>
-      </c>
-      <c r="E35" t="s">
-        <v>142</v>
-      </c>
-      <c r="F35" t="s">
-        <v>196</v>
-      </c>
-      <c r="G35" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" t="s">
-        <v>197</v>
-      </c>
-      <c r="G36" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" t="s">
-        <v>143</v>
-      </c>
-      <c r="F37" t="s">
-        <v>198</v>
-      </c>
-      <c r="G37" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" t="s">
-        <v>144</v>
-      </c>
-      <c r="F38" t="s">
-        <v>144</v>
-      </c>
-      <c r="G38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F39" t="s">
-        <v>199</v>
-      </c>
-      <c r="G39" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" t="s">
-        <v>182</v>
-      </c>
-      <c r="F40" t="s">
-        <v>200</v>
-      </c>
-      <c r="G40" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" t="s">
-        <v>183</v>
-      </c>
-      <c r="F41" t="s">
-        <v>201</v>
-      </c>
-      <c r="G41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" t="s">
-        <v>184</v>
-      </c>
-      <c r="F42" t="s">
-        <v>202</v>
-      </c>
-      <c r="G42" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" t="s">
-        <v>185</v>
-      </c>
-      <c r="F43" t="s">
-        <v>203</v>
-      </c>
-      <c r="G43" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" t="s">
-        <v>46</v>
-      </c>
-      <c r="E44" t="s">
-        <v>186</v>
-      </c>
-      <c r="F44" t="s">
-        <v>204</v>
-      </c>
-      <c r="G44" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" t="s">
-        <v>47</v>
-      </c>
-      <c r="E45" t="s">
-        <v>187</v>
-      </c>
-      <c r="F45" t="s">
-        <v>205</v>
-      </c>
-      <c r="G45" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" t="s">
-        <v>145</v>
-      </c>
-      <c r="E46" t="s">
-        <v>48</v>
-      </c>
-      <c r="F46" t="s">
-        <v>145</v>
-      </c>
-      <c r="G46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" t="s">
-        <v>49</v>
-      </c>
-      <c r="F47" t="s">
-        <v>49</v>
-      </c>
-      <c r="G47" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" t="s">
-        <v>146</v>
-      </c>
-      <c r="E48" t="s">
-        <v>146</v>
-      </c>
-      <c r="F48" t="s">
-        <v>146</v>
-      </c>
-      <c r="G48" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" t="s">
-        <v>147</v>
-      </c>
-      <c r="E49" t="s">
-        <v>147</v>
-      </c>
-      <c r="F49" t="s">
-        <v>206</v>
-      </c>
-      <c r="G49" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" t="s">
-        <v>52</v>
-      </c>
-      <c r="D50" t="s">
-        <v>52</v>
-      </c>
-      <c r="E50" t="s">
-        <v>188</v>
-      </c>
-      <c r="F50" t="s">
-        <v>207</v>
-      </c>
-      <c r="G50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" t="s">
-        <v>148</v>
-      </c>
-      <c r="E51" t="s">
-        <v>148</v>
-      </c>
-      <c r="F51" t="s">
-        <v>208</v>
-      </c>
-      <c r="G51" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" t="s">
-        <v>73</v>
-      </c>
-      <c r="D52" t="s">
-        <v>124</v>
-      </c>
-      <c r="E52" t="s">
-        <v>228</v>
-      </c>
-      <c r="F52" t="s">
-        <v>228</v>
-      </c>
-      <c r="G52" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" t="s">
-        <v>74</v>
-      </c>
-      <c r="D53" t="s">
-        <v>125</v>
-      </c>
-      <c r="E53" t="s">
-        <v>229</v>
-      </c>
-      <c r="F53" t="s">
-        <v>247</v>
-      </c>
-      <c r="G53" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" t="s">
-        <v>79</v>
-      </c>
-      <c r="D54" t="s">
-        <v>126</v>
-      </c>
-      <c r="E54" t="s">
-        <v>230</v>
-      </c>
-      <c r="F54" t="s">
-        <v>248</v>
-      </c>
-      <c r="G54" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55" t="s">
-        <v>84</v>
-      </c>
-      <c r="C55" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" t="s">
-        <v>127</v>
-      </c>
-      <c r="E55" t="s">
-        <v>231</v>
-      </c>
-      <c r="F55" t="s">
-        <v>499</v>
-      </c>
-      <c r="G55" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>85</v>
-      </c>
-      <c r="C56" t="s">
-        <v>75</v>
-      </c>
-      <c r="D56" t="s">
-        <v>130</v>
-      </c>
-      <c r="E56" t="s">
-        <v>232</v>
-      </c>
-      <c r="F56" t="s">
-        <v>249</v>
-      </c>
-      <c r="G56" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57" t="s">
-        <v>76</v>
-      </c>
-      <c r="D57" t="s">
-        <v>129</v>
-      </c>
-      <c r="E57" t="s">
-        <v>233</v>
-      </c>
-      <c r="F57" t="s">
-        <v>500</v>
-      </c>
-      <c r="G57" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" t="s">
-        <v>87</v>
-      </c>
-      <c r="C58" t="s">
-        <v>103</v>
-      </c>
-      <c r="D58" t="s">
-        <v>128</v>
-      </c>
-      <c r="E58" t="s">
-        <v>446</v>
-      </c>
-      <c r="F58" t="s">
-        <v>501</v>
-      </c>
-      <c r="G58" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" t="s">
-        <v>55</v>
-      </c>
-      <c r="B59" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" t="s">
-        <v>534</v>
-      </c>
-      <c r="E59" t="s">
-        <v>234</v>
-      </c>
-      <c r="F59" t="s">
-        <v>502</v>
-      </c>
-      <c r="G59" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" t="s">
-        <v>55</v>
-      </c>
-      <c r="B60" t="s">
-        <v>89</v>
-      </c>
-      <c r="C60" t="s">
-        <v>102</v>
-      </c>
-      <c r="D60" t="s">
-        <v>131</v>
-      </c>
-      <c r="E60" t="s">
-        <v>447</v>
-      </c>
-      <c r="F60" t="s">
-        <v>503</v>
-      </c>
-      <c r="G60" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" t="s">
-        <v>55</v>
-      </c>
-      <c r="B61" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" t="s">
-        <v>132</v>
-      </c>
-      <c r="E61" t="s">
-        <v>448</v>
-      </c>
-      <c r="F61" t="s">
-        <v>245</v>
-      </c>
-      <c r="G61" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" t="s">
-        <v>81</v>
-      </c>
-      <c r="C62" t="s">
-        <v>262</v>
-      </c>
-      <c r="D62" t="s">
-        <v>263</v>
-      </c>
-      <c r="E62" t="s">
-        <v>449</v>
-      </c>
-      <c r="F62" t="s">
-        <v>504</v>
-      </c>
-      <c r="G62" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" t="s">
-        <v>82</v>
-      </c>
-      <c r="C63" t="s">
-        <v>74</v>
-      </c>
-      <c r="D63" t="s">
-        <v>125</v>
-      </c>
-      <c r="E63" t="s">
-        <v>229</v>
-      </c>
-      <c r="F63" t="s">
-        <v>247</v>
-      </c>
-      <c r="G63" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B64" t="s">
-        <v>83</v>
-      </c>
-      <c r="C64" t="s">
-        <v>390</v>
-      </c>
-      <c r="D64" t="s">
-        <v>272</v>
-      </c>
-      <c r="E64" t="s">
-        <v>450</v>
-      </c>
-      <c r="F64" t="s">
-        <v>273</v>
-      </c>
-      <c r="G64" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" t="s">
-        <v>84</v>
-      </c>
-      <c r="C65" t="s">
-        <v>280</v>
-      </c>
-      <c r="D65" t="s">
-        <v>281</v>
-      </c>
-      <c r="E65" t="s">
-        <v>282</v>
-      </c>
-      <c r="F65" t="s">
-        <v>283</v>
-      </c>
-      <c r="G65" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" t="s">
-        <v>60</v>
-      </c>
-      <c r="B66" t="s">
-        <v>85</v>
-      </c>
-      <c r="C66" t="s">
-        <v>159</v>
-      </c>
-      <c r="D66" t="s">
-        <v>535</v>
-      </c>
-      <c r="E66" t="s">
-        <v>451</v>
-      </c>
-      <c r="F66" t="s">
-        <v>505</v>
-      </c>
-      <c r="G66" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67" t="s">
-        <v>86</v>
-      </c>
-      <c r="C67" t="s">
-        <v>158</v>
-      </c>
-      <c r="D67" t="s">
-        <v>536</v>
-      </c>
-      <c r="E67" t="s">
-        <v>452</v>
-      </c>
-      <c r="F67" t="s">
-        <v>506</v>
-      </c>
-      <c r="G67" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" t="s">
-        <v>60</v>
-      </c>
-      <c r="B68" t="s">
-        <v>87</v>
-      </c>
-      <c r="C68" t="s">
-        <v>391</v>
-      </c>
-      <c r="D68" t="s">
-        <v>537</v>
-      </c>
-      <c r="E68" t="s">
-        <v>453</v>
-      </c>
-      <c r="F68" t="s">
-        <v>507</v>
-      </c>
-      <c r="G68" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" t="s">
-        <v>60</v>
-      </c>
-      <c r="B69" t="s">
-        <v>88</v>
-      </c>
-      <c r="C69" t="s">
-        <v>156</v>
-      </c>
-      <c r="D69" t="s">
-        <v>157</v>
-      </c>
-      <c r="E69" t="s">
-        <v>454</v>
-      </c>
-      <c r="F69" t="s">
-        <v>508</v>
-      </c>
-      <c r="G69" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" t="s">
-        <v>60</v>
-      </c>
-      <c r="B70" t="s">
-        <v>89</v>
-      </c>
-      <c r="C70" t="s">
-        <v>392</v>
-      </c>
-      <c r="D70" t="s">
-        <v>538</v>
-      </c>
-      <c r="E70" t="s">
-        <v>455</v>
-      </c>
-      <c r="F70" t="s">
-        <v>402</v>
-      </c>
-      <c r="G70" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" t="s">
-        <v>60</v>
-      </c>
-      <c r="B71" t="s">
-        <v>90</v>
-      </c>
-      <c r="C71" t="s">
-        <v>290</v>
-      </c>
-      <c r="D71" t="s">
-        <v>291</v>
-      </c>
-      <c r="E71" t="s">
-        <v>292</v>
-      </c>
-      <c r="F71" t="s">
-        <v>293</v>
-      </c>
-      <c r="G71" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" t="s">
-        <v>60</v>
-      </c>
-      <c r="B72" t="s">
-        <v>60</v>
-      </c>
-      <c r="C72" t="s">
-        <v>408</v>
-      </c>
-      <c r="D72" t="s">
-        <v>539</v>
-      </c>
-      <c r="E72" t="s">
-        <v>456</v>
-      </c>
-      <c r="F72" t="s">
-        <v>358</v>
-      </c>
-      <c r="G72" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" t="s">
-        <v>55</v>
-      </c>
-      <c r="B73" t="s">
-        <v>100</v>
-      </c>
-      <c r="C73" t="s">
-        <v>99</v>
-      </c>
-      <c r="D73" t="s">
-        <v>318</v>
-      </c>
-      <c r="E73" t="s">
-        <v>457</v>
-      </c>
-      <c r="F73" t="s">
-        <v>509</v>
-      </c>
-      <c r="G73" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" t="s">
-        <v>55</v>
-      </c>
-      <c r="B74" t="s">
-        <v>94</v>
-      </c>
-      <c r="C74" t="s">
-        <v>93</v>
-      </c>
-      <c r="D74" t="s">
-        <v>319</v>
-      </c>
-      <c r="E74" t="s">
-        <v>235</v>
-      </c>
-      <c r="F74" t="s">
-        <v>250</v>
-      </c>
-      <c r="G74" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" t="s">
-        <v>55</v>
-      </c>
-      <c r="B75" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" t="s">
-        <v>96</v>
-      </c>
-      <c r="D75" t="s">
-        <v>320</v>
-      </c>
-      <c r="E75" t="s">
-        <v>236</v>
-      </c>
-      <c r="F75" t="s">
-        <v>510</v>
-      </c>
-      <c r="G75" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>55</v>
-      </c>
-      <c r="B76" t="s">
-        <v>98</v>
-      </c>
-      <c r="C76" t="s">
-        <v>160</v>
-      </c>
-      <c r="D76" t="s">
-        <v>321</v>
-      </c>
-      <c r="E76" t="s">
-        <v>458</v>
-      </c>
-      <c r="F76" t="s">
-        <v>511</v>
-      </c>
-      <c r="G76" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
-        <v>55</v>
-      </c>
-      <c r="B77" t="s">
-        <v>92</v>
-      </c>
-      <c r="C77" t="s">
-        <v>101</v>
-      </c>
-      <c r="D77" t="s">
-        <v>133</v>
-      </c>
-      <c r="E77" t="s">
-        <v>237</v>
-      </c>
-      <c r="F77" t="s">
-        <v>512</v>
-      </c>
-      <c r="G77" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" t="s">
-        <v>55</v>
-      </c>
-      <c r="B78" t="s">
-        <v>95</v>
-      </c>
-      <c r="C78" t="s">
-        <v>104</v>
-      </c>
-      <c r="D78" t="s">
-        <v>322</v>
-      </c>
-      <c r="E78" t="s">
-        <v>238</v>
-      </c>
-      <c r="F78" t="s">
-        <v>251</v>
-      </c>
-      <c r="G78" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" t="s">
-        <v>60</v>
-      </c>
-      <c r="B79" t="s">
-        <v>100</v>
-      </c>
-      <c r="C79" t="s">
-        <v>396</v>
-      </c>
-      <c r="D79" t="s">
-        <v>403</v>
-      </c>
-      <c r="E79" t="s">
-        <v>459</v>
-      </c>
-      <c r="F79" t="s">
-        <v>513</v>
-      </c>
-      <c r="G79" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" t="s">
-        <v>60</v>
-      </c>
-      <c r="B80" t="s">
-        <v>94</v>
-      </c>
-      <c r="C80" t="s">
-        <v>571</v>
-      </c>
-      <c r="D80" t="s">
-        <v>572</v>
-      </c>
-      <c r="E80" t="s">
-        <v>573</v>
-      </c>
-      <c r="F80" t="s">
-        <v>574</v>
-      </c>
-      <c r="G80" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" t="s">
-        <v>60</v>
-      </c>
-      <c r="B81" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" t="s">
-        <v>394</v>
-      </c>
-      <c r="D81" t="s">
-        <v>529</v>
-      </c>
-      <c r="E81" t="s">
-        <v>460</v>
-      </c>
-      <c r="F81" t="s">
-        <v>514</v>
-      </c>
-      <c r="G81" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" t="s">
-        <v>60</v>
-      </c>
-      <c r="B82" t="s">
-        <v>98</v>
-      </c>
-      <c r="C82" t="s">
-        <v>152</v>
-      </c>
-      <c r="D82" t="s">
-        <v>153</v>
-      </c>
-      <c r="E82" t="s">
-        <v>461</v>
-      </c>
-      <c r="F82" t="s">
-        <v>515</v>
-      </c>
-      <c r="G82" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83" t="s">
-        <v>60</v>
-      </c>
-      <c r="B83" t="s">
-        <v>92</v>
-      </c>
-      <c r="C83" t="s">
-        <v>150</v>
-      </c>
-      <c r="D83" t="s">
-        <v>151</v>
-      </c>
-      <c r="E83" t="s">
-        <v>462</v>
-      </c>
-      <c r="F83" t="s">
-        <v>516</v>
-      </c>
-      <c r="G83" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" t="s">
-        <v>60</v>
-      </c>
-      <c r="B84" t="s">
-        <v>95</v>
-      </c>
-      <c r="C84" t="s">
-        <v>154</v>
-      </c>
-      <c r="D84" t="s">
-        <v>155</v>
-      </c>
-      <c r="E84" t="s">
-        <v>463</v>
-      </c>
-      <c r="F84" t="s">
-        <v>517</v>
-      </c>
-      <c r="G84" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" t="s">
-        <v>55</v>
-      </c>
-      <c r="B85" t="s">
-        <v>56</v>
-      </c>
-      <c r="C85" t="s">
-        <v>551</v>
-      </c>
-      <c r="D85" t="s">
-        <v>553</v>
-      </c>
-      <c r="E85" t="s">
-        <v>555</v>
-      </c>
-      <c r="F85" t="s">
-        <v>557</v>
-      </c>
-      <c r="G85" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" t="s">
-        <v>55</v>
-      </c>
-      <c r="B86" t="s">
-        <v>58</v>
-      </c>
-      <c r="C86" t="s">
-        <v>303</v>
-      </c>
-      <c r="D86" t="s">
-        <v>304</v>
-      </c>
-      <c r="E86" t="s">
-        <v>464</v>
-      </c>
-      <c r="F86" t="s">
-        <v>518</v>
-      </c>
-      <c r="G86" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" t="s">
-        <v>55</v>
-      </c>
-      <c r="B87" t="s">
-        <v>61</v>
-      </c>
-      <c r="C87" t="s">
-        <v>62</v>
-      </c>
-      <c r="D87" t="s">
-        <v>135</v>
-      </c>
-      <c r="E87" t="s">
-        <v>242</v>
-      </c>
-      <c r="F87" t="s">
-        <v>256</v>
-      </c>
-      <c r="G87" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" t="s">
-        <v>55</v>
-      </c>
-      <c r="B88" t="s">
-        <v>57</v>
-      </c>
-      <c r="C88" t="s">
-        <v>59</v>
-      </c>
-      <c r="D88" t="s">
-        <v>161</v>
-      </c>
-      <c r="E88" t="s">
-        <v>243</v>
-      </c>
-      <c r="F88" t="s">
-        <v>257</v>
-      </c>
-      <c r="G88" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" t="s">
-        <v>55</v>
-      </c>
-      <c r="B89" t="s">
-        <v>259</v>
-      </c>
-      <c r="C89" t="s">
-        <v>261</v>
-      </c>
-      <c r="D89" t="s">
-        <v>261</v>
-      </c>
-      <c r="E89" t="s">
-        <v>261</v>
-      </c>
-      <c r="F89" t="s">
-        <v>261</v>
-      </c>
-      <c r="G89" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" t="s">
-        <v>55</v>
-      </c>
-      <c r="B90" t="s">
-        <v>260</v>
-      </c>
-      <c r="C90" t="s">
-        <v>398</v>
-      </c>
-      <c r="D90" t="s">
-        <v>398</v>
-      </c>
-      <c r="E90" t="s">
-        <v>398</v>
-      </c>
-      <c r="F90" t="s">
-        <v>398</v>
-      </c>
-      <c r="G90" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="A91" t="s">
-        <v>60</v>
-      </c>
-      <c r="B91" t="s">
-        <v>56</v>
-      </c>
-      <c r="C91" t="s">
-        <v>550</v>
-      </c>
-      <c r="D91" t="s">
-        <v>552</v>
-      </c>
-      <c r="E91" t="s">
-        <v>554</v>
-      </c>
-      <c r="F91" t="s">
-        <v>556</v>
-      </c>
-      <c r="G91" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" t="s">
-        <v>60</v>
-      </c>
-      <c r="B92" t="s">
-        <v>58</v>
-      </c>
-      <c r="C92" t="s">
-        <v>309</v>
-      </c>
-      <c r="D92" t="s">
-        <v>540</v>
-      </c>
-      <c r="E92" t="s">
-        <v>310</v>
-      </c>
-      <c r="F92" t="s">
-        <v>519</v>
-      </c>
-      <c r="G92" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" t="s">
-        <v>60</v>
-      </c>
-      <c r="B93" t="s">
-        <v>61</v>
-      </c>
-      <c r="C93" t="s">
-        <v>560</v>
-      </c>
-      <c r="D93" t="s">
-        <v>541</v>
-      </c>
-      <c r="E93" t="s">
-        <v>465</v>
-      </c>
-      <c r="F93" t="s">
-        <v>520</v>
-      </c>
-      <c r="G93" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" t="s">
-        <v>60</v>
-      </c>
-      <c r="B94" t="s">
-        <v>57</v>
-      </c>
-      <c r="C94" t="s">
-        <v>561</v>
-      </c>
-      <c r="D94" t="s">
-        <v>384</v>
-      </c>
-      <c r="E94" t="s">
-        <v>466</v>
-      </c>
-      <c r="F94" t="s">
-        <v>521</v>
-      </c>
-      <c r="G94" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="A95" t="s">
-        <v>60</v>
-      </c>
-      <c r="B95" t="s">
-        <v>259</v>
-      </c>
-      <c r="C95" t="s">
-        <v>490</v>
-      </c>
-      <c r="D95" t="s">
-        <v>404</v>
-      </c>
-      <c r="E95" t="s">
-        <v>474</v>
-      </c>
-      <c r="F95" t="s">
-        <v>405</v>
-      </c>
-      <c r="G95" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="A96" t="s">
-        <v>60</v>
-      </c>
-      <c r="B96" t="s">
-        <v>260</v>
-      </c>
-      <c r="C96" t="s">
-        <v>397</v>
-      </c>
-      <c r="D96" t="s">
-        <v>397</v>
-      </c>
-      <c r="E96" t="s">
-        <v>467</v>
-      </c>
-      <c r="F96" t="s">
-        <v>522</v>
-      </c>
-      <c r="G96" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" t="s">
-        <v>55</v>
-      </c>
-      <c r="B97" t="s">
-        <v>65</v>
-      </c>
-      <c r="C97" t="s">
-        <v>69</v>
-      </c>
-      <c r="D97" t="s">
-        <v>65</v>
-      </c>
-      <c r="E97" t="s">
-        <v>65</v>
-      </c>
-      <c r="F97" t="s">
-        <v>65</v>
-      </c>
-      <c r="G97" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
-        <v>55</v>
-      </c>
-      <c r="B98" t="s">
-        <v>118</v>
-      </c>
-      <c r="C98" t="s">
-        <v>119</v>
-      </c>
-      <c r="D98" t="s">
-        <v>123</v>
-      </c>
-      <c r="E98" t="s">
-        <v>469</v>
-      </c>
-      <c r="F98" t="s">
-        <v>524</v>
-      </c>
-      <c r="G98" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
-        <v>55</v>
-      </c>
-      <c r="B99" t="s">
-        <v>67</v>
-      </c>
-      <c r="C99" t="s">
-        <v>71</v>
-      </c>
-      <c r="D99" t="s">
-        <v>542</v>
-      </c>
-      <c r="E99" t="s">
-        <v>227</v>
-      </c>
-      <c r="F99" t="s">
-        <v>302</v>
-      </c>
-      <c r="G99" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" t="s">
-        <v>60</v>
-      </c>
-      <c r="B100" t="s">
-        <v>116</v>
-      </c>
-      <c r="C100" t="s">
-        <v>395</v>
-      </c>
-      <c r="D100" t="s">
-        <v>406</v>
-      </c>
-      <c r="E100" t="s">
-        <v>470</v>
-      </c>
-      <c r="F100" t="s">
-        <v>523</v>
-      </c>
-      <c r="G100" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" t="s">
-        <v>60</v>
-      </c>
-      <c r="B101" t="s">
-        <v>117</v>
-      </c>
-      <c r="C101" t="s">
-        <v>400</v>
-      </c>
-      <c r="D101" t="s">
-        <v>359</v>
-      </c>
-      <c r="E101" t="s">
-        <v>471</v>
-      </c>
-      <c r="F101" t="s">
-        <v>525</v>
-      </c>
-      <c r="G101" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" t="s">
-        <v>60</v>
-      </c>
-      <c r="B102" t="s">
-        <v>118</v>
-      </c>
-      <c r="C102" t="s">
-        <v>401</v>
-      </c>
-      <c r="D102" t="s">
-        <v>360</v>
-      </c>
-      <c r="E102" t="s">
-        <v>472</v>
-      </c>
-      <c r="F102" t="s">
-        <v>526</v>
-      </c>
-      <c r="G102" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103" t="s">
-        <v>55</v>
-      </c>
-      <c r="B103" t="s">
-        <v>64</v>
-      </c>
-      <c r="C103" t="s">
-        <v>68</v>
-      </c>
-      <c r="D103" t="s">
-        <v>323</v>
-      </c>
-      <c r="E103" t="s">
-        <v>240</v>
-      </c>
-      <c r="F103" t="s">
-        <v>252</v>
-      </c>
-      <c r="G103" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" t="s">
-        <v>55</v>
-      </c>
-      <c r="B104" t="s">
-        <v>65</v>
-      </c>
-      <c r="C104" t="s">
-        <v>69</v>
-      </c>
-      <c r="D104" t="s">
-        <v>65</v>
-      </c>
-      <c r="E104" t="s">
-        <v>65</v>
-      </c>
-      <c r="F104" t="s">
-        <v>65</v>
-      </c>
-      <c r="G104" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" t="s">
-        <v>55</v>
-      </c>
-      <c r="B105" t="s">
-        <v>66</v>
-      </c>
-      <c r="C105" t="s">
-        <v>70</v>
-      </c>
-      <c r="D105" t="s">
-        <v>324</v>
-      </c>
-      <c r="E105" t="s">
-        <v>239</v>
-      </c>
-      <c r="F105" t="s">
-        <v>253</v>
-      </c>
-      <c r="G105" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106" t="s">
-        <v>55</v>
-      </c>
-      <c r="B106" t="s">
-        <v>67</v>
-      </c>
-      <c r="C106" t="s">
-        <v>71</v>
-      </c>
-      <c r="D106" t="s">
-        <v>67</v>
-      </c>
-      <c r="E106" t="s">
-        <v>227</v>
-      </c>
-      <c r="F106" t="s">
-        <v>302</v>
-      </c>
-      <c r="G106" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107" t="s">
-        <v>335</v>
-      </c>
-      <c r="B107" t="s">
-        <v>270</v>
-      </c>
-      <c r="C107" t="s">
-        <v>530</v>
-      </c>
-      <c r="D107" t="s">
-        <v>530</v>
-      </c>
-      <c r="E107" t="s">
-        <v>530</v>
-      </c>
-      <c r="F107" t="s">
-        <v>530</v>
-      </c>
-      <c r="G107" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" t="s">
-        <v>60</v>
-      </c>
-      <c r="B108" t="s">
-        <v>333</v>
-      </c>
-      <c r="C108" t="s">
-        <v>476</v>
-      </c>
-      <c r="D108" t="s">
-        <v>477</v>
-      </c>
-      <c r="E108" t="s">
-        <v>478</v>
-      </c>
-      <c r="F108" t="s">
-        <v>479</v>
-      </c>
-      <c r="G108" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
-      <c r="A109" t="s">
-        <v>60</v>
-      </c>
-      <c r="B109" t="s">
-        <v>265</v>
-      </c>
-      <c r="C109" t="s">
-        <v>491</v>
-      </c>
-      <c r="D109" t="s">
-        <v>543</v>
-      </c>
-      <c r="E109" t="s">
-        <v>492</v>
-      </c>
-      <c r="F109" t="s">
-        <v>527</v>
-      </c>
-      <c r="G109" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="A110" t="s">
-        <v>60</v>
-      </c>
-      <c r="B110" t="s">
-        <v>270</v>
-      </c>
-      <c r="C110" t="s">
-        <v>531</v>
-      </c>
-      <c r="D110" t="s">
-        <v>567</v>
-      </c>
-      <c r="E110" t="s">
-        <v>568</v>
-      </c>
-      <c r="F110" t="s">
-        <v>569</v>
-      </c>
-      <c r="G110" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" t="s">
-        <v>60</v>
-      </c>
-      <c r="B111" t="s">
-        <v>271</v>
-      </c>
-      <c r="C111" t="s">
-        <v>544</v>
-      </c>
-      <c r="D111" t="s">
-        <v>545</v>
-      </c>
-      <c r="E111" t="s">
-        <v>546</v>
-      </c>
-      <c r="F111" t="s">
-        <v>547</v>
-      </c>
-      <c r="G111" t="s">
-        <v>548</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update: Translation csv, xls
</commit_message>
<xml_diff>
--- a/_specs/slirv_translations.xlsx
+++ b/_specs/slirv_translations.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="trans" sheetId="3" r:id="rId1"/>
-    <sheet name="Blatt1" sheetId="4" r:id="rId2"/>
+    <sheet name="Blatt1" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="slirv_translations" localSheetId="0">trans!$A$2:$H$119</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="580">
   <si>
     <t>typ</t>
   </si>
@@ -1838,12 +1838,84 @@
   <si>
     <t>Dasper la visualisaziun dallas mesiras da survigilaziun publitgescha la Societad Digitala en detaglià raport annual, quel che illuminescha las statisticas sur dallas maseiras da survigilaziun anc pli precis. Igl “Swiss Lawful Interception Report” ins sa chargiar giu qua.&lt;br&gt;&lt;br&gt;&lt;span class='glyphicon glyphicon glyphicon-menu-right' aria-hidden='true'&gt;&lt;/span&gt;&lt;a href='https://www.digitale-gesellschaft.ch/uploads/2015/03/SLIR_2015.pdf' title='Swiss Lawful Interception Report 2015' target='_blank'&gt;Swiss Lawful Interception Report 2015&lt;/a&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;Exclusivamain disponibel en tudestg&lt;/strong&gt;</t>
   </si>
+  <si>
+    <t>tradiment da la patria, desarar malsongas humanas, abus d'uffezi,</t>
+  </si>
+  <si>
+    <t>servetsch d'infurmaziun scumando</t>
+  </si>
+  <si>
+    <r>
+      <t>The Digital Society Switzerland annually publishes the Swiss Lawful Interception Report on the cantons of Switzerland. This Visualization complements the report interactively and shows in detail</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC5000B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">how many people are affected in the cantons. Find out what crimes are limiting your basic liberties. &lt;br&gt;&lt;br&gt;Data in these statistics only include surveillance measures in accordance with the Criminal Procedure Code. Except </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC5000B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>operations of IMSI catchers, government</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC5000B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-issued </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>trojans or surveillance of intelligence agencies.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1882,6 +1954,29 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC5000B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFC5000B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1900,7 +1995,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="295">
+  <cellStyleXfs count="299">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2187,6 +2282,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2206,7 +2305,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="295">
+  <cellStyles count="299">
     <cellStyle name="Besuchter Link" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
@@ -2366,6 +2465,8 @@
     <cellStyle name="Besuchter Link" xfId="290" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="292" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
@@ -2501,6 +2602,8 @@
     <cellStyle name="Link" xfId="289" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="291" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -2886,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H119"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6085,46 +6188,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G111"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>121</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>162</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>163</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>171</v>
-      </c>
-      <c r="C2" t="s">
-        <v>166</v>
       </c>
       <c r="D2" t="s">
         <v>166</v>
@@ -6138,16 +6244,19 @@
       <c r="G2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>172</v>
-      </c>
-      <c r="C3" t="s">
-        <v>167</v>
       </c>
       <c r="D3" t="s">
         <v>167</v>
@@ -6161,16 +6270,19 @@
       <c r="G3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>168</v>
       </c>
       <c r="D4" t="s">
         <v>168</v>
@@ -6184,16 +6296,19 @@
       <c r="G4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>173</v>
-      </c>
-      <c r="C5" t="s">
-        <v>169</v>
       </c>
       <c r="D5" t="s">
         <v>169</v>
@@ -6207,16 +6322,19 @@
       <c r="G5" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
         <v>174</v>
-      </c>
-      <c r="C6" t="s">
-        <v>170</v>
       </c>
       <c r="D6" t="s">
         <v>170</v>
@@ -6230,154 +6348,175 @@
       <c r="G6" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
         <v>72</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>149</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>331</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>442</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>332</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
         <v>109</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>354</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>353</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>352</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>351</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>108</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>407</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>529</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>308</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>492</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
         <v>91</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>113</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>278</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>443</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>313</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
         <v>63</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>112</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>276</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>112</v>
-      </c>
-      <c r="F11" t="s">
-        <v>314</v>
       </c>
       <c r="G11" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
         <v>0</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>111</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>277</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>444</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>316</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
         <v>270</v>
-      </c>
-      <c r="C13" t="s">
-        <v>393</v>
       </c>
       <c r="D13" t="s">
         <v>393</v>
@@ -6391,522 +6530,591 @@
       <c r="G13" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
         <v>271</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>311</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>312</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>311</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>493</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
         <v>333</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>342</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>343</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>344</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>345</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>55</v>
       </c>
       <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
         <v>115</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>114</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>279</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>254</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>255</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>105</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>106</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>134</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>241</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>494</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>55</v>
       </c>
       <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
         <v>347</v>
-      </c>
-      <c r="C18" t="s">
-        <v>348</v>
       </c>
       <c r="D18" t="s">
         <v>348</v>
       </c>
       <c r="E18" t="s">
+        <v>348</v>
+      </c>
+      <c r="F18" t="s">
         <v>347</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>349</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>55</v>
       </c>
       <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
         <v>409</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>410</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>530</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>411</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>412</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>55</v>
       </c>
       <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
         <v>355</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>385</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>356</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>445</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>495</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
         <v>480</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>481</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>483</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>486</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>487</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>480</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>482</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>484</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>485</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>488</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
         <v>362</v>
-      </c>
-      <c r="C23" t="s">
-        <v>367</v>
       </c>
       <c r="D23" t="s">
         <v>367</v>
       </c>
       <c r="E23" t="s">
+        <v>367</v>
+      </c>
+      <c r="F23" t="s">
         <v>369</v>
-      </c>
-      <c r="F23" t="s">
-        <v>368</v>
       </c>
       <c r="G23" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
         <v>363</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>365</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>370</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>371</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>372</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
         <v>364</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>366</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>374</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>375</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>376</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
         <v>26</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>29</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>136</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>225</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>226</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
         <v>266</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>267</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>268</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>269</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>496</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
         <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>33</v>
       </c>
       <c r="D28" t="s">
         <v>33</v>
       </c>
       <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
         <v>178</v>
-      </c>
-      <c r="F28" t="s">
-        <v>189</v>
       </c>
       <c r="G28" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>31</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>139</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>175</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>190</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
         <v>5</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>32</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>140</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>176</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>191</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>28</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>138</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>177</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>192</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
         <v>6</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>34</v>
-      </c>
-      <c r="D32" t="s">
-        <v>137</v>
       </c>
       <c r="E32" t="s">
         <v>137</v>
       </c>
       <c r="F32" t="s">
+        <v>137</v>
+      </c>
+      <c r="G32" t="s">
         <v>193</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
         <v>7</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>35</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>141</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>179</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>194</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s">
         <v>8</v>
-      </c>
-      <c r="C34" t="s">
-        <v>36</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
       </c>
       <c r="E34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" t="s">
         <v>180</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>195</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
         <v>9</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>37</v>
-      </c>
-      <c r="D35" t="s">
-        <v>142</v>
       </c>
       <c r="E35" t="s">
         <v>142</v>
       </c>
       <c r="F35" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" t="s">
         <v>196</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
         <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>38</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -6915,47 +7123,53 @@
         <v>38</v>
       </c>
       <c r="F36" t="s">
-        <v>197</v>
+        <v>38</v>
       </c>
       <c r="G36" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" t="s">
         <v>11</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>39</v>
-      </c>
-      <c r="D37" t="s">
-        <v>143</v>
       </c>
       <c r="E37" t="s">
         <v>143</v>
       </c>
       <c r="F37" t="s">
-        <v>198</v>
+        <v>143</v>
       </c>
       <c r="G37" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
         <v>12</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>40</v>
-      </c>
-      <c r="D38" t="s">
-        <v>144</v>
       </c>
       <c r="E38" t="s">
         <v>144</v>
@@ -6964,202 +7178,229 @@
         <v>144</v>
       </c>
       <c r="G38" t="s">
+        <v>144</v>
+      </c>
+      <c r="H38" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
         <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>41</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
       </c>
       <c r="E39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" t="s">
         <v>181</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>199</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
         <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>42</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
       </c>
       <c r="E40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" t="s">
         <v>182</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>200</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
         <v>15</v>
-      </c>
-      <c r="C41" t="s">
-        <v>43</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
       </c>
       <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" t="s">
         <v>183</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>201</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
         <v>16</v>
-      </c>
-      <c r="C42" t="s">
-        <v>44</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
       </c>
       <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
         <v>184</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>202</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
         <v>18</v>
-      </c>
-      <c r="C43" t="s">
-        <v>45</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
       </c>
       <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
         <v>185</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>203</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
         <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>46</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
       </c>
       <c r="E44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" t="s">
         <v>186</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>204</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
         <v>19</v>
-      </c>
-      <c r="C45" t="s">
-        <v>47</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
       </c>
       <c r="E45" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" t="s">
         <v>187</v>
-      </c>
-      <c r="F45" t="s">
-        <v>205</v>
       </c>
       <c r="G45" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" t="s">
         <v>20</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>48</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>145</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>48</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>145</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
         <v>21</v>
-      </c>
-      <c r="C47" t="s">
-        <v>49</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -7173,19 +7414,22 @@
       <c r="G47" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
         <v>22</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>50</v>
-      </c>
-      <c r="D48" t="s">
-        <v>146</v>
       </c>
       <c r="E48" t="s">
         <v>146</v>
@@ -7194,1455 +7438,1652 @@
         <v>146</v>
       </c>
       <c r="G48" t="s">
+        <v>146</v>
+      </c>
+      <c r="H48" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" t="s">
         <v>23</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>51</v>
-      </c>
-      <c r="D49" t="s">
-        <v>147</v>
       </c>
       <c r="E49" t="s">
         <v>147</v>
       </c>
       <c r="F49" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" t="s">
         <v>206</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
         <v>24</v>
-      </c>
-      <c r="C50" t="s">
-        <v>52</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
       </c>
       <c r="E50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" t="s">
         <v>188</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>207</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
         <v>25</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>30</v>
-      </c>
-      <c r="D51" t="s">
-        <v>148</v>
       </c>
       <c r="E51" t="s">
         <v>148</v>
       </c>
       <c r="F51" t="s">
+        <v>148</v>
+      </c>
+      <c r="G51" t="s">
         <v>208</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
         <v>81</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>73</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>124</v>
-      </c>
-      <c r="E52" t="s">
-        <v>228</v>
       </c>
       <c r="F52" t="s">
         <v>228</v>
       </c>
       <c r="G52" t="s">
+        <v>228</v>
+      </c>
+      <c r="H52" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" t="s">
         <v>82</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>74</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>125</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>229</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>247</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" t="s">
         <v>83</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>79</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>126</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>230</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>248</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" t="s">
         <v>84</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>80</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>127</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>231</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>497</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" t="s">
         <v>85</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>75</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>130</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>232</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>249</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" t="s">
         <v>86</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>76</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>129</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>233</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>498</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" t="s">
         <v>87</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>103</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>128</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>446</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>499</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" t="s">
         <v>88</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>77</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>531</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>234</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>500</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
         <v>89</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>102</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>131</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>447</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>501</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" t="s">
         <v>90</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>78</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>132</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>448</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>245</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" t="s">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>81</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>262</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>263</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>449</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>502</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" t="s">
         <v>60</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>82</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>74</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>125</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>229</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>247</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64" t="s">
         <v>60</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>83</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>390</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>272</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>450</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>273</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" t="s">
         <v>60</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>84</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>280</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>281</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>282</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>283</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" t="s">
         <v>60</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>85</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>159</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>532</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>451</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>503</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" t="s">
         <v>60</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>86</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>158</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>533</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>452</v>
       </c>
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>504</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" t="s">
         <v>60</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>87</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>391</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>534</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>453</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>505</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" t="s">
         <v>60</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>88</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>156</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>157</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>454</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>506</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:8" ht="120" customHeight="1">
       <c r="A70" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" t="s">
         <v>60</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>89</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>392</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>535</v>
       </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>455</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>402</v>
       </c>
-      <c r="G70" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" t="s">
-        <v>60</v>
-      </c>
-      <c r="B71" t="s">
-        <v>90</v>
-      </c>
-      <c r="C71" t="s">
-        <v>290</v>
-      </c>
-      <c r="D71" t="s">
-        <v>291</v>
-      </c>
-      <c r="E71" t="s">
-        <v>292</v>
-      </c>
-      <c r="F71" t="s">
-        <v>293</v>
-      </c>
-      <c r="G71" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="H70" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="H71" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
         <v>60</v>
       </c>
       <c r="C72" t="s">
+        <v>90</v>
+      </c>
+      <c r="D72" t="s">
+        <v>290</v>
+      </c>
+      <c r="E72" t="s">
+        <v>291</v>
+      </c>
+      <c r="F72" t="s">
+        <v>292</v>
+      </c>
+      <c r="G72" t="s">
+        <v>293</v>
+      </c>
+      <c r="H72" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" t="s">
+        <v>60</v>
+      </c>
+      <c r="C73" t="s">
+        <v>60</v>
+      </c>
+      <c r="D73" t="s">
         <v>408</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E73" t="s">
         <v>536</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F73" t="s">
         <v>456</v>
       </c>
-      <c r="F72" t="s">
+      <c r="G73" t="s">
         <v>358</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H73" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
-      <c r="A73" t="s">
-        <v>55</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74" t="s">
         <v>100</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D74" t="s">
         <v>99</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E74" t="s">
         <v>318</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F74" t="s">
         <v>457</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G74" t="s">
         <v>507</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H74" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
-      <c r="A74" t="s">
-        <v>55</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" t="s">
         <v>94</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D75" t="s">
         <v>93</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E75" t="s">
         <v>319</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F75" t="s">
         <v>235</v>
       </c>
-      <c r="F74" t="s">
+      <c r="G75" t="s">
         <v>250</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H75" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
-      <c r="A75" t="s">
-        <v>55</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" t="s">
         <v>97</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D76" t="s">
         <v>96</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E76" t="s">
         <v>320</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F76" t="s">
         <v>236</v>
       </c>
-      <c r="F75" t="s">
+      <c r="G76" t="s">
         <v>508</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H76" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>55</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" t="s">
         <v>98</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D77" t="s">
         <v>160</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E77" t="s">
         <v>321</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F77" t="s">
         <v>458</v>
       </c>
-      <c r="F76" t="s">
+      <c r="G77" t="s">
         <v>509</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H77" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
-        <v>55</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78" t="s">
         <v>92</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D78" t="s">
         <v>101</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E78" t="s">
         <v>133</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F78" t="s">
         <v>237</v>
       </c>
-      <c r="F77" t="s">
+      <c r="G78" t="s">
         <v>510</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H78" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
-      <c r="A78" t="s">
-        <v>55</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79" t="s">
         <v>95</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D79" t="s">
         <v>104</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E79" t="s">
         <v>322</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F79" t="s">
         <v>238</v>
       </c>
-      <c r="F78" t="s">
+      <c r="G79" t="s">
         <v>251</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H79" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
-      <c r="A79" t="s">
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" t="s">
         <v>60</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C80" t="s">
         <v>100</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D80" t="s">
         <v>396</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E80" t="s">
         <v>403</v>
       </c>
-      <c r="E79" t="s">
+      <c r="F80" t="s">
         <v>459</v>
       </c>
-      <c r="F79" t="s">
+      <c r="G80" t="s">
         <v>511</v>
       </c>
-      <c r="G79" t="s">
+      <c r="H80" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
-      <c r="A80" t="s">
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" t="s">
         <v>60</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C81" t="s">
         <v>94</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D81" t="s">
         <v>562</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E81" t="s">
         <v>563</v>
       </c>
-      <c r="E80" t="s">
+      <c r="F81" t="s">
         <v>564</v>
       </c>
-      <c r="F80" t="s">
+      <c r="G81" t="s">
         <v>565</v>
       </c>
-      <c r="G80" t="s">
+      <c r="H81" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
-      <c r="A81" t="s">
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>91</v>
+      </c>
+      <c r="B82" t="s">
         <v>60</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C82" t="s">
         <v>97</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D82" t="s">
         <v>394</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E82" t="s">
         <v>527</v>
       </c>
-      <c r="E81" t="s">
+      <c r="F82" t="s">
         <v>460</v>
       </c>
-      <c r="F81" t="s">
+      <c r="G82" t="s">
         <v>512</v>
       </c>
-      <c r="G81" t="s">
+      <c r="H82" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
-      <c r="A82" t="s">
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83" t="s">
         <v>60</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C83" t="s">
         <v>98</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D83" t="s">
         <v>152</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E83" t="s">
         <v>153</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F83" t="s">
         <v>461</v>
       </c>
-      <c r="F82" t="s">
+      <c r="G83" t="s">
         <v>513</v>
       </c>
-      <c r="G82" t="s">
+      <c r="H83" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
-      <c r="A83" t="s">
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" t="s">
         <v>60</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C84" t="s">
         <v>92</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D84" t="s">
         <v>150</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E84" t="s">
         <v>151</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F84" t="s">
         <v>462</v>
       </c>
-      <c r="F83" t="s">
+      <c r="G84" t="s">
         <v>514</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H84" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
-      <c r="A84" t="s">
+    <row r="85" spans="1:8">
+      <c r="A85" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" t="s">
         <v>60</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C85" t="s">
         <v>95</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D85" t="s">
         <v>154</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E85" t="s">
         <v>155</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F85" t="s">
         <v>463</v>
       </c>
-      <c r="F84" t="s">
+      <c r="G85" t="s">
         <v>515</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H85" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
-      <c r="A85" t="s">
-        <v>55</v>
-      </c>
-      <c r="B85" t="s">
+    <row r="86" spans="1:8">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" t="s">
         <v>56</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D86" t="s">
         <v>546</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E86" t="s">
         <v>548</v>
       </c>
-      <c r="E85" t="s">
+      <c r="F86" t="s">
         <v>550</v>
       </c>
-      <c r="F85" t="s">
+      <c r="G86" t="s">
         <v>552</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H86" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
-      <c r="A86" t="s">
-        <v>55</v>
-      </c>
-      <c r="B86" t="s">
+    <row r="87" spans="1:8">
+      <c r="A87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" t="s">
         <v>58</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D87" t="s">
         <v>303</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E87" t="s">
         <v>304</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F87" t="s">
         <v>464</v>
       </c>
-      <c r="F86" t="s">
+      <c r="G87" t="s">
         <v>516</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H87" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
-      <c r="A87" t="s">
-        <v>55</v>
-      </c>
-      <c r="B87" t="s">
+    <row r="88" spans="1:8">
+      <c r="A88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" t="s">
         <v>61</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D88" t="s">
         <v>62</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E88" t="s">
         <v>135</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F88" t="s">
         <v>242</v>
       </c>
-      <c r="F87" t="s">
+      <c r="G88" t="s">
         <v>256</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H88" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
-      <c r="A88" t="s">
-        <v>55</v>
-      </c>
-      <c r="B88" t="s">
+    <row r="89" spans="1:8">
+      <c r="A89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C89" t="s">
         <v>57</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D89" t="s">
         <v>59</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E89" t="s">
         <v>161</v>
       </c>
-      <c r="E88" t="s">
+      <c r="F89" t="s">
         <v>243</v>
       </c>
-      <c r="F88" t="s">
+      <c r="G89" t="s">
         <v>257</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H89" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
-      <c r="A89" t="s">
-        <v>55</v>
-      </c>
-      <c r="B89" t="s">
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" t="s">
+        <v>55</v>
+      </c>
+      <c r="C90" t="s">
         <v>259</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D90" t="s">
         <v>261</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E90" t="s">
         <v>261</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F90" t="s">
         <v>261</v>
       </c>
-      <c r="F89" t="s">
+      <c r="G90" t="s">
         <v>261</v>
       </c>
-      <c r="G89" t="s">
+      <c r="H90" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
-      <c r="A90" t="s">
-        <v>55</v>
-      </c>
-      <c r="B90" t="s">
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" t="s">
+        <v>55</v>
+      </c>
+      <c r="C91" t="s">
         <v>260</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D91" t="s">
         <v>398</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E91" t="s">
         <v>398</v>
       </c>
-      <c r="E90" t="s">
+      <c r="F91" t="s">
         <v>398</v>
       </c>
-      <c r="F90" t="s">
+      <c r="G91" t="s">
         <v>398</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H91" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
-      <c r="A91" t="s">
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" t="s">
         <v>60</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C92" t="s">
         <v>56</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D92" t="s">
         <v>545</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E92" t="s">
         <v>547</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F92" t="s">
         <v>549</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G92" t="s">
         <v>551</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H92" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
-      <c r="A92" t="s">
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
         <v>60</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C93" t="s">
         <v>58</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D93" t="s">
         <v>309</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E93" t="s">
         <v>537</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F93" t="s">
         <v>310</v>
       </c>
-      <c r="F92" t="s">
+      <c r="G93" t="s">
         <v>517</v>
       </c>
-      <c r="G92" t="s">
+      <c r="H93" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
-      <c r="A93" t="s">
+    <row r="94" spans="1:8">
+      <c r="A94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" t="s">
         <v>60</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C94" t="s">
         <v>61</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D94" t="s">
         <v>555</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E94" t="s">
         <v>538</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F94" t="s">
         <v>465</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G94" t="s">
         <v>518</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H94" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
-      <c r="A94" t="s">
+    <row r="95" spans="1:8">
+      <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" t="s">
         <v>60</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C95" t="s">
         <v>57</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D95" t="s">
         <v>556</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E95" t="s">
         <v>384</v>
       </c>
-      <c r="E94" t="s">
+      <c r="F95" t="s">
         <v>466</v>
       </c>
-      <c r="F94" t="s">
+      <c r="G95" t="s">
         <v>519</v>
       </c>
-      <c r="G94" t="s">
+      <c r="H95" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
-      <c r="A95" t="s">
+    <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" t="s">
         <v>60</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C96" t="s">
         <v>259</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D96" t="s">
         <v>489</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E96" t="s">
         <v>404</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F96" t="s">
         <v>473</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G96" t="s">
         <v>405</v>
       </c>
-      <c r="G95" t="s">
+      <c r="H96" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
-      <c r="A96" t="s">
+    <row r="97" spans="1:8">
+      <c r="A97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
         <v>60</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C97" t="s">
         <v>260</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D97" t="s">
         <v>397</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E97" t="s">
         <v>397</v>
       </c>
-      <c r="E96" t="s">
+      <c r="F97" t="s">
         <v>467</v>
       </c>
-      <c r="F96" t="s">
+      <c r="G97" t="s">
         <v>520</v>
       </c>
-      <c r="G96" t="s">
+      <c r="H97" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
-      <c r="A97" t="s">
-        <v>55</v>
-      </c>
-      <c r="B97" t="s">
+    <row r="98" spans="1:8">
+      <c r="A98" t="s">
+        <v>110</v>
+      </c>
+      <c r="B98" t="s">
+        <v>55</v>
+      </c>
+      <c r="C98" t="s">
         <v>65</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D98" t="s">
         <v>69</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E98" t="s">
         <v>65</v>
       </c>
-      <c r="E97" t="s">
+      <c r="F98" t="s">
         <v>65</v>
       </c>
-      <c r="F97" t="s">
+      <c r="G98" t="s">
         <v>65</v>
       </c>
-      <c r="G97" t="s">
+      <c r="H98" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
-        <v>55</v>
-      </c>
-      <c r="B98" t="s">
+    <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99" t="s">
+        <v>55</v>
+      </c>
+      <c r="C99" t="s">
         <v>118</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D99" t="s">
         <v>119</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E99" t="s">
         <v>123</v>
       </c>
-      <c r="E98" t="s">
+      <c r="F99" t="s">
         <v>469</v>
       </c>
-      <c r="F98" t="s">
+      <c r="G99" t="s">
         <v>522</v>
       </c>
-      <c r="G98" t="s">
+      <c r="H99" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
-        <v>55</v>
-      </c>
-      <c r="B99" t="s">
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>110</v>
+      </c>
+      <c r="B100" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100" t="s">
         <v>67</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D100" t="s">
         <v>71</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E100" t="s">
         <v>539</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F100" t="s">
         <v>227</v>
       </c>
-      <c r="F99" t="s">
+      <c r="G100" t="s">
         <v>302</v>
       </c>
-      <c r="G99" t="s">
+      <c r="H100" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
-      <c r="A100" t="s">
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>110</v>
+      </c>
+      <c r="B101" t="s">
         <v>60</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C101" t="s">
         <v>116</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D101" t="s">
         <v>395</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E101" t="s">
         <v>406</v>
       </c>
-      <c r="E100" t="s">
+      <c r="F101" t="s">
         <v>470</v>
       </c>
-      <c r="F100" t="s">
+      <c r="G101" t="s">
         <v>521</v>
       </c>
-      <c r="G100" t="s">
+      <c r="H101" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
-      <c r="A101" t="s">
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102" t="s">
         <v>60</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C102" t="s">
         <v>117</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D102" t="s">
         <v>400</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E102" t="s">
         <v>359</v>
       </c>
-      <c r="E101" t="s">
+      <c r="F102" t="s">
         <v>471</v>
       </c>
-      <c r="F101" t="s">
+      <c r="G102" t="s">
         <v>523</v>
       </c>
-      <c r="G101" t="s">
+      <c r="H102" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
-      <c r="A102" t="s">
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>110</v>
+      </c>
+      <c r="B103" t="s">
         <v>60</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C103" t="s">
         <v>118</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D103" t="s">
         <v>401</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E103" t="s">
         <v>360</v>
       </c>
-      <c r="E102" t="s">
+      <c r="F103" t="s">
         <v>472</v>
       </c>
-      <c r="F102" t="s">
+      <c r="G103" t="s">
         <v>524</v>
       </c>
-      <c r="G102" t="s">
+      <c r="H103" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
-      <c r="A103" t="s">
-        <v>55</v>
-      </c>
-      <c r="B103" t="s">
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>63</v>
+      </c>
+      <c r="B104" t="s">
+        <v>55</v>
+      </c>
+      <c r="C104" t="s">
         <v>64</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D104" t="s">
         <v>68</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E104" t="s">
         <v>323</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F104" t="s">
         <v>240</v>
       </c>
-      <c r="F103" t="s">
+      <c r="G104" t="s">
         <v>252</v>
       </c>
-      <c r="G103" t="s">
+      <c r="H104" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
-      <c r="A104" t="s">
-        <v>55</v>
-      </c>
-      <c r="B104" t="s">
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>63</v>
+      </c>
+      <c r="B105" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" t="s">
         <v>65</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D105" t="s">
         <v>69</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E105" t="s">
         <v>65</v>
       </c>
-      <c r="E104" t="s">
+      <c r="F105" t="s">
         <v>65</v>
       </c>
-      <c r="F104" t="s">
+      <c r="G105" t="s">
         <v>65</v>
       </c>
-      <c r="G104" t="s">
+      <c r="H105" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
-      <c r="A105" t="s">
-        <v>55</v>
-      </c>
-      <c r="B105" t="s">
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>63</v>
+      </c>
+      <c r="B106" t="s">
+        <v>55</v>
+      </c>
+      <c r="C106" t="s">
         <v>66</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D106" t="s">
         <v>70</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E106" t="s">
         <v>324</v>
       </c>
-      <c r="E105" t="s">
+      <c r="F106" t="s">
         <v>239</v>
       </c>
-      <c r="F105" t="s">
+      <c r="G106" t="s">
         <v>253</v>
       </c>
-      <c r="G105" t="s">
+      <c r="H106" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
-      <c r="A106" t="s">
-        <v>55</v>
-      </c>
-      <c r="B106" t="s">
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>63</v>
+      </c>
+      <c r="B107" t="s">
+        <v>55</v>
+      </c>
+      <c r="C107" t="s">
         <v>67</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D107" t="s">
         <v>71</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E107" t="s">
         <v>67</v>
       </c>
-      <c r="E106" t="s">
+      <c r="F107" t="s">
         <v>227</v>
       </c>
-      <c r="F106" t="s">
+      <c r="G107" t="s">
         <v>302</v>
       </c>
-      <c r="G106" t="s">
+      <c r="H107" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
-      <c r="A107" t="s">
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>334</v>
+      </c>
+      <c r="B108" t="s">
         <v>335</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C108" t="s">
         <v>270</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D108" t="s">
         <v>528</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E108" t="s">
         <v>528</v>
       </c>
-      <c r="E107" t="s">
+      <c r="F108" t="s">
         <v>528</v>
       </c>
-      <c r="F107" t="s">
+      <c r="G108" t="s">
         <v>528</v>
       </c>
-      <c r="G107" t="s">
+      <c r="H108" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
-      <c r="A108" t="s">
+    <row r="109" spans="1:8">
+      <c r="A109" t="s">
+        <v>264</v>
+      </c>
+      <c r="B109" t="s">
         <v>60</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C109" t="s">
         <v>333</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D109" t="s">
         <v>475</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E109" t="s">
         <v>476</v>
       </c>
-      <c r="E108" t="s">
+      <c r="F109" t="s">
         <v>477</v>
       </c>
-      <c r="F108" t="s">
+      <c r="G109" t="s">
         <v>478</v>
       </c>
-      <c r="G108" t="s">
+      <c r="H109" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
-      <c r="A109" t="s">
+    <row r="110" spans="1:8">
+      <c r="A110" t="s">
+        <v>264</v>
+      </c>
+      <c r="B110" t="s">
         <v>60</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C110" t="s">
         <v>265</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D110" t="s">
         <v>490</v>
       </c>
-      <c r="D109" t="s">
-        <v>540</v>
-      </c>
-      <c r="E109" t="s">
+      <c r="E110" t="s">
+        <v>579</v>
+      </c>
+      <c r="F110" t="s">
         <v>568</v>
       </c>
-      <c r="F109" t="s">
+      <c r="G110" t="s">
         <v>525</v>
       </c>
-      <c r="G109" t="s">
+      <c r="H110" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
-      <c r="A110" t="s">
+    <row r="111" spans="1:8">
+      <c r="A111" t="s">
+        <v>264</v>
+      </c>
+      <c r="B111" t="s">
         <v>60</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C111" t="s">
         <v>270</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D111" t="s">
         <v>572</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E111" t="s">
         <v>573</v>
       </c>
-      <c r="E110" t="s">
+      <c r="F111" t="s">
         <v>574</v>
       </c>
-      <c r="F110" t="s">
+      <c r="G111" t="s">
         <v>575</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H111" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
-      <c r="A111" t="s">
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
+        <v>264</v>
+      </c>
+      <c r="B112" t="s">
         <v>60</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C112" t="s">
         <v>271</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D112" t="s">
         <v>541</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E112" t="s">
         <v>542</v>
       </c>
-      <c r="E111" t="s">
+      <c r="F112" t="s">
         <v>570</v>
       </c>
-      <c r="F111" t="s">
+      <c r="G112" t="s">
         <v>543</v>
       </c>
-      <c r="G111" t="s">
+      <c r="H112" t="s">
         <v>567</v>
       </c>
     </row>

</xml_diff>